<commit_message>
Update binary sheet in repo
</commit_message>
<xml_diff>
--- a/VMW_to_AVGO_ESPP_and_RSU.xlsx
+++ b/VMW_to_AVGO_ESPP_and_RSU.xlsx
@@ -153,6 +153,9 @@
         <t xml:space="preserve">If the fractional share should come out of a specific lot, or set of lots, check those lots here. If multiple are selected the sheet will spread the fraction equally over those lots, accounting for differences in cost-basis.
 For me, eTrade took the entire fraction from a single lot and I expect that's what happened for most people.
 If it came out of an ESPP lot, that's a sale and will incur the ordinary income portion of tax shown in column "Income &amp; short term gain".
+The fractional quantity should be added back into "Share amounts from eTrade" column for the lot that eTrade took it from.
+This is done because we need the cost-basis of the lot calculated _before_ that fraction is removed as it's a serial conversion - convert entire lot, THEN sell factional part.
+It also avoids substantial complexity in formulae.
 </t>
       </text>
     </comment>
@@ -165,7 +168,8 @@
       <text>
         <t xml:space="preserve">The quantities of converted shares from eTrade lots.
 The colour of the cell will alter slightly if the value here does not equal the value calculated via AVGO ratio.
-You can toggle whether to use this manual value or the calculated value in the Tweaks on the first Sheet.</t>
+You can toggle whether to use this manual value or the calculated value in the Tweaks on the first Sheet.
+If this is the lot from which a fraction was taken by etrade then you should add then fractional AVGO quantity back into this value and check the Fraction box. See the note on the fraction column.</t>
       </text>
     </comment>
     <comment authorId="0" ref="O4">
@@ -223,8 +227,12 @@
     <comment authorId="0" ref="J3">
       <text>
         <t xml:space="preserve">If the fractional share should come out of a specific lot, or set of lots, check those lots here. If multiple are selected the sheet will spread the fraction equally over those lots, accounting for differences in cost-basis.
-You REALLY don't want it to come out of an ESPP lot as that's a sale and will incur the ordinary income portion of tax shown in column AB.
-For me, eTrade took the entire fraction from a single lot and I expect that's what happened for most people.</t>
+For me, eTrade took the entire fraction from a single lot and I expect that's what happened for most people.
+If it came out of an ESPP lot, that's a sale and will incur the ordinary income portion of tax shown in column "Income &amp; short term gain".
+The fractional quantity should be added back into "Share amounts from eTrade" column for the lot that eTrade took it from.
+This is done because we need the cost-basis of the lot calculated _before_ that fraction is removed as it's a serial conversion - convert entire lot, THEN sell factional part.
+It also avoids substantial complexity in formulae.
+</t>
       </text>
     </comment>
     <comment authorId="0" ref="D4">
@@ -240,7 +248,8 @@
       <text>
         <t xml:space="preserve">The quantities of converted shares from eTrade lots.
 The colour of the cell will alter slightly if the value here does not equal the value calculated via AVGO ratio.
-You can toggle whether to use this manual value or the calculated value in the Tweaks on the first Sheet.</t>
+You can toggle whether to use this manual value or the calculated value in the Tweaks on the first Sheet.
+If this is the lot from which a fraction was taken by etrade then you should add then fractional AVGO quantity back into this value and check the Fraction box. See the note on the fraction column.</t>
       </text>
     </comment>
     <comment authorId="0" ref="K4">
@@ -406,7 +415,7 @@
         <color rgb="FF1155CC"/>
         <u/>
       </rPr>
-      <t>v0.1.2</t>
+      <t>v0.1.3</t>
     </r>
   </si>
   <si>
@@ -425,7 +434,7 @@
     <t>c. It's expected you'll need to add rows for RSU grants where you had more than one vest on a given date - in that case it's easiest to insert a row below the entry for the corresponding date, copy the entire populated row down to get the release date and market value, then fill in the specific share quantity for the lot.</t>
   </si>
   <si>
-    <t>8. For the fractional share - if you're providing the manual values for number of shares, add the fractional amount back into any lot it came from if deducted. This avoids needing a single row with different handling based on whether the manual value has a fraction removed or not.</t>
+    <t>8. For the fractional share - if you're providing the manual values for number of shares, add the fractional amount back into any lot it came from if deducted in "Share amounts from eTrade". This avoids needing a single row with different handling based on whether the manual value has a fraction removed or not.</t>
   </si>
   <si>
     <t>a. Check the Fraction box for any lot you want to the fraction to be attributed to. The fraction is evenly spread across the selected lots.</t>
@@ -3261,8 +3270,8 @@
         <v>59</v>
       </c>
       <c r="M28" s="58">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),1227.45)</f>
-        <v>1227.45</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),1296.23)</f>
+        <v>1296.23</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -4563,7 +4572,7 @@
       <c r="L5" s="80"/>
       <c r="M5" s="178">
         <f>SUM(M7:M26)</f>
-        <v>218.034</v>
+        <v>0</v>
       </c>
       <c r="N5" s="82">
         <f>COUNTIF(N7:N26, TRUE)</f>
@@ -4730,9 +4739,7 @@
         <f t="shared" ref="L7:L13" si="8">0.85*MIN(E7,F7)</f>
         <v>65.008</v>
       </c>
-      <c r="M7" s="201">
-        <v>0.0</v>
-      </c>
+      <c r="M7" s="201"/>
       <c r="N7" s="202" t="b">
         <v>0</v>
       </c>
@@ -4880,9 +4887,7 @@
         <f t="shared" si="8"/>
         <v>66.9715</v>
       </c>
-      <c r="M8" s="201">
-        <v>0.0</v>
-      </c>
+      <c r="M8" s="201"/>
       <c r="N8" s="202" t="b">
         <v>0</v>
       </c>
@@ -5030,9 +5035,7 @@
         <f t="shared" si="8"/>
         <v>69.785</v>
       </c>
-      <c r="M9" s="201">
-        <v>0.0</v>
-      </c>
+      <c r="M9" s="201"/>
       <c r="N9" s="218" t="b">
         <v>0</v>
       </c>
@@ -5180,9 +5183,7 @@
         <f t="shared" si="8"/>
         <v>76.619</v>
       </c>
-      <c r="M10" s="201">
-        <v>0.0</v>
-      </c>
+      <c r="M10" s="201"/>
       <c r="N10" s="202" t="b">
         <v>0</v>
       </c>
@@ -5329,9 +5330,7 @@
         <f t="shared" si="8"/>
         <v>65.535</v>
       </c>
-      <c r="M11" s="219">
-        <v>14.965</v>
-      </c>
+      <c r="M11" s="219"/>
       <c r="N11" s="218" t="b">
         <v>0</v>
       </c>
@@ -5479,9 +5478,7 @@
         <f t="shared" si="8"/>
         <v>65.535</v>
       </c>
-      <c r="M12" s="201">
-        <v>14.964</v>
-      </c>
+      <c r="M12" s="201"/>
       <c r="N12" s="218" t="b">
         <v>0</v>
       </c>
@@ -5629,9 +5626,7 @@
         <f t="shared" si="8"/>
         <v>38.8875</v>
       </c>
-      <c r="M13" s="201">
-        <v>25.203</v>
-      </c>
+      <c r="M13" s="201"/>
       <c r="N13" s="220" t="b">
         <v>0</v>
       </c>
@@ -5779,9 +5774,7 @@
         <f t="shared" ref="L14:L26" si="18">ROUND(0.85*MIN(E14,F14),2)</f>
         <v>38.67</v>
       </c>
-      <c r="M14" s="219">
-        <v>25.334</v>
-      </c>
+      <c r="M14" s="219"/>
       <c r="N14" s="220" t="b">
         <v>0</v>
       </c>
@@ -5928,9 +5921,7 @@
         <f t="shared" si="18"/>
         <v>38.67</v>
       </c>
-      <c r="M15" s="219">
-        <v>25.334</v>
-      </c>
+      <c r="M15" s="219"/>
       <c r="N15" s="220" t="b">
         <v>0</v>
       </c>
@@ -6077,9 +6068,7 @@
         <f t="shared" si="18"/>
         <v>74.11</v>
       </c>
-      <c r="M16" s="201">
-        <v>13.258</v>
-      </c>
+      <c r="M16" s="201"/>
       <c r="N16" s="220" t="b">
         <v>0</v>
       </c>
@@ -6226,9 +6215,7 @@
         <f t="shared" si="18"/>
         <v>74.11</v>
       </c>
-      <c r="M17" s="201">
-        <v>15.49</v>
-      </c>
+      <c r="M17" s="201"/>
       <c r="N17" s="220" t="b">
         <v>0</v>
       </c>
@@ -6375,9 +6362,7 @@
         <f t="shared" si="18"/>
         <v>105.11</v>
       </c>
-      <c r="M18" s="201">
-        <v>9.32</v>
-      </c>
+      <c r="M18" s="201"/>
       <c r="N18" s="220" t="b">
         <v>0</v>
       </c>
@@ -6524,9 +6509,7 @@
         <f t="shared" si="18"/>
         <v>105.11</v>
       </c>
-      <c r="M19" s="201">
-        <v>9.32</v>
-      </c>
+      <c r="M19" s="201"/>
       <c r="N19" s="220" t="b">
         <v>0</v>
       </c>
@@ -6673,9 +6656,7 @@
         <f t="shared" si="18"/>
         <v>120.22</v>
       </c>
-      <c r="M20" s="219">
-        <v>8.138</v>
-      </c>
+      <c r="M20" s="219"/>
       <c r="N20" s="220" t="b">
         <v>0</v>
       </c>
@@ -6822,9 +6803,7 @@
         <f t="shared" si="18"/>
         <v>102.44</v>
       </c>
-      <c r="M21" s="219">
-        <v>9.583</v>
-      </c>
+      <c r="M21" s="219"/>
       <c r="N21" s="220" t="b">
         <v>0</v>
       </c>
@@ -6971,9 +6950,7 @@
         <f t="shared" si="18"/>
         <v>102.44</v>
       </c>
-      <c r="M22" s="201">
-        <v>9.582</v>
-      </c>
+      <c r="M22" s="201"/>
       <c r="N22" s="220" t="b">
         <v>0</v>
       </c>
@@ -7120,9 +7097,7 @@
         <f t="shared" si="18"/>
         <v>102.44</v>
       </c>
-      <c r="M23" s="219">
-        <v>9.583</v>
-      </c>
+      <c r="M23" s="219"/>
       <c r="N23" s="220" t="b">
         <v>0</v>
       </c>
@@ -7269,9 +7244,7 @@
         <f t="shared" si="18"/>
         <v>119.35</v>
       </c>
-      <c r="M24" s="201">
-        <v>8.139</v>
-      </c>
+      <c r="M24" s="201"/>
       <c r="N24" s="220" t="b">
         <v>0</v>
       </c>
@@ -7418,9 +7391,7 @@
         <f t="shared" si="18"/>
         <v>99.72</v>
       </c>
-      <c r="M25" s="201">
-        <v>9.845</v>
-      </c>
+      <c r="M25" s="201"/>
       <c r="N25" s="220" t="b">
         <v>0</v>
       </c>
@@ -7567,9 +7538,7 @@
         <f t="shared" si="18"/>
         <v>98.52</v>
       </c>
-      <c r="M26" s="230">
-        <v>9.976</v>
-      </c>
+      <c r="M26" s="230"/>
       <c r="N26" s="231" t="b">
         <v>0</v>
       </c>
@@ -7742,7 +7711,7 @@
       <c r="L28" s="97"/>
       <c r="M28" s="252">
         <f>SUM(M7:M26)</f>
-        <v>218.034</v>
+        <v>0</v>
       </c>
       <c r="N28" s="250">
         <f>COUNTIF(N7:N26, TRUE)</f>
@@ -18507,7 +18476,7 @@
       </c>
       <c r="B10" s="330">
         <f>Summary!M28</f>
-        <v>1227.45</v>
+        <v>1296.23</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -18817,7 +18786,7 @@
       </c>
       <c r="B29" s="338">
         <f>SWITCH(Summary!$K$28,"today",TODAY(),"last year","2023-12-31",Summary!$K$28)</f>
-        <v>45343</v>
+        <v>45350</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>

</xml_diff>

<commit_message>
Optimizer uses values from Summary for number of shares to assign to cash/stock (#65)
The optimizer was using hardcoded values for target shares for assignment.
This would have rendered it useless for anyone. This changes pulls those values
from the Necessary Inputs cells.

Expands on notes to add the fractional share back into the lot.
</commit_message>
<xml_diff>
--- a/VMW_to_AVGO_ESPP_and_RSU.xlsx
+++ b/VMW_to_AVGO_ESPP_and_RSU.xlsx
@@ -153,6 +153,9 @@
         <t xml:space="preserve">If the fractional share should come out of a specific lot, or set of lots, check those lots here. If multiple are selected the sheet will spread the fraction equally over those lots, accounting for differences in cost-basis.
 For me, eTrade took the entire fraction from a single lot and I expect that's what happened for most people.
 If it came out of an ESPP lot, that's a sale and will incur the ordinary income portion of tax shown in column "Income &amp; short term gain".
+The fractional quantity should be added back into "Share amounts from eTrade" column for the lot that eTrade took it from.
+This is done because we need the cost-basis of the lot calculated _before_ that fraction is removed as it's a serial conversion - convert entire lot, THEN sell factional part.
+It also avoids substantial complexity in formulae.
 </t>
       </text>
     </comment>
@@ -165,7 +168,8 @@
       <text>
         <t xml:space="preserve">The quantities of converted shares from eTrade lots.
 The colour of the cell will alter slightly if the value here does not equal the value calculated via AVGO ratio.
-You can toggle whether to use this manual value or the calculated value in the Tweaks on the first Sheet.</t>
+You can toggle whether to use this manual value or the calculated value in the Tweaks on the first Sheet.
+If this is the lot from which a fraction was taken by etrade then you should add then fractional AVGO quantity back into this value and check the Fraction box. See the note on the fraction column.</t>
       </text>
     </comment>
     <comment authorId="0" ref="O4">
@@ -223,8 +227,12 @@
     <comment authorId="0" ref="J3">
       <text>
         <t xml:space="preserve">If the fractional share should come out of a specific lot, or set of lots, check those lots here. If multiple are selected the sheet will spread the fraction equally over those lots, accounting for differences in cost-basis.
-You REALLY don't want it to come out of an ESPP lot as that's a sale and will incur the ordinary income portion of tax shown in column AB.
-For me, eTrade took the entire fraction from a single lot and I expect that's what happened for most people.</t>
+For me, eTrade took the entire fraction from a single lot and I expect that's what happened for most people.
+If it came out of an ESPP lot, that's a sale and will incur the ordinary income portion of tax shown in column "Income &amp; short term gain".
+The fractional quantity should be added back into "Share amounts from eTrade" column for the lot that eTrade took it from.
+This is done because we need the cost-basis of the lot calculated _before_ that fraction is removed as it's a serial conversion - convert entire lot, THEN sell factional part.
+It also avoids substantial complexity in formulae.
+</t>
       </text>
     </comment>
     <comment authorId="0" ref="D4">
@@ -240,7 +248,8 @@
       <text>
         <t xml:space="preserve">The quantities of converted shares from eTrade lots.
 The colour of the cell will alter slightly if the value here does not equal the value calculated via AVGO ratio.
-You can toggle whether to use this manual value or the calculated value in the Tweaks on the first Sheet.</t>
+You can toggle whether to use this manual value or the calculated value in the Tweaks on the first Sheet.
+If this is the lot from which a fraction was taken by etrade then you should add then fractional AVGO quantity back into this value and check the Fraction box. See the note on the fraction column.</t>
       </text>
     </comment>
     <comment authorId="0" ref="K4">
@@ -406,7 +415,7 @@
         <color rgb="FF1155CC"/>
         <u/>
       </rPr>
-      <t>v0.1.2</t>
+      <t>v0.1.3</t>
     </r>
   </si>
   <si>
@@ -425,7 +434,7 @@
     <t>c. It's expected you'll need to add rows for RSU grants where you had more than one vest on a given date - in that case it's easiest to insert a row below the entry for the corresponding date, copy the entire populated row down to get the release date and market value, then fill in the specific share quantity for the lot.</t>
   </si>
   <si>
-    <t>8. For the fractional share - if you're providing the manual values for number of shares, add the fractional amount back into any lot it came from if deducted. This avoids needing a single row with different handling based on whether the manual value has a fraction removed or not.</t>
+    <t>8. For the fractional share - if you're providing the manual values for number of shares, add the fractional amount back into any lot it came from if deducted in "Share amounts from eTrade". This avoids needing a single row with different handling based on whether the manual value has a fraction removed or not.</t>
   </si>
   <si>
     <t>a. Check the Fraction box for any lot you want to the fraction to be attributed to. The fraction is evenly spread across the selected lots.</t>
@@ -3261,8 +3270,8 @@
         <v>59</v>
       </c>
       <c r="M28" s="58">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),1227.45)</f>
-        <v>1227.45</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),1296.23)</f>
+        <v>1296.23</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -4563,7 +4572,7 @@
       <c r="L5" s="80"/>
       <c r="M5" s="178">
         <f>SUM(M7:M26)</f>
-        <v>218.034</v>
+        <v>0</v>
       </c>
       <c r="N5" s="82">
         <f>COUNTIF(N7:N26, TRUE)</f>
@@ -4730,9 +4739,7 @@
         <f t="shared" ref="L7:L13" si="8">0.85*MIN(E7,F7)</f>
         <v>65.008</v>
       </c>
-      <c r="M7" s="201">
-        <v>0.0</v>
-      </c>
+      <c r="M7" s="201"/>
       <c r="N7" s="202" t="b">
         <v>0</v>
       </c>
@@ -4880,9 +4887,7 @@
         <f t="shared" si="8"/>
         <v>66.9715</v>
       </c>
-      <c r="M8" s="201">
-        <v>0.0</v>
-      </c>
+      <c r="M8" s="201"/>
       <c r="N8" s="202" t="b">
         <v>0</v>
       </c>
@@ -5030,9 +5035,7 @@
         <f t="shared" si="8"/>
         <v>69.785</v>
       </c>
-      <c r="M9" s="201">
-        <v>0.0</v>
-      </c>
+      <c r="M9" s="201"/>
       <c r="N9" s="218" t="b">
         <v>0</v>
       </c>
@@ -5180,9 +5183,7 @@
         <f t="shared" si="8"/>
         <v>76.619</v>
       </c>
-      <c r="M10" s="201">
-        <v>0.0</v>
-      </c>
+      <c r="M10" s="201"/>
       <c r="N10" s="202" t="b">
         <v>0</v>
       </c>
@@ -5329,9 +5330,7 @@
         <f t="shared" si="8"/>
         <v>65.535</v>
       </c>
-      <c r="M11" s="219">
-        <v>14.965</v>
-      </c>
+      <c r="M11" s="219"/>
       <c r="N11" s="218" t="b">
         <v>0</v>
       </c>
@@ -5479,9 +5478,7 @@
         <f t="shared" si="8"/>
         <v>65.535</v>
       </c>
-      <c r="M12" s="201">
-        <v>14.964</v>
-      </c>
+      <c r="M12" s="201"/>
       <c r="N12" s="218" t="b">
         <v>0</v>
       </c>
@@ -5629,9 +5626,7 @@
         <f t="shared" si="8"/>
         <v>38.8875</v>
       </c>
-      <c r="M13" s="201">
-        <v>25.203</v>
-      </c>
+      <c r="M13" s="201"/>
       <c r="N13" s="220" t="b">
         <v>0</v>
       </c>
@@ -5779,9 +5774,7 @@
         <f t="shared" ref="L14:L26" si="18">ROUND(0.85*MIN(E14,F14),2)</f>
         <v>38.67</v>
       </c>
-      <c r="M14" s="219">
-        <v>25.334</v>
-      </c>
+      <c r="M14" s="219"/>
       <c r="N14" s="220" t="b">
         <v>0</v>
       </c>
@@ -5928,9 +5921,7 @@
         <f t="shared" si="18"/>
         <v>38.67</v>
       </c>
-      <c r="M15" s="219">
-        <v>25.334</v>
-      </c>
+      <c r="M15" s="219"/>
       <c r="N15" s="220" t="b">
         <v>0</v>
       </c>
@@ -6077,9 +6068,7 @@
         <f t="shared" si="18"/>
         <v>74.11</v>
       </c>
-      <c r="M16" s="201">
-        <v>13.258</v>
-      </c>
+      <c r="M16" s="201"/>
       <c r="N16" s="220" t="b">
         <v>0</v>
       </c>
@@ -6226,9 +6215,7 @@
         <f t="shared" si="18"/>
         <v>74.11</v>
       </c>
-      <c r="M17" s="201">
-        <v>15.49</v>
-      </c>
+      <c r="M17" s="201"/>
       <c r="N17" s="220" t="b">
         <v>0</v>
       </c>
@@ -6375,9 +6362,7 @@
         <f t="shared" si="18"/>
         <v>105.11</v>
       </c>
-      <c r="M18" s="201">
-        <v>9.32</v>
-      </c>
+      <c r="M18" s="201"/>
       <c r="N18" s="220" t="b">
         <v>0</v>
       </c>
@@ -6524,9 +6509,7 @@
         <f t="shared" si="18"/>
         <v>105.11</v>
       </c>
-      <c r="M19" s="201">
-        <v>9.32</v>
-      </c>
+      <c r="M19" s="201"/>
       <c r="N19" s="220" t="b">
         <v>0</v>
       </c>
@@ -6673,9 +6656,7 @@
         <f t="shared" si="18"/>
         <v>120.22</v>
       </c>
-      <c r="M20" s="219">
-        <v>8.138</v>
-      </c>
+      <c r="M20" s="219"/>
       <c r="N20" s="220" t="b">
         <v>0</v>
       </c>
@@ -6822,9 +6803,7 @@
         <f t="shared" si="18"/>
         <v>102.44</v>
       </c>
-      <c r="M21" s="219">
-        <v>9.583</v>
-      </c>
+      <c r="M21" s="219"/>
       <c r="N21" s="220" t="b">
         <v>0</v>
       </c>
@@ -6971,9 +6950,7 @@
         <f t="shared" si="18"/>
         <v>102.44</v>
       </c>
-      <c r="M22" s="201">
-        <v>9.582</v>
-      </c>
+      <c r="M22" s="201"/>
       <c r="N22" s="220" t="b">
         <v>0</v>
       </c>
@@ -7120,9 +7097,7 @@
         <f t="shared" si="18"/>
         <v>102.44</v>
       </c>
-      <c r="M23" s="219">
-        <v>9.583</v>
-      </c>
+      <c r="M23" s="219"/>
       <c r="N23" s="220" t="b">
         <v>0</v>
       </c>
@@ -7269,9 +7244,7 @@
         <f t="shared" si="18"/>
         <v>119.35</v>
       </c>
-      <c r="M24" s="201">
-        <v>8.139</v>
-      </c>
+      <c r="M24" s="201"/>
       <c r="N24" s="220" t="b">
         <v>0</v>
       </c>
@@ -7418,9 +7391,7 @@
         <f t="shared" si="18"/>
         <v>99.72</v>
       </c>
-      <c r="M25" s="201">
-        <v>9.845</v>
-      </c>
+      <c r="M25" s="201"/>
       <c r="N25" s="220" t="b">
         <v>0</v>
       </c>
@@ -7567,9 +7538,7 @@
         <f t="shared" si="18"/>
         <v>98.52</v>
       </c>
-      <c r="M26" s="230">
-        <v>9.976</v>
-      </c>
+      <c r="M26" s="230"/>
       <c r="N26" s="231" t="b">
         <v>0</v>
       </c>
@@ -7742,7 +7711,7 @@
       <c r="L28" s="97"/>
       <c r="M28" s="252">
         <f>SUM(M7:M26)</f>
-        <v>218.034</v>
+        <v>0</v>
       </c>
       <c r="N28" s="250">
         <f>COUNTIF(N7:N26, TRUE)</f>
@@ -18507,7 +18476,7 @@
       </c>
       <c r="B10" s="330">
         <f>Summary!M28</f>
-        <v>1227.45</v>
+        <v>1296.23</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -18817,7 +18786,7 @@
       </c>
       <c r="B29" s="338">
         <f>SWITCH(Summary!$K$28,"today",TODAY(),"last year","2023-12-31",Summary!$K$28)</f>
-        <v>45343</v>
+        <v>45350</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>

</xml_diff>

<commit_message>
Fix potential capital gain calculation for fractional share lot
Should have been subtracting the fraction before calculating the gain, but was instead subtracting the fractional share, eg. 0.123, from the dollar value of shares.
</commit_message>
<xml_diff>
--- a/VMW_to_AVGO_ESPP_and_RSU.xlsx
+++ b/VMW_to_AVGO_ESPP_and_RSU.xlsx
@@ -622,7 +622,7 @@
     <t>Post merger sale of AVGO</t>
   </si>
   <si>
-    <t>today</t>
+    <t>last year</t>
   </si>
   <si>
     <t xml:space="preserve">  @ </t>
@@ -3862,9 +3862,9 @@
       <c r="L28" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="M28" s="58" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),"Loading...")</f>
-        <v>Loading...</v>
+      <c r="M28" s="58">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),1361.34)</f>
+        <v>1361.34</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -4804,11 +4804,11 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="K42:O42"/>
     <mergeCell ref="C48:H48"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="F51:G51"/>
-    <mergeCell ref="K42:O42"/>
   </mergeCells>
   <conditionalFormatting sqref="B29">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
@@ -5610,7 +5610,7 @@
         <v>n/a</v>
       </c>
       <c r="AX7" s="247">
-        <f>iferror((Reference!$B$10-AW7)*(AH7) - AJ7, 0)</f>
+        <f>iferror((Reference!$B$10-AW7)*(AH7 - AJ7), 0)</f>
         <v>0</v>
       </c>
       <c r="AY7" s="248" t="b">
@@ -5806,7 +5806,7 @@
         <v>n/a</v>
       </c>
       <c r="AX8" s="247">
-        <f>iferror((Reference!$B$10-AW8)*(AH8) - AJ8, 0)</f>
+        <f>iferror((Reference!$B$10-AW8)*(AH8 - AJ8), 0)</f>
         <v>0</v>
       </c>
       <c r="AY8" s="248" t="b">
@@ -6002,7 +6002,7 @@
         <v>n/a</v>
       </c>
       <c r="AX9" s="247">
-        <f>iferror((Reference!$B$10-AW9)*(AH9) - AJ9, 0)</f>
+        <f>iferror((Reference!$B$10-AW9)*(AH9 - AJ9), 0)</f>
         <v>0</v>
       </c>
       <c r="AY9" s="248" t="b">
@@ -6198,7 +6198,7 @@
         <v>n/a</v>
       </c>
       <c r="AX10" s="247">
-        <f>iferror((Reference!$B$10-AW10)*(AH10) - AJ10, 0)</f>
+        <f>iferror((Reference!$B$10-AW10)*(AH10 - AJ10), 0)</f>
         <v>0</v>
       </c>
       <c r="AY10" s="248" t="b">
@@ -6393,7 +6393,7 @@
         <v>n/a</v>
       </c>
       <c r="AX11" s="247">
-        <f>iferror((Reference!$B$10-AW11)*(AH11) - AJ11, 0)</f>
+        <f>iferror((Reference!$B$10-AW11)*(AH11 - AJ11), 0)</f>
         <v>0</v>
       </c>
       <c r="AY11" s="248" t="b">
@@ -6589,7 +6589,7 @@
         <v>n/a</v>
       </c>
       <c r="AX12" s="247">
-        <f>iferror((Reference!$B$10-AW12)*(AH12) - AJ12, 0)</f>
+        <f>iferror((Reference!$B$10-AW12)*(AH12 - AJ12), 0)</f>
         <v>0</v>
       </c>
       <c r="AY12" s="248" t="b">
@@ -6785,7 +6785,7 @@
         <v>n/a</v>
       </c>
       <c r="AX13" s="247">
-        <f>iferror((Reference!$B$10-AW13)*(AH13) - AJ13, 0)</f>
+        <f>iferror((Reference!$B$10-AW13)*(AH13 - AJ13), 0)</f>
         <v>0</v>
       </c>
       <c r="AY13" s="248" t="b">
@@ -6981,7 +6981,7 @@
         <v>n/a</v>
       </c>
       <c r="AX14" s="247">
-        <f>iferror((Reference!$B$10-AW14)*(AH14) - AJ14, 0)</f>
+        <f>iferror((Reference!$B$10-AW14)*(AH14 - AJ14), 0)</f>
         <v>0</v>
       </c>
       <c r="AY14" s="248" t="b">
@@ -7176,7 +7176,7 @@
         <v>n/a</v>
       </c>
       <c r="AX15" s="247">
-        <f>iferror((Reference!$B$10-AW15)*(AH15) - AJ15, 0)</f>
+        <f>iferror((Reference!$B$10-AW15)*(AH15 - AJ15), 0)</f>
         <v>0</v>
       </c>
       <c r="AY15" s="248" t="b">
@@ -7371,7 +7371,7 @@
         <v>n/a</v>
       </c>
       <c r="AX16" s="247">
-        <f>iferror((Reference!$B$10-AW16)*(AH16) - AJ16, 0)</f>
+        <f>iferror((Reference!$B$10-AW16)*(AH16 - AJ16), 0)</f>
         <v>0</v>
       </c>
       <c r="AY16" s="248" t="b">
@@ -7566,7 +7566,7 @@
         <v>n/a</v>
       </c>
       <c r="AX17" s="247">
-        <f>iferror((Reference!$B$10-AW17)*(AH17) - AJ17, 0)</f>
+        <f>iferror((Reference!$B$10-AW17)*(AH17 - AJ17), 0)</f>
         <v>0</v>
       </c>
       <c r="AY17" s="248" t="b">
@@ -7761,7 +7761,7 @@
         <v>n/a</v>
       </c>
       <c r="AX18" s="247">
-        <f>iferror((Reference!$B$10-AW18)*(AH18) - AJ18, 0)</f>
+        <f>iferror((Reference!$B$10-AW18)*(AH18 - AJ18), 0)</f>
         <v>0</v>
       </c>
       <c r="AY18" s="248" t="b">
@@ -7956,7 +7956,7 @@
         <v>n/a</v>
       </c>
       <c r="AX19" s="247">
-        <f>iferror((Reference!$B$10-AW19)*(AH19) - AJ19, 0)</f>
+        <f>iferror((Reference!$B$10-AW19)*(AH19 - AJ19), 0)</f>
         <v>0</v>
       </c>
       <c r="AY19" s="248" t="b">
@@ -8151,7 +8151,7 @@
         <v>n/a</v>
       </c>
       <c r="AX20" s="247">
-        <f>iferror((Reference!$B$10-AW20)*(AH20) - AJ20, 0)</f>
+        <f>iferror((Reference!$B$10-AW20)*(AH20 - AJ20), 0)</f>
         <v>0</v>
       </c>
       <c r="AY20" s="248" t="b">
@@ -8346,7 +8346,7 @@
         <v>n/a</v>
       </c>
       <c r="AX21" s="247">
-        <f>iferror((Reference!$B$10-AW21)*(AH21) - AJ21, 0)</f>
+        <f>iferror((Reference!$B$10-AW21)*(AH21 - AJ21), 0)</f>
         <v>0</v>
       </c>
       <c r="AY21" s="248" t="b">
@@ -8541,7 +8541,7 @@
         <v>n/a</v>
       </c>
       <c r="AX22" s="247">
-        <f>iferror((Reference!$B$10-AW22)*(AH22) - AJ22, 0)</f>
+        <f>iferror((Reference!$B$10-AW22)*(AH22 - AJ22), 0)</f>
         <v>0</v>
       </c>
       <c r="AY22" s="248" t="b">
@@ -8736,7 +8736,7 @@
         <v>n/a</v>
       </c>
       <c r="AX23" s="247">
-        <f>iferror((Reference!$B$10-AW23)*(AH23) - AJ23, 0)</f>
+        <f>iferror((Reference!$B$10-AW23)*(AH23 - AJ23), 0)</f>
         <v>0</v>
       </c>
       <c r="AY23" s="248" t="b">
@@ -8931,7 +8931,7 @@
         <v>n/a</v>
       </c>
       <c r="AX24" s="247">
-        <f>iferror((Reference!$B$10-AW24)*(AH24) - AJ24, 0)</f>
+        <f>iferror((Reference!$B$10-AW24)*(AH24 - AJ24), 0)</f>
         <v>0</v>
       </c>
       <c r="AY24" s="248" t="b">
@@ -9126,7 +9126,7 @@
         <v>n/a</v>
       </c>
       <c r="AX25" s="247">
-        <f>iferror((Reference!$B$10-AW25)*(AH25) - AJ25, 0)</f>
+        <f>iferror((Reference!$B$10-AW25)*(AH25 - AJ25), 0)</f>
         <v>0</v>
       </c>
       <c r="AY25" s="248" t="b">
@@ -9321,12 +9321,12 @@
         <v>n/a</v>
       </c>
       <c r="AX26" s="290">
-        <f>iferror((Reference!$B$10-AW26)*(AH26) - AJ26, 0)</f>
+        <f>iferror((Reference!$B$10-AW26)*(AH26 - AJ26), 0)</f>
         <v>0</v>
       </c>
       <c r="AY26" s="291" t="b">
         <f>AND(DATEDIF(B26,Reference!$B$29,"Y")&gt;=1, DATEDIF(A26, Reference!$B$29, "Y")&gt;=2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ26" s="290">
         <f t="shared" si="20"/>
@@ -9546,18 +9546,18 @@
     <mergeCell ref="X2:AI2"/>
     <mergeCell ref="AK2:AV2"/>
     <mergeCell ref="AW2:BB2"/>
+    <mergeCell ref="AE3:AH3"/>
     <mergeCell ref="AK3:AL3"/>
     <mergeCell ref="AM3:AN3"/>
     <mergeCell ref="AO3:AV3"/>
     <mergeCell ref="AW3:BB3"/>
-    <mergeCell ref="AE3:AH3"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="O3:T3"/>
     <mergeCell ref="U3:W3"/>
+    <mergeCell ref="X3:AA3"/>
     <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="X3:AA3"/>
   </mergeCells>
   <conditionalFormatting sqref="M7:M26">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="notEqual">
@@ -9962,7 +9962,7 @@
       </c>
       <c r="H5" s="299">
         <f t="shared" si="1"/>
-        <v>571638.27</v>
+        <v>0</v>
       </c>
       <c r="I5" s="340">
         <f t="shared" si="1"/>
@@ -10141,9 +10141,7 @@
       <c r="E7" s="353">
         <v>82.1</v>
       </c>
-      <c r="F7" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F7" s="354"/>
       <c r="G7" s="225">
         <f t="shared" ref="G7:G84" si="7">D7*E7</f>
         <v>0</v>
@@ -10292,7 +10290,7 @@
         <v>n/a</v>
       </c>
       <c r="AU7" s="247">
-        <f>iferror((Reference!$B$10-AT7)*AE7 - AG7, 0)</f>
+        <f>iferror((Reference!$B$10-AT7)*(AE7 - AG7), 0)</f>
         <v>0</v>
       </c>
       <c r="AV7" s="247">
@@ -10316,9 +10314,7 @@
       <c r="E8" s="353">
         <v>90.14</v>
       </c>
-      <c r="F8" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F8" s="354"/>
       <c r="G8" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -10467,7 +10463,7 @@
         <v>n/a</v>
       </c>
       <c r="AU8" s="247">
-        <f>iferror((Reference!$B$10-AT8)*AE8 - AG8, 0)</f>
+        <f>iferror((Reference!$B$10-AT8)*(AE8 - AG8), 0)</f>
         <v>0</v>
       </c>
       <c r="AV8" s="247">
@@ -10493,16 +10489,14 @@
       <c r="E9" s="353">
         <v>98.33</v>
       </c>
-      <c r="F9" s="354">
-        <v>25.0</v>
-      </c>
+      <c r="F9" s="354"/>
       <c r="G9" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H9" s="236">
         <f t="shared" si="8"/>
-        <v>2458.25</v>
+        <v>0</v>
       </c>
       <c r="I9" s="355"/>
       <c r="J9" s="366" t="b">
@@ -10644,7 +10638,7 @@
         <v>n/a</v>
       </c>
       <c r="AU9" s="247">
-        <f>iferror((Reference!$B$10-AT9)*AE9 - AG9, 0)</f>
+        <f>iferror((Reference!$B$10-AT9)*(AE9 - AG9), 0)</f>
         <v>0</v>
       </c>
       <c r="AV9" s="247">
@@ -10670,16 +10664,14 @@
       <c r="E10" s="353">
         <v>77.1</v>
       </c>
-      <c r="F10" s="354">
-        <v>25.0</v>
-      </c>
+      <c r="F10" s="354"/>
       <c r="G10" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H10" s="236">
         <f t="shared" si="8"/>
-        <v>1927.5</v>
+        <v>0</v>
       </c>
       <c r="I10" s="367"/>
       <c r="J10" s="259" t="b">
@@ -10821,7 +10813,7 @@
         <v>n/a</v>
       </c>
       <c r="AU10" s="247">
-        <f>iferror((Reference!$B$10-AT10)*AE10 - AG10, 0)</f>
+        <f>iferror((Reference!$B$10-AT10)*(AE10 - AG10), 0)</f>
         <v>0</v>
       </c>
       <c r="AV10" s="247">
@@ -10847,16 +10839,14 @@
       <c r="E11" s="353">
         <v>87.47</v>
       </c>
-      <c r="F11" s="354">
-        <v>47.0</v>
-      </c>
+      <c r="F11" s="354"/>
       <c r="G11" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H11" s="236">
         <f t="shared" si="8"/>
-        <v>4111.09</v>
+        <v>0</v>
       </c>
       <c r="I11" s="355"/>
       <c r="J11" s="259" t="b">
@@ -10998,7 +10988,7 @@
         <v>n/a</v>
       </c>
       <c r="AU11" s="247">
-        <f>iferror((Reference!$B$10-AT11)*AE11 - AG11, 0)</f>
+        <f>iferror((Reference!$B$10-AT11)*(AE11 - AG11), 0)</f>
         <v>0</v>
       </c>
       <c r="AV11" s="247">
@@ -11024,16 +11014,14 @@
       <c r="E12" s="353">
         <v>89.13</v>
       </c>
-      <c r="F12" s="354">
-        <v>25.0</v>
-      </c>
+      <c r="F12" s="354"/>
       <c r="G12" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H12" s="236">
         <f t="shared" si="8"/>
-        <v>2228.25</v>
+        <v>0</v>
       </c>
       <c r="I12" s="355"/>
       <c r="J12" s="259" t="b">
@@ -11175,7 +11163,7 @@
         <v>n/a</v>
       </c>
       <c r="AU12" s="247">
-        <f>iferror((Reference!$B$10-AT12)*AE12 - AG12, 0)</f>
+        <f>iferror((Reference!$B$10-AT12)*(AE12 - AG12), 0)</f>
         <v>0</v>
       </c>
       <c r="AV12" s="247">
@@ -11201,16 +11189,14 @@
       <c r="E13" s="353">
         <v>60.15</v>
       </c>
-      <c r="F13" s="354">
-        <v>20.0</v>
-      </c>
+      <c r="F13" s="354"/>
       <c r="G13" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H13" s="236">
         <f t="shared" si="8"/>
-        <v>1203</v>
+        <v>0</v>
       </c>
       <c r="I13" s="355"/>
       <c r="J13" s="259" t="b">
@@ -11352,7 +11338,7 @@
         <v>n/a</v>
       </c>
       <c r="AU13" s="247">
-        <f>iferror((Reference!$B$10-AT13)*AE13 - AG13, 0)</f>
+        <f>iferror((Reference!$B$10-AT13)*(AE13 - AG13), 0)</f>
         <v>0</v>
       </c>
       <c r="AV13" s="247">
@@ -11378,16 +11364,14 @@
       <c r="E14" s="353">
         <v>45.49</v>
       </c>
-      <c r="F14" s="354">
-        <v>25.0</v>
-      </c>
+      <c r="F14" s="354"/>
       <c r="G14" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H14" s="236">
         <f t="shared" si="8"/>
-        <v>1137.25</v>
+        <v>0</v>
       </c>
       <c r="I14" s="355"/>
       <c r="J14" s="259" t="b">
@@ -11529,7 +11513,7 @@
         <v>n/a</v>
       </c>
       <c r="AU14" s="247">
-        <f>iferror((Reference!$B$10-AT14)*AE14 - AG14, 0)</f>
+        <f>iferror((Reference!$B$10-AT14)*(AE14 - AG14), 0)</f>
         <v>0</v>
       </c>
       <c r="AV14" s="247">
@@ -11555,16 +11539,14 @@
       <c r="E15" s="353">
         <v>56.91</v>
       </c>
-      <c r="F15" s="354">
-        <v>24.0</v>
-      </c>
+      <c r="F15" s="354"/>
       <c r="G15" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H15" s="236">
         <f t="shared" si="8"/>
-        <v>1365.84</v>
+        <v>0</v>
       </c>
       <c r="I15" s="355"/>
       <c r="J15" s="259" t="b">
@@ -11706,7 +11688,7 @@
         <v>n/a</v>
       </c>
       <c r="AU15" s="247">
-        <f>iferror((Reference!$B$10-AT15)*AE15 - AG15, 0)</f>
+        <f>iferror((Reference!$B$10-AT15)*(AE15 - AG15), 0)</f>
         <v>0</v>
       </c>
       <c r="AV15" s="247">
@@ -11732,16 +11714,14 @@
       <c r="E16" s="353">
         <v>56.91</v>
       </c>
-      <c r="F16" s="354">
-        <v>46.0</v>
-      </c>
+      <c r="F16" s="354"/>
       <c r="G16" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H16" s="236">
         <f t="shared" si="8"/>
-        <v>2617.86</v>
+        <v>0</v>
       </c>
       <c r="I16" s="355"/>
       <c r="J16" s="259" t="b">
@@ -11883,7 +11863,7 @@
         <v>n/a</v>
       </c>
       <c r="AU16" s="247">
-        <f>iferror((Reference!$B$10-AT16)*AE16 - AG16, 0)</f>
+        <f>iferror((Reference!$B$10-AT16)*(AE16 - AG16), 0)</f>
         <v>0</v>
       </c>
       <c r="AV16" s="247">
@@ -11909,16 +11889,14 @@
       <c r="E17" s="353">
         <v>77.97</v>
       </c>
-      <c r="F17" s="354">
-        <v>21.0</v>
-      </c>
+      <c r="F17" s="354"/>
       <c r="G17" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H17" s="236">
         <f t="shared" si="8"/>
-        <v>1637.37</v>
+        <v>0</v>
       </c>
       <c r="I17" s="355"/>
       <c r="J17" s="259" t="b">
@@ -12060,7 +12038,7 @@
         <v>n/a</v>
       </c>
       <c r="AU17" s="247">
-        <f>iferror((Reference!$B$10-AT17)*AE17 - AG17, 0)</f>
+        <f>iferror((Reference!$B$10-AT17)*(AE17 - AG17), 0)</f>
         <v>0</v>
       </c>
       <c r="AV17" s="247">
@@ -12086,16 +12064,14 @@
       <c r="E18" s="353">
         <v>77.97</v>
       </c>
-      <c r="F18" s="354">
-        <v>20.0</v>
-      </c>
+      <c r="F18" s="354"/>
       <c r="G18" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H18" s="236">
         <f t="shared" si="8"/>
-        <v>1559.4</v>
+        <v>0</v>
       </c>
       <c r="I18" s="355"/>
       <c r="J18" s="259" t="b">
@@ -12237,7 +12213,7 @@
         <v>n/a</v>
       </c>
       <c r="AU18" s="247">
-        <f>iferror((Reference!$B$10-AT18)*AE18 - AG18, 0)</f>
+        <f>iferror((Reference!$B$10-AT18)*(AE18 - AG18), 0)</f>
         <v>0</v>
       </c>
       <c r="AV18" s="247">
@@ -12263,16 +12239,14 @@
       <c r="E19" s="353">
         <v>78.04</v>
       </c>
-      <c r="F19" s="354">
-        <v>571.0</v>
-      </c>
+      <c r="F19" s="354"/>
       <c r="G19" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H19" s="236">
         <f t="shared" si="8"/>
-        <v>44560.84</v>
+        <v>0</v>
       </c>
       <c r="I19" s="355"/>
       <c r="J19" s="259" t="b">
@@ -12414,7 +12388,7 @@
         <v>n/a</v>
       </c>
       <c r="AU19" s="247">
-        <f>iferror((Reference!$B$10-AT19)*AE19 - AG19, 0)</f>
+        <f>iferror((Reference!$B$10-AT19)*(AE19 - AG19), 0)</f>
         <v>0</v>
       </c>
       <c r="AV19" s="247">
@@ -12440,16 +12414,14 @@
       <c r="E20" s="353">
         <v>94.58</v>
       </c>
-      <c r="F20" s="354">
-        <v>24.0</v>
-      </c>
+      <c r="F20" s="354"/>
       <c r="G20" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H20" s="236">
         <f t="shared" si="8"/>
-        <v>2269.92</v>
+        <v>0</v>
       </c>
       <c r="I20" s="355"/>
       <c r="J20" s="259" t="b">
@@ -12591,7 +12563,7 @@
         <v>n/a</v>
       </c>
       <c r="AU20" s="247">
-        <f>iferror((Reference!$B$10-AT20)*AE20 - AG20, 0)</f>
+        <f>iferror((Reference!$B$10-AT20)*(AE20 - AG20), 0)</f>
         <v>0</v>
       </c>
       <c r="AV20" s="247">
@@ -12617,16 +12589,14 @@
       <c r="E21" s="353">
         <v>94.58</v>
       </c>
-      <c r="F21" s="354">
-        <v>23.0</v>
-      </c>
+      <c r="F21" s="354"/>
       <c r="G21" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H21" s="236">
         <f t="shared" si="8"/>
-        <v>2175.34</v>
+        <v>0</v>
       </c>
       <c r="I21" s="355"/>
       <c r="J21" s="259" t="b">
@@ -12768,7 +12738,7 @@
         <v>n/a</v>
       </c>
       <c r="AU21" s="247">
-        <f>iferror((Reference!$B$10-AT21)*AE21 - AG21, 0)</f>
+        <f>iferror((Reference!$B$10-AT21)*(AE21 - AG21), 0)</f>
         <v>0</v>
       </c>
       <c r="AV21" s="247">
@@ -12794,16 +12764,14 @@
       <c r="E22" s="353">
         <v>94.58</v>
       </c>
-      <c r="F22" s="354">
-        <v>118.0</v>
-      </c>
+      <c r="F22" s="354"/>
       <c r="G22" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H22" s="236">
         <f t="shared" si="8"/>
-        <v>11160.44</v>
+        <v>0</v>
       </c>
       <c r="I22" s="367"/>
       <c r="J22" s="259" t="b">
@@ -12945,7 +12913,7 @@
         <v>n/a</v>
       </c>
       <c r="AU22" s="247">
-        <f>iferror((Reference!$B$10-AT22)*AE22 - AG22, 0)</f>
+        <f>iferror((Reference!$B$10-AT22)*(AE22 - AG22), 0)</f>
         <v>0</v>
       </c>
       <c r="AV22" s="247">
@@ -12971,16 +12939,14 @@
       <c r="E23" s="353">
         <v>97.4</v>
       </c>
-      <c r="F23" s="354">
-        <v>286.0</v>
-      </c>
+      <c r="F23" s="354"/>
       <c r="G23" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H23" s="236">
         <f t="shared" si="8"/>
-        <v>27856.4</v>
+        <v>0</v>
       </c>
       <c r="I23" s="355"/>
       <c r="J23" s="259" t="b">
@@ -13122,7 +13088,7 @@
         <v>n/a</v>
       </c>
       <c r="AU23" s="247">
-        <f>iferror((Reference!$B$10-AT23)*AE23 - AG23, 0)</f>
+        <f>iferror((Reference!$B$10-AT23)*(AE23 - AG23), 0)</f>
         <v>0</v>
       </c>
       <c r="AV23" s="247">
@@ -13148,16 +13114,14 @@
       <c r="E24" s="353">
         <v>119.12</v>
       </c>
-      <c r="F24" s="354">
-        <v>20.0</v>
-      </c>
+      <c r="F24" s="354"/>
       <c r="G24" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H24" s="236">
         <f t="shared" si="8"/>
-        <v>2382.4</v>
+        <v>0</v>
       </c>
       <c r="I24" s="355"/>
       <c r="J24" s="259" t="b">
@@ -13299,7 +13263,7 @@
         <v>n/a</v>
       </c>
       <c r="AU24" s="247">
-        <f>iferror((Reference!$B$10-AT24)*AE24 - AG24, 0)</f>
+        <f>iferror((Reference!$B$10-AT24)*(AE24 - AG24), 0)</f>
         <v>0</v>
       </c>
       <c r="AV24" s="247">
@@ -13325,16 +13289,14 @@
       <c r="E25" s="353">
         <v>119.12</v>
       </c>
-      <c r="F25" s="354">
-        <v>20.0</v>
-      </c>
+      <c r="F25" s="354"/>
       <c r="G25" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H25" s="236">
         <f t="shared" si="8"/>
-        <v>2382.4</v>
+        <v>0</v>
       </c>
       <c r="I25" s="367"/>
       <c r="J25" s="259" t="b">
@@ -13476,7 +13438,7 @@
         <v>n/a</v>
       </c>
       <c r="AU25" s="247">
-        <f>iferror((Reference!$B$10-AT25)*AE25 - AG25, 0)</f>
+        <f>iferror((Reference!$B$10-AT25)*(AE25 - AG25), 0)</f>
         <v>0</v>
       </c>
       <c r="AV25" s="247">
@@ -13502,16 +13464,14 @@
       <c r="E26" s="353">
         <v>119.12</v>
       </c>
-      <c r="F26" s="354">
-        <v>58.0</v>
-      </c>
+      <c r="F26" s="354"/>
       <c r="G26" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H26" s="236">
         <f t="shared" si="8"/>
-        <v>6908.96</v>
+        <v>0</v>
       </c>
       <c r="I26" s="355"/>
       <c r="J26" s="259" t="b">
@@ -13653,7 +13613,7 @@
         <v>n/a</v>
       </c>
       <c r="AU26" s="247">
-        <f>iferror((Reference!$B$10-AT26)*AE26 - AG26, 0)</f>
+        <f>iferror((Reference!$B$10-AT26)*(AE26 - AG26), 0)</f>
         <v>0</v>
       </c>
       <c r="AV26" s="247">
@@ -13679,16 +13639,14 @@
       <c r="E27" s="353">
         <v>124.44</v>
       </c>
-      <c r="F27" s="354">
-        <v>290.0</v>
-      </c>
+      <c r="F27" s="354"/>
       <c r="G27" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H27" s="236">
         <f t="shared" si="8"/>
-        <v>36087.6</v>
+        <v>0</v>
       </c>
       <c r="I27" s="355"/>
       <c r="J27" s="259" t="b">
@@ -13830,7 +13788,7 @@
         <v>n/a</v>
       </c>
       <c r="AU27" s="247">
-        <f>iferror((Reference!$B$10-AT27)*AE27 - AG27, 0)</f>
+        <f>iferror((Reference!$B$10-AT27)*(AE27 - AG27), 0)</f>
         <v>0</v>
       </c>
       <c r="AV27" s="247">
@@ -13856,16 +13814,14 @@
       <c r="E28" s="353">
         <v>133.22</v>
       </c>
-      <c r="F28" s="354">
-        <v>23.0</v>
-      </c>
+      <c r="F28" s="354"/>
       <c r="G28" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H28" s="236">
         <f t="shared" si="8"/>
-        <v>3064.06</v>
+        <v>0</v>
       </c>
       <c r="I28" s="367"/>
       <c r="J28" s="259" t="b">
@@ -14007,7 +13963,7 @@
         <v>n/a</v>
       </c>
       <c r="AU28" s="247">
-        <f>iferror((Reference!$B$10-AT28)*AE28 - AG28, 0)</f>
+        <f>iferror((Reference!$B$10-AT28)*(AE28 - AG28), 0)</f>
         <v>0</v>
       </c>
       <c r="AV28" s="247">
@@ -14033,16 +13989,14 @@
       <c r="E29" s="353">
         <v>133.22</v>
       </c>
-      <c r="F29" s="354">
-        <v>22.0</v>
-      </c>
+      <c r="F29" s="354"/>
       <c r="G29" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H29" s="236">
         <f t="shared" si="8"/>
-        <v>2930.84</v>
+        <v>0</v>
       </c>
       <c r="I29" s="355"/>
       <c r="J29" s="259" t="b">
@@ -14184,7 +14138,7 @@
         <v>n/a</v>
       </c>
       <c r="AU29" s="247">
-        <f>iferror((Reference!$B$10-AT29)*AE29 - AG29, 0)</f>
+        <f>iferror((Reference!$B$10-AT29)*(AE29 - AG29), 0)</f>
         <v>0</v>
       </c>
       <c r="AV29" s="247">
@@ -14210,16 +14164,14 @@
       <c r="E30" s="353">
         <v>133.22</v>
       </c>
-      <c r="F30" s="354">
-        <v>63.0</v>
-      </c>
+      <c r="F30" s="354"/>
       <c r="G30" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H30" s="236">
         <f t="shared" si="8"/>
-        <v>8392.86</v>
+        <v>0</v>
       </c>
       <c r="I30" s="367"/>
       <c r="J30" s="259" t="b">
@@ -14361,7 +14313,7 @@
         <v>n/a</v>
       </c>
       <c r="AU30" s="247">
-        <f>iferror((Reference!$B$10-AT30)*AE30 - AG30, 0)</f>
+        <f>iferror((Reference!$B$10-AT30)*(AE30 - AG30), 0)</f>
         <v>0</v>
       </c>
       <c r="AV30" s="247">
@@ -14387,16 +14339,14 @@
       <c r="E31" s="353">
         <v>145.93</v>
       </c>
-      <c r="F31" s="354">
-        <v>264.0</v>
-      </c>
+      <c r="F31" s="354"/>
       <c r="G31" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H31" s="236">
         <f t="shared" si="8"/>
-        <v>38525.52</v>
+        <v>0</v>
       </c>
       <c r="I31" s="355"/>
       <c r="J31" s="259" t="b">
@@ -14538,7 +14488,7 @@
         <v>n/a</v>
       </c>
       <c r="AU31" s="247">
-        <f>iferror((Reference!$B$10-AT31)*AE31 - AG31, 0)</f>
+        <f>iferror((Reference!$B$10-AT31)*(AE31 - AG31), 0)</f>
         <v>0</v>
       </c>
       <c r="AV31" s="247">
@@ -14564,16 +14514,14 @@
       <c r="E32" s="353">
         <v>146.97</v>
       </c>
-      <c r="F32" s="354">
-        <v>85.0</v>
-      </c>
+      <c r="F32" s="354"/>
       <c r="G32" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H32" s="236">
         <f t="shared" si="8"/>
-        <v>12492.45</v>
+        <v>0</v>
       </c>
       <c r="I32" s="355"/>
       <c r="J32" s="259" t="b">
@@ -14715,7 +14663,7 @@
         <v>n/a</v>
       </c>
       <c r="AU32" s="247">
-        <f>iferror((Reference!$B$10-AT32)*AE32 - AG32, 0)</f>
+        <f>iferror((Reference!$B$10-AT32)*(AE32 - AG32), 0)</f>
         <v>0</v>
       </c>
       <c r="AV32" s="247">
@@ -14741,16 +14689,14 @@
       <c r="E33" s="353">
         <v>144.64</v>
       </c>
-      <c r="F33" s="354">
-        <v>19.0</v>
-      </c>
+      <c r="F33" s="354"/>
       <c r="G33" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H33" s="236">
         <f t="shared" si="8"/>
-        <v>2748.16</v>
+        <v>0</v>
       </c>
       <c r="I33" s="355"/>
       <c r="J33" s="259" t="b">
@@ -14892,7 +14838,7 @@
         <v>n/a</v>
       </c>
       <c r="AU33" s="247">
-        <f>iferror((Reference!$B$10-AT33)*AE33 - AG33, 0)</f>
+        <f>iferror((Reference!$B$10-AT33)*(AE33 - AG33), 0)</f>
         <v>0</v>
       </c>
       <c r="AV33" s="247">
@@ -14918,16 +14864,14 @@
       <c r="E34" s="353">
         <v>144.64</v>
       </c>
-      <c r="F34" s="354">
-        <v>54.0</v>
-      </c>
+      <c r="F34" s="354"/>
       <c r="G34" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H34" s="236">
         <f t="shared" si="8"/>
-        <v>7810.56</v>
+        <v>0</v>
       </c>
       <c r="I34" s="355"/>
       <c r="J34" s="259" t="b">
@@ -15069,7 +15013,7 @@
         <v>n/a</v>
       </c>
       <c r="AU34" s="247">
-        <f>iferror((Reference!$B$10-AT34)*AE34 - AG34, 0)</f>
+        <f>iferror((Reference!$B$10-AT34)*(AE34 - AG34), 0)</f>
         <v>0</v>
       </c>
       <c r="AV34" s="247">
@@ -15095,16 +15039,14 @@
       <c r="E35" s="353">
         <v>167.34</v>
       </c>
-      <c r="F35" s="354">
-        <v>267.0</v>
-      </c>
+      <c r="F35" s="354"/>
       <c r="G35" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H35" s="236">
         <f t="shared" si="8"/>
-        <v>44679.78</v>
+        <v>0</v>
       </c>
       <c r="I35" s="355"/>
       <c r="J35" s="259" t="b">
@@ -15246,7 +15188,7 @@
         <v>n/a</v>
       </c>
       <c r="AU35" s="247">
-        <f>iferror((Reference!$B$10-AT35)*AE35 - AG35, 0)</f>
+        <f>iferror((Reference!$B$10-AT35)*(AE35 - AG35), 0)</f>
         <v>0</v>
       </c>
       <c r="AV35" s="247">
@@ -15272,16 +15214,14 @@
       <c r="E36" s="353">
         <v>148.88</v>
       </c>
-      <c r="F36" s="354">
-        <v>61.0</v>
-      </c>
+      <c r="F36" s="354"/>
       <c r="G36" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H36" s="236">
         <f t="shared" si="8"/>
-        <v>9081.68</v>
+        <v>0</v>
       </c>
       <c r="I36" s="355"/>
       <c r="J36" s="259" t="b">
@@ -15423,7 +15363,7 @@
         <v>n/a</v>
       </c>
       <c r="AU36" s="247">
-        <f>iferror((Reference!$B$10-AT36)*AE36 - AG36, 0)</f>
+        <f>iferror((Reference!$B$10-AT36)*(AE36 - AG36), 0)</f>
         <v>0</v>
       </c>
       <c r="AV36" s="247">
@@ -15449,16 +15389,14 @@
       <c r="E37" s="353">
         <v>202.46</v>
       </c>
-      <c r="F37" s="354">
-        <v>23.0</v>
-      </c>
+      <c r="F37" s="354"/>
       <c r="G37" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H37" s="236">
         <f t="shared" si="8"/>
-        <v>4656.58</v>
+        <v>0</v>
       </c>
       <c r="I37" s="355"/>
       <c r="J37" s="259" t="b">
@@ -15600,7 +15538,7 @@
         <v>n/a</v>
       </c>
       <c r="AU37" s="247">
-        <f>iferror((Reference!$B$10-AT37)*AE37 - AG37, 0)</f>
+        <f>iferror((Reference!$B$10-AT37)*(AE37 - AG37), 0)</f>
         <v>0</v>
       </c>
       <c r="AV37" s="247">
@@ -15626,16 +15564,14 @@
       <c r="E38" s="353">
         <v>202.46</v>
       </c>
-      <c r="F38" s="354">
-        <v>63.0</v>
-      </c>
+      <c r="F38" s="354"/>
       <c r="G38" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H38" s="236">
         <f t="shared" si="8"/>
-        <v>12754.98</v>
+        <v>0</v>
       </c>
       <c r="I38" s="355"/>
       <c r="J38" s="259" t="b">
@@ -15777,7 +15713,7 @@
         <v>n/a</v>
       </c>
       <c r="AU38" s="247">
-        <f>iferror((Reference!$B$10-AT38)*AE38 - AG38, 0)</f>
+        <f>iferror((Reference!$B$10-AT38)*(AE38 - AG38), 0)</f>
         <v>0</v>
       </c>
       <c r="AV38" s="247">
@@ -15803,16 +15739,14 @@
       <c r="E39" s="353">
         <v>176.98</v>
       </c>
-      <c r="F39" s="354">
-        <v>71.0</v>
-      </c>
+      <c r="F39" s="354"/>
       <c r="G39" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H39" s="236">
         <f t="shared" si="8"/>
-        <v>12565.58</v>
+        <v>0</v>
       </c>
       <c r="I39" s="367"/>
       <c r="J39" s="259" t="b">
@@ -15954,7 +15888,7 @@
         <v>n/a</v>
       </c>
       <c r="AU39" s="247">
-        <f>iferror((Reference!$B$10-AT39)*AE39 - AG39, 0)</f>
+        <f>iferror((Reference!$B$10-AT39)*(AE39 - AG39), 0)</f>
         <v>0</v>
       </c>
       <c r="AV39" s="247">
@@ -15980,16 +15914,14 @@
       <c r="E40" s="353">
         <v>168.77</v>
       </c>
-      <c r="F40" s="354">
-        <v>51.0</v>
-      </c>
+      <c r="F40" s="354"/>
       <c r="G40" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H40" s="236">
         <f t="shared" si="8"/>
-        <v>8607.27</v>
+        <v>0</v>
       </c>
       <c r="I40" s="355"/>
       <c r="J40" s="259" t="b">
@@ -16131,7 +16063,7 @@
         <v>n/a</v>
       </c>
       <c r="AU40" s="247">
-        <f>iferror((Reference!$B$10-AT40)*AE40 - AG40, 0)</f>
+        <f>iferror((Reference!$B$10-AT40)*(AE40 - AG40), 0)</f>
         <v>0</v>
       </c>
       <c r="AV40" s="247">
@@ -16157,16 +16089,14 @@
       <c r="E41" s="353">
         <v>163.06</v>
       </c>
-      <c r="F41" s="354">
-        <v>65.0</v>
-      </c>
+      <c r="F41" s="354"/>
       <c r="G41" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H41" s="236">
         <f t="shared" si="8"/>
-        <v>10598.9</v>
+        <v>0</v>
       </c>
       <c r="I41" s="367"/>
       <c r="J41" s="259" t="b">
@@ -16308,7 +16238,7 @@
         <v>n/a</v>
       </c>
       <c r="AU41" s="247">
-        <f>iferror((Reference!$B$10-AT41)*AE41 - AG41, 0)</f>
+        <f>iferror((Reference!$B$10-AT41)*(AE41 - AG41), 0)</f>
         <v>0</v>
       </c>
       <c r="AV41" s="247">
@@ -16334,16 +16264,14 @@
       <c r="E42" s="353">
         <v>155.62</v>
       </c>
-      <c r="F42" s="354">
-        <v>36.0</v>
-      </c>
+      <c r="F42" s="354"/>
       <c r="G42" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H42" s="236">
         <f t="shared" si="8"/>
-        <v>5602.32</v>
+        <v>0</v>
       </c>
       <c r="I42" s="367"/>
       <c r="J42" s="259" t="b">
@@ -16485,7 +16413,7 @@
         <v>n/a</v>
       </c>
       <c r="AU42" s="247">
-        <f>iferror((Reference!$B$10-AT42)*AE42 - AG42, 0)</f>
+        <f>iferror((Reference!$B$10-AT42)*(AE42 - AG42), 0)</f>
         <v>0</v>
       </c>
       <c r="AV42" s="247">
@@ -16511,16 +16439,14 @@
       <c r="E43" s="353">
         <v>151.79</v>
       </c>
-      <c r="F43" s="354">
-        <v>61.0</v>
-      </c>
+      <c r="F43" s="354"/>
       <c r="G43" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H43" s="236">
         <f t="shared" si="8"/>
-        <v>9259.19</v>
+        <v>0</v>
       </c>
       <c r="I43" s="355"/>
       <c r="J43" s="259" t="b">
@@ -16662,7 +16588,7 @@
         <v>n/a</v>
       </c>
       <c r="AU43" s="247">
-        <f>iferror((Reference!$B$10-AT43)*AE43 - AG43, 0)</f>
+        <f>iferror((Reference!$B$10-AT43)*(AE43 - AG43), 0)</f>
         <v>0</v>
       </c>
       <c r="AV43" s="247">
@@ -16684,9 +16610,7 @@
       <c r="E44" s="353">
         <v>148.06</v>
       </c>
-      <c r="F44" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F44" s="354"/>
       <c r="G44" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -16835,7 +16759,7 @@
         <v>n/a</v>
       </c>
       <c r="AU44" s="247">
-        <f>iferror((Reference!$B$10-AT44)*AE44 - AG44, 0)</f>
+        <f>iferror((Reference!$B$10-AT44)*(AE44 - AG44), 0)</f>
         <v>0</v>
       </c>
       <c r="AV44" s="247">
@@ -16857,9 +16781,7 @@
       <c r="E45" s="223">
         <v>120.52</v>
       </c>
-      <c r="F45" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F45" s="354"/>
       <c r="G45" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -17008,7 +16930,7 @@
         <v>n/a</v>
       </c>
       <c r="AU45" s="247">
-        <f>iferror((Reference!$B$10-AT45)*AE45 - AG45, 0)</f>
+        <f>iferror((Reference!$B$10-AT45)*(AE45 - AG45), 0)</f>
         <v>0</v>
       </c>
       <c r="AV45" s="247">
@@ -17034,16 +16956,14 @@
       <c r="E46" s="353">
         <v>125.34</v>
       </c>
-      <c r="F46" s="354">
-        <v>68.0</v>
-      </c>
+      <c r="F46" s="354"/>
       <c r="G46" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H46" s="236">
         <f t="shared" si="8"/>
-        <v>8523.12</v>
+        <v>0</v>
       </c>
       <c r="I46" s="355"/>
       <c r="J46" s="259" t="b">
@@ -17185,7 +17105,7 @@
         <v>n/a</v>
       </c>
       <c r="AU46" s="247">
-        <f>iferror((Reference!$B$10-AT46)*AE46 - AG46, 0)</f>
+        <f>iferror((Reference!$B$10-AT46)*(AE46 - AG46), 0)</f>
         <v>0</v>
       </c>
       <c r="AV46" s="247">
@@ -17211,16 +17131,14 @@
       <c r="E47" s="353">
         <v>154.14</v>
       </c>
-      <c r="F47" s="354">
-        <v>89.0</v>
-      </c>
+      <c r="F47" s="354"/>
       <c r="G47" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H47" s="236">
         <f t="shared" si="8"/>
-        <v>13718.46</v>
+        <v>0</v>
       </c>
       <c r="I47" s="367"/>
       <c r="J47" s="259" t="b">
@@ -17362,7 +17280,7 @@
         <v>n/a</v>
       </c>
       <c r="AU47" s="247">
-        <f>iferror((Reference!$B$10-AT47)*AE47 - AG47, 0)</f>
+        <f>iferror((Reference!$B$10-AT47)*(AE47 - AG47), 0)</f>
         <v>0</v>
       </c>
       <c r="AV47" s="247">
@@ -17388,16 +17306,14 @@
       <c r="E48" s="353">
         <v>154.14</v>
       </c>
-      <c r="F48" s="354">
-        <v>35.0</v>
-      </c>
+      <c r="F48" s="354"/>
       <c r="G48" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H48" s="236">
         <f t="shared" si="8"/>
-        <v>5394.9</v>
+        <v>0</v>
       </c>
       <c r="I48" s="355"/>
       <c r="J48" s="259" t="b">
@@ -17539,7 +17455,7 @@
         <v>n/a</v>
       </c>
       <c r="AU48" s="247">
-        <f>iferror((Reference!$B$10-AT48)*AE48 - AG48, 0)</f>
+        <f>iferror((Reference!$B$10-AT48)*(AE48 - AG48), 0)</f>
         <v>0</v>
       </c>
       <c r="AV48" s="247">
@@ -17565,16 +17481,14 @@
       <c r="E49" s="353">
         <v>153.1</v>
       </c>
-      <c r="F49" s="354">
-        <v>51.0</v>
-      </c>
+      <c r="F49" s="354"/>
       <c r="G49" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H49" s="236">
         <f t="shared" si="8"/>
-        <v>7808.1</v>
+        <v>0</v>
       </c>
       <c r="I49" s="355"/>
       <c r="J49" s="259" t="b">
@@ -17716,7 +17630,7 @@
         <v>n/a</v>
       </c>
       <c r="AU49" s="247">
-        <f>iferror((Reference!$B$10-AT49)*AE49 - AG49, 0)</f>
+        <f>iferror((Reference!$B$10-AT49)*(AE49 - AG49), 0)</f>
         <v>0</v>
       </c>
       <c r="AV49" s="247">
@@ -17738,9 +17652,7 @@
       <c r="E50" s="353">
         <v>141.28</v>
       </c>
-      <c r="F50" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F50" s="354"/>
       <c r="G50" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -17889,7 +17801,7 @@
         <v>n/a</v>
       </c>
       <c r="AU50" s="247">
-        <f>iferror((Reference!$B$10-AT50)*AE50 - AG50, 0)</f>
+        <f>iferror((Reference!$B$10-AT50)*(AE50 - AG50), 0)</f>
         <v>0</v>
       </c>
       <c r="AV50" s="247">
@@ -17915,16 +17827,14 @@
       <c r="E51" s="353">
         <v>140.75</v>
       </c>
-      <c r="F51" s="354">
-        <v>45.0</v>
-      </c>
+      <c r="F51" s="354"/>
       <c r="G51" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H51" s="236">
         <f t="shared" si="8"/>
-        <v>6333.75</v>
+        <v>0</v>
       </c>
       <c r="I51" s="367"/>
       <c r="J51" s="259" t="b">
@@ -18066,7 +17976,7 @@
         <v>n/a</v>
       </c>
       <c r="AU51" s="247">
-        <f>iferror((Reference!$B$10-AT51)*AE51 - AG51, 0)</f>
+        <f>iferror((Reference!$B$10-AT51)*(AE51 - AG51), 0)</f>
         <v>0</v>
       </c>
       <c r="AV51" s="247">
@@ -18092,16 +18002,14 @@
       <c r="E52" s="353">
         <v>140.75</v>
       </c>
-      <c r="F52" s="354">
-        <v>36.0</v>
-      </c>
+      <c r="F52" s="354"/>
       <c r="G52" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H52" s="236">
         <f t="shared" si="8"/>
-        <v>5067</v>
+        <v>0</v>
       </c>
       <c r="I52" s="355"/>
       <c r="J52" s="259" t="b">
@@ -18243,7 +18151,7 @@
         <v>n/a</v>
       </c>
       <c r="AU52" s="247">
-        <f>iferror((Reference!$B$10-AT52)*AE52 - AG52, 0)</f>
+        <f>iferror((Reference!$B$10-AT52)*(AE52 - AG52), 0)</f>
         <v>0</v>
       </c>
       <c r="AV52" s="247">
@@ -18269,16 +18177,14 @@
       <c r="E53" s="353">
         <v>140.26</v>
       </c>
-      <c r="F53" s="354">
-        <v>61.0</v>
-      </c>
+      <c r="F53" s="354"/>
       <c r="G53" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H53" s="236">
         <f t="shared" si="8"/>
-        <v>8555.86</v>
+        <v>0</v>
       </c>
       <c r="I53" s="367"/>
       <c r="J53" s="259" t="b">
@@ -18420,7 +18326,7 @@
         <v>n/a</v>
       </c>
       <c r="AU53" s="247">
-        <f>iferror((Reference!$B$10-AT53)*AE53 - AG53, 0)</f>
+        <f>iferror((Reference!$B$10-AT53)*(AE53 - AG53), 0)</f>
         <v>0</v>
       </c>
       <c r="AV53" s="247">
@@ -18442,9 +18348,7 @@
       <c r="E54" s="353">
         <v>140.41</v>
       </c>
-      <c r="F54" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F54" s="354"/>
       <c r="G54" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -18593,7 +18497,7 @@
         <v>n/a</v>
       </c>
       <c r="AU54" s="247">
-        <f>iferror((Reference!$B$10-AT54)*AE54 - AG54, 0)</f>
+        <f>iferror((Reference!$B$10-AT54)*(AE54 - AG54), 0)</f>
         <v>0</v>
       </c>
       <c r="AV54" s="247">
@@ -18619,16 +18523,14 @@
       <c r="E55" s="353">
         <v>160.83</v>
       </c>
-      <c r="F55" s="354">
-        <v>107.0</v>
-      </c>
+      <c r="F55" s="354"/>
       <c r="G55" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H55" s="236">
         <f t="shared" si="8"/>
-        <v>17208.81</v>
+        <v>0</v>
       </c>
       <c r="I55" s="355"/>
       <c r="J55" s="259" t="b">
@@ -18770,7 +18672,7 @@
         <v>n/a</v>
       </c>
       <c r="AU55" s="247">
-        <f>iferror((Reference!$B$10-AT55)*AE55 - AG55, 0)</f>
+        <f>iferror((Reference!$B$10-AT55)*(AE55 - AG55), 0)</f>
         <v>0</v>
       </c>
       <c r="AV55" s="247">
@@ -18796,16 +18698,14 @@
       <c r="E56" s="353">
         <v>161.26</v>
       </c>
-      <c r="F56" s="354">
-        <v>45.0</v>
-      </c>
+      <c r="F56" s="354"/>
       <c r="G56" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H56" s="236">
         <f t="shared" si="8"/>
-        <v>7256.7</v>
+        <v>0</v>
       </c>
       <c r="I56" s="355"/>
       <c r="J56" s="259" t="b">
@@ -18947,7 +18847,7 @@
         <v>n/a</v>
       </c>
       <c r="AU56" s="247">
-        <f>iferror((Reference!$B$10-AT56)*AE56 - AG56, 0)</f>
+        <f>iferror((Reference!$B$10-AT56)*(AE56 - AG56), 0)</f>
         <v>0</v>
       </c>
       <c r="AV56" s="247">
@@ -18973,16 +18873,14 @@
       <c r="E57" s="353">
         <v>161.26</v>
       </c>
-      <c r="F57" s="354">
-        <v>36.0</v>
-      </c>
+      <c r="F57" s="354"/>
       <c r="G57" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H57" s="236">
         <f t="shared" si="8"/>
-        <v>5805.36</v>
+        <v>0</v>
       </c>
       <c r="I57" s="355"/>
       <c r="J57" s="259" t="b">
@@ -19124,7 +19022,7 @@
         <v>n/a</v>
       </c>
       <c r="AU57" s="247">
-        <f>iferror((Reference!$B$10-AT57)*AE57 - AG57, 0)</f>
+        <f>iferror((Reference!$B$10-AT57)*(AE57 - AG57), 0)</f>
         <v>0</v>
       </c>
       <c r="AV57" s="247">
@@ -19150,16 +19048,14 @@
       <c r="E58" s="353">
         <v>156.13</v>
       </c>
-      <c r="F58" s="354">
-        <v>50.0</v>
-      </c>
+      <c r="F58" s="354"/>
       <c r="G58" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H58" s="236">
         <f t="shared" si="8"/>
-        <v>7806.5</v>
+        <v>0</v>
       </c>
       <c r="I58" s="355"/>
       <c r="J58" s="259" t="b">
@@ -19301,7 +19197,7 @@
         <v>n/a</v>
       </c>
       <c r="AU58" s="247">
-        <f>iferror((Reference!$B$10-AT58)*AE58 - AG58, 0)</f>
+        <f>iferror((Reference!$B$10-AT58)*(AE58 - AG58), 0)</f>
         <v>0</v>
       </c>
       <c r="AV58" s="247">
@@ -19323,9 +19219,7 @@
       <c r="E59" s="353">
         <v>146.86</v>
       </c>
-      <c r="F59" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F59" s="354"/>
       <c r="G59" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -19474,7 +19368,7 @@
         <v>n/a</v>
       </c>
       <c r="AU59" s="247">
-        <f>iferror((Reference!$B$10-AT59)*AE59 - AG59, 0)</f>
+        <f>iferror((Reference!$B$10-AT59)*(AE59 - AG59), 0)</f>
         <v>0</v>
       </c>
       <c r="AV59" s="247">
@@ -19500,16 +19394,14 @@
       <c r="E60" s="353">
         <v>124.18</v>
       </c>
-      <c r="F60" s="354">
-        <v>67.0</v>
-      </c>
+      <c r="F60" s="354"/>
       <c r="G60" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H60" s="236">
         <f t="shared" si="8"/>
-        <v>8320.06</v>
+        <v>0</v>
       </c>
       <c r="I60" s="355"/>
       <c r="J60" s="259" t="b">
@@ -19651,7 +19543,7 @@
         <v>n/a</v>
       </c>
       <c r="AU60" s="247">
-        <f>iferror((Reference!$B$10-AT60)*AE60 - AG60, 0)</f>
+        <f>iferror((Reference!$B$10-AT60)*(AE60 - AG60), 0)</f>
         <v>0</v>
       </c>
       <c r="AV60" s="247">
@@ -19677,16 +19569,14 @@
       <c r="E61" s="353">
         <v>114.0</v>
       </c>
-      <c r="F61" s="354">
-        <v>44.0</v>
-      </c>
+      <c r="F61" s="354"/>
       <c r="G61" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H61" s="236">
         <f t="shared" si="8"/>
-        <v>5016</v>
+        <v>0</v>
       </c>
       <c r="I61" s="355"/>
       <c r="J61" s="259" t="b">
@@ -19828,7 +19718,7 @@
         <v>n/a</v>
       </c>
       <c r="AU61" s="247">
-        <f>iferror((Reference!$B$10-AT61)*AE61 - AG61, 0)</f>
+        <f>iferror((Reference!$B$10-AT61)*(AE61 - AG61), 0)</f>
         <v>0</v>
       </c>
       <c r="AV61" s="247">
@@ -19854,16 +19744,14 @@
       <c r="E62" s="353">
         <v>114.0</v>
       </c>
-      <c r="F62" s="354">
-        <v>55.0</v>
-      </c>
+      <c r="F62" s="354"/>
       <c r="G62" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H62" s="236">
         <f t="shared" si="8"/>
-        <v>6270</v>
+        <v>0</v>
       </c>
       <c r="I62" s="355"/>
       <c r="J62" s="259" t="b">
@@ -20005,7 +19893,7 @@
         <v>n/a</v>
       </c>
       <c r="AU62" s="247">
-        <f>iferror((Reference!$B$10-AT62)*AE62 - AG62, 0)</f>
+        <f>iferror((Reference!$B$10-AT62)*(AE62 - AG62), 0)</f>
         <v>0</v>
       </c>
       <c r="AV62" s="247">
@@ -20027,9 +19915,7 @@
       <c r="E63" s="353">
         <v>115.88</v>
       </c>
-      <c r="F63" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F63" s="354"/>
       <c r="G63" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -20178,7 +20064,7 @@
         <v>n/a</v>
       </c>
       <c r="AU63" s="247">
-        <f>iferror((Reference!$B$10-AT63)*AE63 - AG63, 0)</f>
+        <f>iferror((Reference!$B$10-AT63)*(AE63 - AG63), 0)</f>
         <v>0</v>
       </c>
       <c r="AV63" s="247">
@@ -20204,16 +20090,14 @@
       <c r="E64" s="353">
         <v>128.47</v>
       </c>
-      <c r="F64" s="354">
-        <v>92.0</v>
-      </c>
+      <c r="F64" s="354"/>
       <c r="G64" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H64" s="236">
         <f t="shared" si="8"/>
-        <v>11819.24</v>
+        <v>0</v>
       </c>
       <c r="I64" s="355"/>
       <c r="J64" s="259" t="b">
@@ -20355,7 +20239,7 @@
         <v>n/a</v>
       </c>
       <c r="AU64" s="247">
-        <f>iferror((Reference!$B$10-AT64)*AE64 - AG64, 0)</f>
+        <f>iferror((Reference!$B$10-AT64)*(AE64 - AG64), 0)</f>
         <v>0</v>
       </c>
       <c r="AV64" s="247">
@@ -20377,9 +20261,7 @@
       <c r="E65" s="353">
         <v>115.91</v>
       </c>
-      <c r="F65" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F65" s="354"/>
       <c r="G65" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -20528,7 +20410,7 @@
         <v>n/a</v>
       </c>
       <c r="AU65" s="247">
-        <f>iferror((Reference!$B$10-AT65)*AE65 - AG65, 0)</f>
+        <f>iferror((Reference!$B$10-AT65)*(AE65 - AG65), 0)</f>
         <v>0</v>
       </c>
       <c r="AV65" s="247">
@@ -20554,16 +20436,14 @@
       <c r="E66" s="353">
         <v>108.04</v>
       </c>
-      <c r="F66" s="354">
-        <v>65.0</v>
-      </c>
+      <c r="F66" s="354"/>
       <c r="G66" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H66" s="236">
         <f t="shared" si="8"/>
-        <v>7022.6</v>
+        <v>0</v>
       </c>
       <c r="I66" s="355"/>
       <c r="J66" s="259" t="b">
@@ -20705,7 +20585,7 @@
         <v>n/a</v>
       </c>
       <c r="AU66" s="247">
-        <f>iferror((Reference!$B$10-AT66)*AE66 - AG66, 0)</f>
+        <f>iferror((Reference!$B$10-AT66)*(AE66 - AG66), 0)</f>
         <v>0</v>
       </c>
       <c r="AV66" s="247">
@@ -20731,16 +20611,14 @@
       <c r="E67" s="353">
         <v>108.04</v>
       </c>
-      <c r="F67" s="354">
-        <v>26.0</v>
-      </c>
+      <c r="F67" s="354"/>
       <c r="G67" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H67" s="236">
         <f t="shared" si="8"/>
-        <v>2809.04</v>
+        <v>0</v>
       </c>
       <c r="I67" s="355"/>
       <c r="J67" s="259" t="b">
@@ -20882,7 +20760,7 @@
         <v>n/a</v>
       </c>
       <c r="AU67" s="247">
-        <f>iferror((Reference!$B$10-AT67)*AE67 - AG67, 0)</f>
+        <f>iferror((Reference!$B$10-AT67)*(AE67 - AG67), 0)</f>
         <v>0</v>
       </c>
       <c r="AV67" s="247">
@@ -20908,16 +20786,14 @@
       <c r="E68" s="353">
         <v>129.41</v>
       </c>
-      <c r="F68" s="354">
-        <v>44.0</v>
-      </c>
+      <c r="F68" s="354"/>
       <c r="G68" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H68" s="236">
         <f t="shared" si="8"/>
-        <v>5694.04</v>
+        <v>0</v>
       </c>
       <c r="I68" s="355"/>
       <c r="J68" s="259" t="b">
@@ -21059,7 +20935,7 @@
         <v>n/a</v>
       </c>
       <c r="AU68" s="247">
-        <f>iferror((Reference!$B$10-AT68)*AE68 - AG68, 0)</f>
+        <f>iferror((Reference!$B$10-AT68)*(AE68 - AG68), 0)</f>
         <v>0</v>
       </c>
       <c r="AV68" s="247">
@@ -21085,16 +20961,14 @@
       <c r="E69" s="353">
         <v>129.41</v>
       </c>
-      <c r="F69" s="354">
-        <v>55.0</v>
-      </c>
+      <c r="F69" s="354"/>
       <c r="G69" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H69" s="236">
         <f t="shared" si="8"/>
-        <v>7117.55</v>
+        <v>0</v>
       </c>
       <c r="I69" s="367"/>
       <c r="J69" s="259" t="b">
@@ -21236,7 +21110,7 @@
         <v>n/a</v>
       </c>
       <c r="AU69" s="247">
-        <f>iferror((Reference!$B$10-AT69)*AE69 - AG69, 0)</f>
+        <f>iferror((Reference!$B$10-AT69)*(AE69 - AG69), 0)</f>
         <v>0</v>
       </c>
       <c r="AV69" s="247">
@@ -21258,9 +21132,7 @@
       <c r="E70" s="353">
         <v>114.06</v>
       </c>
-      <c r="F70" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F70" s="354"/>
       <c r="G70" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -21409,7 +21281,7 @@
         <v>n/a</v>
       </c>
       <c r="AU70" s="247">
-        <f>iferror((Reference!$B$10-AT70)*AE70 - AG70, 0)</f>
+        <f>iferror((Reference!$B$10-AT70)*(AE70 - AG70), 0)</f>
         <v>0</v>
       </c>
       <c r="AV70" s="247">
@@ -21435,16 +21307,14 @@
       <c r="E71" s="353">
         <v>116.17</v>
       </c>
-      <c r="F71" s="354">
-        <v>26.0</v>
-      </c>
+      <c r="F71" s="354"/>
       <c r="G71" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H71" s="236">
         <f t="shared" si="8"/>
-        <v>3020.42</v>
+        <v>0</v>
       </c>
       <c r="I71" s="355"/>
       <c r="J71" s="259" t="b">
@@ -21586,7 +21456,7 @@
         <v>n/a</v>
       </c>
       <c r="AU71" s="247">
-        <f>iferror((Reference!$B$10-AT71)*AE71 - AG71, 0)</f>
+        <f>iferror((Reference!$B$10-AT71)*(AE71 - AG71), 0)</f>
         <v>0</v>
       </c>
       <c r="AV71" s="247">
@@ -21608,9 +21478,7 @@
       <c r="E72" s="353">
         <v>114.82</v>
       </c>
-      <c r="F72" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F72" s="354"/>
       <c r="G72" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -21759,7 +21627,7 @@
         <v>n/a</v>
       </c>
       <c r="AU72" s="247">
-        <f>iferror((Reference!$B$10-AT72)*AE72 - AG72, 0)</f>
+        <f>iferror((Reference!$B$10-AT72)*(AE72 - AG72), 0)</f>
         <v>0</v>
       </c>
       <c r="AV72" s="247">
@@ -21785,16 +21653,14 @@
       <c r="E73" s="353">
         <v>112.62</v>
       </c>
-      <c r="F73" s="354">
-        <v>66.0</v>
-      </c>
+      <c r="F73" s="354"/>
       <c r="G73" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H73" s="236">
         <f t="shared" si="8"/>
-        <v>7432.92</v>
+        <v>0</v>
       </c>
       <c r="I73" s="355"/>
       <c r="J73" s="259" t="b">
@@ -21936,7 +21802,7 @@
         <v>n/a</v>
       </c>
       <c r="AU73" s="247">
-        <f>iferror((Reference!$B$10-AT73)*AE73 - AG73, 0)</f>
+        <f>iferror((Reference!$B$10-AT73)*(AE73 - AG73), 0)</f>
         <v>0</v>
       </c>
       <c r="AV73" s="247">
@@ -21962,16 +21828,14 @@
       <c r="E74" s="353">
         <v>112.62</v>
       </c>
-      <c r="F74" s="354">
-        <v>26.0</v>
-      </c>
+      <c r="F74" s="354"/>
       <c r="G74" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H74" s="236">
         <f t="shared" si="8"/>
-        <v>2928.12</v>
+        <v>0</v>
       </c>
       <c r="I74" s="355"/>
       <c r="J74" s="259" t="b">
@@ -22113,7 +21977,7 @@
         <v>n/a</v>
       </c>
       <c r="AU74" s="247">
-        <f>iferror((Reference!$B$10-AT74)*AE74 - AG74, 0)</f>
+        <f>iferror((Reference!$B$10-AT74)*(AE74 - AG74), 0)</f>
         <v>0</v>
       </c>
       <c r="AV74" s="247">
@@ -22139,16 +22003,14 @@
       <c r="E75" s="353">
         <v>121.68</v>
       </c>
-      <c r="F75" s="354">
-        <v>55.0</v>
-      </c>
+      <c r="F75" s="354"/>
       <c r="G75" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H75" s="236">
         <f t="shared" si="8"/>
-        <v>6692.4</v>
+        <v>0</v>
       </c>
       <c r="I75" s="355"/>
       <c r="J75" s="259" t="b">
@@ -22290,7 +22152,7 @@
         <v>n/a</v>
       </c>
       <c r="AU75" s="247">
-        <f>iferror((Reference!$B$10-AT75)*AE75 - AG75, 0)</f>
+        <f>iferror((Reference!$B$10-AT75)*(AE75 - AG75), 0)</f>
         <v>0</v>
       </c>
       <c r="AV75" s="247">
@@ -22312,9 +22174,7 @@
       <c r="E76" s="353">
         <v>122.76</v>
       </c>
-      <c r="F76" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F76" s="354"/>
       <c r="G76" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -22463,7 +22323,7 @@
         <v>n/a</v>
       </c>
       <c r="AU76" s="247">
-        <f>iferror((Reference!$B$10-AT76)*AE76 - AG76, 0)</f>
+        <f>iferror((Reference!$B$10-AT76)*(AE76 - AG76), 0)</f>
         <v>0</v>
       </c>
       <c r="AV76" s="247">
@@ -22489,16 +22349,14 @@
       <c r="E77" s="353">
         <v>123.34</v>
       </c>
-      <c r="F77" s="354">
-        <v>31.0</v>
-      </c>
+      <c r="F77" s="354"/>
       <c r="G77" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H77" s="236">
         <f t="shared" si="8"/>
-        <v>3823.54</v>
+        <v>0</v>
       </c>
       <c r="I77" s="367"/>
       <c r="J77" s="259" t="b">
@@ -22640,7 +22498,7 @@
         <v>n/a</v>
       </c>
       <c r="AU77" s="247">
-        <f>iferror((Reference!$B$10-AT77)*AE77 - AG77, 0)</f>
+        <f>iferror((Reference!$B$10-AT77)*(AE77 - AG77), 0)</f>
         <v>0</v>
       </c>
       <c r="AV77" s="247">
@@ -22666,16 +22524,14 @@
       <c r="E78" s="353">
         <v>110.09</v>
       </c>
-      <c r="F78" s="354">
-        <v>178.0</v>
-      </c>
+      <c r="F78" s="354"/>
       <c r="G78" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H78" s="236">
         <f t="shared" si="8"/>
-        <v>19596.02</v>
+        <v>0</v>
       </c>
       <c r="I78" s="355"/>
       <c r="J78" s="259" t="b">
@@ -22817,7 +22673,7 @@
         <v>n/a</v>
       </c>
       <c r="AU78" s="247">
-        <f>iferror((Reference!$B$10-AT78)*AE78 - AG78, 0)</f>
+        <f>iferror((Reference!$B$10-AT78)*(AE78 - AG78), 0)</f>
         <v>0</v>
       </c>
       <c r="AV78" s="247">
@@ -22843,16 +22699,14 @@
       <c r="E79" s="353">
         <v>126.98</v>
       </c>
-      <c r="F79" s="354">
-        <v>66.0</v>
-      </c>
+      <c r="F79" s="354"/>
       <c r="G79" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H79" s="236">
         <f t="shared" si="8"/>
-        <v>8380.68</v>
+        <v>0</v>
       </c>
       <c r="I79" s="355"/>
       <c r="J79" s="259" t="b">
@@ -22994,7 +22848,7 @@
         <v>n/a</v>
       </c>
       <c r="AU79" s="247">
-        <f>iferror((Reference!$B$10-AT79)*AE79 - AG79, 0)</f>
+        <f>iferror((Reference!$B$10-AT79)*(AE79 - AG79), 0)</f>
         <v>0</v>
       </c>
       <c r="AV79" s="247">
@@ -23020,16 +22874,14 @@
       <c r="E80" s="353">
         <v>126.98</v>
       </c>
-      <c r="F80" s="354">
-        <v>26.0</v>
-      </c>
+      <c r="F80" s="354"/>
       <c r="G80" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H80" s="236">
         <f t="shared" si="8"/>
-        <v>3301.48</v>
+        <v>0</v>
       </c>
       <c r="I80" s="355"/>
       <c r="J80" s="259" t="b">
@@ -23171,7 +23023,7 @@
         <v>n/a</v>
       </c>
       <c r="AU80" s="247">
-        <f>iferror((Reference!$B$10-AT80)*AE80 - AG80, 0)</f>
+        <f>iferror((Reference!$B$10-AT80)*(AE80 - AG80), 0)</f>
         <v>0</v>
       </c>
       <c r="AV80" s="247">
@@ -23197,16 +23049,14 @@
       <c r="E81" s="353">
         <v>133.94</v>
       </c>
-      <c r="F81" s="354">
-        <v>25.0</v>
-      </c>
+      <c r="F81" s="354"/>
       <c r="G81" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H81" s="236">
         <f t="shared" si="8"/>
-        <v>3348.5</v>
+        <v>0</v>
       </c>
       <c r="I81" s="355"/>
       <c r="J81" s="259" t="b">
@@ -23348,7 +23198,7 @@
         <v>n/a</v>
       </c>
       <c r="AU81" s="247">
-        <f>iferror((Reference!$B$10-AT81)*AE81 - AG81, 0)</f>
+        <f>iferror((Reference!$B$10-AT81)*(AE81 - AG81), 0)</f>
         <v>0</v>
       </c>
       <c r="AV81" s="247">
@@ -23374,16 +23224,14 @@
       <c r="E82" s="353">
         <v>133.94</v>
       </c>
-      <c r="F82" s="354">
-        <v>55.0</v>
-      </c>
+      <c r="F82" s="354"/>
       <c r="G82" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H82" s="236">
         <f t="shared" si="8"/>
-        <v>7366.7</v>
+        <v>0</v>
       </c>
       <c r="I82" s="367"/>
       <c r="J82" s="259" t="b">
@@ -23525,7 +23373,7 @@
         <v>n/a</v>
       </c>
       <c r="AU82" s="247">
-        <f>iferror((Reference!$B$10-AT82)*AE82 - AG82, 0)</f>
+        <f>iferror((Reference!$B$10-AT82)*(AE82 - AG82), 0)</f>
         <v>0</v>
       </c>
       <c r="AV82" s="247">
@@ -23551,16 +23399,14 @@
       <c r="E83" s="353">
         <v>158.96</v>
       </c>
-      <c r="F83" s="354">
-        <v>26.0</v>
-      </c>
+      <c r="F83" s="354"/>
       <c r="G83" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H83" s="236">
         <f t="shared" si="8"/>
-        <v>4132.96</v>
+        <v>0</v>
       </c>
       <c r="I83" s="355"/>
       <c r="J83" s="259" t="b">
@@ -23702,7 +23548,7 @@
         <v>n/a</v>
       </c>
       <c r="AU83" s="247">
-        <f>iferror((Reference!$B$10-AT83)*AE83 - AG83, 0)</f>
+        <f>iferror((Reference!$B$10-AT83)*(AE83 - AG83), 0)</f>
         <v>0</v>
       </c>
       <c r="AV83" s="247">
@@ -23728,16 +23574,14 @@
       <c r="E84" s="372">
         <v>164.1</v>
       </c>
-      <c r="F84" s="373">
-        <v>26.0</v>
-      </c>
+      <c r="F84" s="373"/>
       <c r="G84" s="268">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H84" s="279">
         <f t="shared" si="8"/>
-        <v>4266.6</v>
+        <v>0</v>
       </c>
       <c r="I84" s="374"/>
       <c r="J84" s="271" t="b">
@@ -23879,7 +23723,7 @@
         <v>n/a</v>
       </c>
       <c r="AU84" s="290">
-        <f>iferror((Reference!$B$10-AT84)*AE84 - AG84, 0)</f>
+        <f>iferror((Reference!$B$10-AT84)*(AE84 - AG84), 0)</f>
         <v>0</v>
       </c>
       <c r="AV84" s="290">
@@ -23915,7 +23759,7 @@
       </c>
       <c r="H86" s="299">
         <f t="shared" si="19"/>
-        <v>571638.27</v>
+        <v>0</v>
       </c>
       <c r="I86" s="340">
         <f t="shared" si="19"/>
@@ -24289,9 +24133,9 @@
       <c r="A10" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B10" s="397" t="str">
+      <c r="B10" s="397">
         <f>Summary!M28</f>
-        <v>Loading...</v>
+        <v>1361.34</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -24603,9 +24447,9 @@
       <c r="A29" s="53" t="s">
         <v>236</v>
       </c>
-      <c r="B29" s="405">
+      <c r="B29" s="405" t="str">
         <f>SWITCH(Summary!$K$28,"today",TODAY(),"last year","2023-12-31",Summary!$K$28)</f>
-        <v>45354</v>
+        <v>2023-12-31</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>

</xml_diff>

<commit_message>
Fix potential capital gain calculation for fractional share lot (#78)
Should have been subtracting the fraction before calculating the gain, but was instead subtracting the fractional share, eg. 0.123, from the dollar value of shares.

Fixes #70
</commit_message>
<xml_diff>
--- a/VMW_to_AVGO_ESPP_and_RSU.xlsx
+++ b/VMW_to_AVGO_ESPP_and_RSU.xlsx
@@ -622,7 +622,7 @@
     <t>Post merger sale of AVGO</t>
   </si>
   <si>
-    <t>today</t>
+    <t>last year</t>
   </si>
   <si>
     <t xml:space="preserve">  @ </t>
@@ -3862,9 +3862,9 @@
       <c r="L28" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="M28" s="58" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),"Loading...")</f>
-        <v>Loading...</v>
+      <c r="M28" s="58">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),1361.34)</f>
+        <v>1361.34</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -4804,11 +4804,11 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="K42:O42"/>
     <mergeCell ref="C48:H48"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="F51:G51"/>
-    <mergeCell ref="K42:O42"/>
   </mergeCells>
   <conditionalFormatting sqref="B29">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
@@ -5610,7 +5610,7 @@
         <v>n/a</v>
       </c>
       <c r="AX7" s="247">
-        <f>iferror((Reference!$B$10-AW7)*(AH7) - AJ7, 0)</f>
+        <f>iferror((Reference!$B$10-AW7)*(AH7 - AJ7), 0)</f>
         <v>0</v>
       </c>
       <c r="AY7" s="248" t="b">
@@ -5806,7 +5806,7 @@
         <v>n/a</v>
       </c>
       <c r="AX8" s="247">
-        <f>iferror((Reference!$B$10-AW8)*(AH8) - AJ8, 0)</f>
+        <f>iferror((Reference!$B$10-AW8)*(AH8 - AJ8), 0)</f>
         <v>0</v>
       </c>
       <c r="AY8" s="248" t="b">
@@ -6002,7 +6002,7 @@
         <v>n/a</v>
       </c>
       <c r="AX9" s="247">
-        <f>iferror((Reference!$B$10-AW9)*(AH9) - AJ9, 0)</f>
+        <f>iferror((Reference!$B$10-AW9)*(AH9 - AJ9), 0)</f>
         <v>0</v>
       </c>
       <c r="AY9" s="248" t="b">
@@ -6198,7 +6198,7 @@
         <v>n/a</v>
       </c>
       <c r="AX10" s="247">
-        <f>iferror((Reference!$B$10-AW10)*(AH10) - AJ10, 0)</f>
+        <f>iferror((Reference!$B$10-AW10)*(AH10 - AJ10), 0)</f>
         <v>0</v>
       </c>
       <c r="AY10" s="248" t="b">
@@ -6393,7 +6393,7 @@
         <v>n/a</v>
       </c>
       <c r="AX11" s="247">
-        <f>iferror((Reference!$B$10-AW11)*(AH11) - AJ11, 0)</f>
+        <f>iferror((Reference!$B$10-AW11)*(AH11 - AJ11), 0)</f>
         <v>0</v>
       </c>
       <c r="AY11" s="248" t="b">
@@ -6589,7 +6589,7 @@
         <v>n/a</v>
       </c>
       <c r="AX12" s="247">
-        <f>iferror((Reference!$B$10-AW12)*(AH12) - AJ12, 0)</f>
+        <f>iferror((Reference!$B$10-AW12)*(AH12 - AJ12), 0)</f>
         <v>0</v>
       </c>
       <c r="AY12" s="248" t="b">
@@ -6785,7 +6785,7 @@
         <v>n/a</v>
       </c>
       <c r="AX13" s="247">
-        <f>iferror((Reference!$B$10-AW13)*(AH13) - AJ13, 0)</f>
+        <f>iferror((Reference!$B$10-AW13)*(AH13 - AJ13), 0)</f>
         <v>0</v>
       </c>
       <c r="AY13" s="248" t="b">
@@ -6981,7 +6981,7 @@
         <v>n/a</v>
       </c>
       <c r="AX14" s="247">
-        <f>iferror((Reference!$B$10-AW14)*(AH14) - AJ14, 0)</f>
+        <f>iferror((Reference!$B$10-AW14)*(AH14 - AJ14), 0)</f>
         <v>0</v>
       </c>
       <c r="AY14" s="248" t="b">
@@ -7176,7 +7176,7 @@
         <v>n/a</v>
       </c>
       <c r="AX15" s="247">
-        <f>iferror((Reference!$B$10-AW15)*(AH15) - AJ15, 0)</f>
+        <f>iferror((Reference!$B$10-AW15)*(AH15 - AJ15), 0)</f>
         <v>0</v>
       </c>
       <c r="AY15" s="248" t="b">
@@ -7371,7 +7371,7 @@
         <v>n/a</v>
       </c>
       <c r="AX16" s="247">
-        <f>iferror((Reference!$B$10-AW16)*(AH16) - AJ16, 0)</f>
+        <f>iferror((Reference!$B$10-AW16)*(AH16 - AJ16), 0)</f>
         <v>0</v>
       </c>
       <c r="AY16" s="248" t="b">
@@ -7566,7 +7566,7 @@
         <v>n/a</v>
       </c>
       <c r="AX17" s="247">
-        <f>iferror((Reference!$B$10-AW17)*(AH17) - AJ17, 0)</f>
+        <f>iferror((Reference!$B$10-AW17)*(AH17 - AJ17), 0)</f>
         <v>0</v>
       </c>
       <c r="AY17" s="248" t="b">
@@ -7761,7 +7761,7 @@
         <v>n/a</v>
       </c>
       <c r="AX18" s="247">
-        <f>iferror((Reference!$B$10-AW18)*(AH18) - AJ18, 0)</f>
+        <f>iferror((Reference!$B$10-AW18)*(AH18 - AJ18), 0)</f>
         <v>0</v>
       </c>
       <c r="AY18" s="248" t="b">
@@ -7956,7 +7956,7 @@
         <v>n/a</v>
       </c>
       <c r="AX19" s="247">
-        <f>iferror((Reference!$B$10-AW19)*(AH19) - AJ19, 0)</f>
+        <f>iferror((Reference!$B$10-AW19)*(AH19 - AJ19), 0)</f>
         <v>0</v>
       </c>
       <c r="AY19" s="248" t="b">
@@ -8151,7 +8151,7 @@
         <v>n/a</v>
       </c>
       <c r="AX20" s="247">
-        <f>iferror((Reference!$B$10-AW20)*(AH20) - AJ20, 0)</f>
+        <f>iferror((Reference!$B$10-AW20)*(AH20 - AJ20), 0)</f>
         <v>0</v>
       </c>
       <c r="AY20" s="248" t="b">
@@ -8346,7 +8346,7 @@
         <v>n/a</v>
       </c>
       <c r="AX21" s="247">
-        <f>iferror((Reference!$B$10-AW21)*(AH21) - AJ21, 0)</f>
+        <f>iferror((Reference!$B$10-AW21)*(AH21 - AJ21), 0)</f>
         <v>0</v>
       </c>
       <c r="AY21" s="248" t="b">
@@ -8541,7 +8541,7 @@
         <v>n/a</v>
       </c>
       <c r="AX22" s="247">
-        <f>iferror((Reference!$B$10-AW22)*(AH22) - AJ22, 0)</f>
+        <f>iferror((Reference!$B$10-AW22)*(AH22 - AJ22), 0)</f>
         <v>0</v>
       </c>
       <c r="AY22" s="248" t="b">
@@ -8736,7 +8736,7 @@
         <v>n/a</v>
       </c>
       <c r="AX23" s="247">
-        <f>iferror((Reference!$B$10-AW23)*(AH23) - AJ23, 0)</f>
+        <f>iferror((Reference!$B$10-AW23)*(AH23 - AJ23), 0)</f>
         <v>0</v>
       </c>
       <c r="AY23" s="248" t="b">
@@ -8931,7 +8931,7 @@
         <v>n/a</v>
       </c>
       <c r="AX24" s="247">
-        <f>iferror((Reference!$B$10-AW24)*(AH24) - AJ24, 0)</f>
+        <f>iferror((Reference!$B$10-AW24)*(AH24 - AJ24), 0)</f>
         <v>0</v>
       </c>
       <c r="AY24" s="248" t="b">
@@ -9126,7 +9126,7 @@
         <v>n/a</v>
       </c>
       <c r="AX25" s="247">
-        <f>iferror((Reference!$B$10-AW25)*(AH25) - AJ25, 0)</f>
+        <f>iferror((Reference!$B$10-AW25)*(AH25 - AJ25), 0)</f>
         <v>0</v>
       </c>
       <c r="AY25" s="248" t="b">
@@ -9321,12 +9321,12 @@
         <v>n/a</v>
       </c>
       <c r="AX26" s="290">
-        <f>iferror((Reference!$B$10-AW26)*(AH26) - AJ26, 0)</f>
+        <f>iferror((Reference!$B$10-AW26)*(AH26 - AJ26), 0)</f>
         <v>0</v>
       </c>
       <c r="AY26" s="291" t="b">
         <f>AND(DATEDIF(B26,Reference!$B$29,"Y")&gt;=1, DATEDIF(A26, Reference!$B$29, "Y")&gt;=2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ26" s="290">
         <f t="shared" si="20"/>
@@ -9546,18 +9546,18 @@
     <mergeCell ref="X2:AI2"/>
     <mergeCell ref="AK2:AV2"/>
     <mergeCell ref="AW2:BB2"/>
+    <mergeCell ref="AE3:AH3"/>
     <mergeCell ref="AK3:AL3"/>
     <mergeCell ref="AM3:AN3"/>
     <mergeCell ref="AO3:AV3"/>
     <mergeCell ref="AW3:BB3"/>
-    <mergeCell ref="AE3:AH3"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="O3:T3"/>
     <mergeCell ref="U3:W3"/>
+    <mergeCell ref="X3:AA3"/>
     <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="X3:AA3"/>
   </mergeCells>
   <conditionalFormatting sqref="M7:M26">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="notEqual">
@@ -9962,7 +9962,7 @@
       </c>
       <c r="H5" s="299">
         <f t="shared" si="1"/>
-        <v>571638.27</v>
+        <v>0</v>
       </c>
       <c r="I5" s="340">
         <f t="shared" si="1"/>
@@ -10141,9 +10141,7 @@
       <c r="E7" s="353">
         <v>82.1</v>
       </c>
-      <c r="F7" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F7" s="354"/>
       <c r="G7" s="225">
         <f t="shared" ref="G7:G84" si="7">D7*E7</f>
         <v>0</v>
@@ -10292,7 +10290,7 @@
         <v>n/a</v>
       </c>
       <c r="AU7" s="247">
-        <f>iferror((Reference!$B$10-AT7)*AE7 - AG7, 0)</f>
+        <f>iferror((Reference!$B$10-AT7)*(AE7 - AG7), 0)</f>
         <v>0</v>
       </c>
       <c r="AV7" s="247">
@@ -10316,9 +10314,7 @@
       <c r="E8" s="353">
         <v>90.14</v>
       </c>
-      <c r="F8" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F8" s="354"/>
       <c r="G8" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -10467,7 +10463,7 @@
         <v>n/a</v>
       </c>
       <c r="AU8" s="247">
-        <f>iferror((Reference!$B$10-AT8)*AE8 - AG8, 0)</f>
+        <f>iferror((Reference!$B$10-AT8)*(AE8 - AG8), 0)</f>
         <v>0</v>
       </c>
       <c r="AV8" s="247">
@@ -10493,16 +10489,14 @@
       <c r="E9" s="353">
         <v>98.33</v>
       </c>
-      <c r="F9" s="354">
-        <v>25.0</v>
-      </c>
+      <c r="F9" s="354"/>
       <c r="G9" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H9" s="236">
         <f t="shared" si="8"/>
-        <v>2458.25</v>
+        <v>0</v>
       </c>
       <c r="I9" s="355"/>
       <c r="J9" s="366" t="b">
@@ -10644,7 +10638,7 @@
         <v>n/a</v>
       </c>
       <c r="AU9" s="247">
-        <f>iferror((Reference!$B$10-AT9)*AE9 - AG9, 0)</f>
+        <f>iferror((Reference!$B$10-AT9)*(AE9 - AG9), 0)</f>
         <v>0</v>
       </c>
       <c r="AV9" s="247">
@@ -10670,16 +10664,14 @@
       <c r="E10" s="353">
         <v>77.1</v>
       </c>
-      <c r="F10" s="354">
-        <v>25.0</v>
-      </c>
+      <c r="F10" s="354"/>
       <c r="G10" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H10" s="236">
         <f t="shared" si="8"/>
-        <v>1927.5</v>
+        <v>0</v>
       </c>
       <c r="I10" s="367"/>
       <c r="J10" s="259" t="b">
@@ -10821,7 +10813,7 @@
         <v>n/a</v>
       </c>
       <c r="AU10" s="247">
-        <f>iferror((Reference!$B$10-AT10)*AE10 - AG10, 0)</f>
+        <f>iferror((Reference!$B$10-AT10)*(AE10 - AG10), 0)</f>
         <v>0</v>
       </c>
       <c r="AV10" s="247">
@@ -10847,16 +10839,14 @@
       <c r="E11" s="353">
         <v>87.47</v>
       </c>
-      <c r="F11" s="354">
-        <v>47.0</v>
-      </c>
+      <c r="F11" s="354"/>
       <c r="G11" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H11" s="236">
         <f t="shared" si="8"/>
-        <v>4111.09</v>
+        <v>0</v>
       </c>
       <c r="I11" s="355"/>
       <c r="J11" s="259" t="b">
@@ -10998,7 +10988,7 @@
         <v>n/a</v>
       </c>
       <c r="AU11" s="247">
-        <f>iferror((Reference!$B$10-AT11)*AE11 - AG11, 0)</f>
+        <f>iferror((Reference!$B$10-AT11)*(AE11 - AG11), 0)</f>
         <v>0</v>
       </c>
       <c r="AV11" s="247">
@@ -11024,16 +11014,14 @@
       <c r="E12" s="353">
         <v>89.13</v>
       </c>
-      <c r="F12" s="354">
-        <v>25.0</v>
-      </c>
+      <c r="F12" s="354"/>
       <c r="G12" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H12" s="236">
         <f t="shared" si="8"/>
-        <v>2228.25</v>
+        <v>0</v>
       </c>
       <c r="I12" s="355"/>
       <c r="J12" s="259" t="b">
@@ -11175,7 +11163,7 @@
         <v>n/a</v>
       </c>
       <c r="AU12" s="247">
-        <f>iferror((Reference!$B$10-AT12)*AE12 - AG12, 0)</f>
+        <f>iferror((Reference!$B$10-AT12)*(AE12 - AG12), 0)</f>
         <v>0</v>
       </c>
       <c r="AV12" s="247">
@@ -11201,16 +11189,14 @@
       <c r="E13" s="353">
         <v>60.15</v>
       </c>
-      <c r="F13" s="354">
-        <v>20.0</v>
-      </c>
+      <c r="F13" s="354"/>
       <c r="G13" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H13" s="236">
         <f t="shared" si="8"/>
-        <v>1203</v>
+        <v>0</v>
       </c>
       <c r="I13" s="355"/>
       <c r="J13" s="259" t="b">
@@ -11352,7 +11338,7 @@
         <v>n/a</v>
       </c>
       <c r="AU13" s="247">
-        <f>iferror((Reference!$B$10-AT13)*AE13 - AG13, 0)</f>
+        <f>iferror((Reference!$B$10-AT13)*(AE13 - AG13), 0)</f>
         <v>0</v>
       </c>
       <c r="AV13" s="247">
@@ -11378,16 +11364,14 @@
       <c r="E14" s="353">
         <v>45.49</v>
       </c>
-      <c r="F14" s="354">
-        <v>25.0</v>
-      </c>
+      <c r="F14" s="354"/>
       <c r="G14" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H14" s="236">
         <f t="shared" si="8"/>
-        <v>1137.25</v>
+        <v>0</v>
       </c>
       <c r="I14" s="355"/>
       <c r="J14" s="259" t="b">
@@ -11529,7 +11513,7 @@
         <v>n/a</v>
       </c>
       <c r="AU14" s="247">
-        <f>iferror((Reference!$B$10-AT14)*AE14 - AG14, 0)</f>
+        <f>iferror((Reference!$B$10-AT14)*(AE14 - AG14), 0)</f>
         <v>0</v>
       </c>
       <c r="AV14" s="247">
@@ -11555,16 +11539,14 @@
       <c r="E15" s="353">
         <v>56.91</v>
       </c>
-      <c r="F15" s="354">
-        <v>24.0</v>
-      </c>
+      <c r="F15" s="354"/>
       <c r="G15" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H15" s="236">
         <f t="shared" si="8"/>
-        <v>1365.84</v>
+        <v>0</v>
       </c>
       <c r="I15" s="355"/>
       <c r="J15" s="259" t="b">
@@ -11706,7 +11688,7 @@
         <v>n/a</v>
       </c>
       <c r="AU15" s="247">
-        <f>iferror((Reference!$B$10-AT15)*AE15 - AG15, 0)</f>
+        <f>iferror((Reference!$B$10-AT15)*(AE15 - AG15), 0)</f>
         <v>0</v>
       </c>
       <c r="AV15" s="247">
@@ -11732,16 +11714,14 @@
       <c r="E16" s="353">
         <v>56.91</v>
       </c>
-      <c r="F16" s="354">
-        <v>46.0</v>
-      </c>
+      <c r="F16" s="354"/>
       <c r="G16" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H16" s="236">
         <f t="shared" si="8"/>
-        <v>2617.86</v>
+        <v>0</v>
       </c>
       <c r="I16" s="355"/>
       <c r="J16" s="259" t="b">
@@ -11883,7 +11863,7 @@
         <v>n/a</v>
       </c>
       <c r="AU16" s="247">
-        <f>iferror((Reference!$B$10-AT16)*AE16 - AG16, 0)</f>
+        <f>iferror((Reference!$B$10-AT16)*(AE16 - AG16), 0)</f>
         <v>0</v>
       </c>
       <c r="AV16" s="247">
@@ -11909,16 +11889,14 @@
       <c r="E17" s="353">
         <v>77.97</v>
       </c>
-      <c r="F17" s="354">
-        <v>21.0</v>
-      </c>
+      <c r="F17" s="354"/>
       <c r="G17" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H17" s="236">
         <f t="shared" si="8"/>
-        <v>1637.37</v>
+        <v>0</v>
       </c>
       <c r="I17" s="355"/>
       <c r="J17" s="259" t="b">
@@ -12060,7 +12038,7 @@
         <v>n/a</v>
       </c>
       <c r="AU17" s="247">
-        <f>iferror((Reference!$B$10-AT17)*AE17 - AG17, 0)</f>
+        <f>iferror((Reference!$B$10-AT17)*(AE17 - AG17), 0)</f>
         <v>0</v>
       </c>
       <c r="AV17" s="247">
@@ -12086,16 +12064,14 @@
       <c r="E18" s="353">
         <v>77.97</v>
       </c>
-      <c r="F18" s="354">
-        <v>20.0</v>
-      </c>
+      <c r="F18" s="354"/>
       <c r="G18" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H18" s="236">
         <f t="shared" si="8"/>
-        <v>1559.4</v>
+        <v>0</v>
       </c>
       <c r="I18" s="355"/>
       <c r="J18" s="259" t="b">
@@ -12237,7 +12213,7 @@
         <v>n/a</v>
       </c>
       <c r="AU18" s="247">
-        <f>iferror((Reference!$B$10-AT18)*AE18 - AG18, 0)</f>
+        <f>iferror((Reference!$B$10-AT18)*(AE18 - AG18), 0)</f>
         <v>0</v>
       </c>
       <c r="AV18" s="247">
@@ -12263,16 +12239,14 @@
       <c r="E19" s="353">
         <v>78.04</v>
       </c>
-      <c r="F19" s="354">
-        <v>571.0</v>
-      </c>
+      <c r="F19" s="354"/>
       <c r="G19" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H19" s="236">
         <f t="shared" si="8"/>
-        <v>44560.84</v>
+        <v>0</v>
       </c>
       <c r="I19" s="355"/>
       <c r="J19" s="259" t="b">
@@ -12414,7 +12388,7 @@
         <v>n/a</v>
       </c>
       <c r="AU19" s="247">
-        <f>iferror((Reference!$B$10-AT19)*AE19 - AG19, 0)</f>
+        <f>iferror((Reference!$B$10-AT19)*(AE19 - AG19), 0)</f>
         <v>0</v>
       </c>
       <c r="AV19" s="247">
@@ -12440,16 +12414,14 @@
       <c r="E20" s="353">
         <v>94.58</v>
       </c>
-      <c r="F20" s="354">
-        <v>24.0</v>
-      </c>
+      <c r="F20" s="354"/>
       <c r="G20" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H20" s="236">
         <f t="shared" si="8"/>
-        <v>2269.92</v>
+        <v>0</v>
       </c>
       <c r="I20" s="355"/>
       <c r="J20" s="259" t="b">
@@ -12591,7 +12563,7 @@
         <v>n/a</v>
       </c>
       <c r="AU20" s="247">
-        <f>iferror((Reference!$B$10-AT20)*AE20 - AG20, 0)</f>
+        <f>iferror((Reference!$B$10-AT20)*(AE20 - AG20), 0)</f>
         <v>0</v>
       </c>
       <c r="AV20" s="247">
@@ -12617,16 +12589,14 @@
       <c r="E21" s="353">
         <v>94.58</v>
       </c>
-      <c r="F21" s="354">
-        <v>23.0</v>
-      </c>
+      <c r="F21" s="354"/>
       <c r="G21" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H21" s="236">
         <f t="shared" si="8"/>
-        <v>2175.34</v>
+        <v>0</v>
       </c>
       <c r="I21" s="355"/>
       <c r="J21" s="259" t="b">
@@ -12768,7 +12738,7 @@
         <v>n/a</v>
       </c>
       <c r="AU21" s="247">
-        <f>iferror((Reference!$B$10-AT21)*AE21 - AG21, 0)</f>
+        <f>iferror((Reference!$B$10-AT21)*(AE21 - AG21), 0)</f>
         <v>0</v>
       </c>
       <c r="AV21" s="247">
@@ -12794,16 +12764,14 @@
       <c r="E22" s="353">
         <v>94.58</v>
       </c>
-      <c r="F22" s="354">
-        <v>118.0</v>
-      </c>
+      <c r="F22" s="354"/>
       <c r="G22" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H22" s="236">
         <f t="shared" si="8"/>
-        <v>11160.44</v>
+        <v>0</v>
       </c>
       <c r="I22" s="367"/>
       <c r="J22" s="259" t="b">
@@ -12945,7 +12913,7 @@
         <v>n/a</v>
       </c>
       <c r="AU22" s="247">
-        <f>iferror((Reference!$B$10-AT22)*AE22 - AG22, 0)</f>
+        <f>iferror((Reference!$B$10-AT22)*(AE22 - AG22), 0)</f>
         <v>0</v>
       </c>
       <c r="AV22" s="247">
@@ -12971,16 +12939,14 @@
       <c r="E23" s="353">
         <v>97.4</v>
       </c>
-      <c r="F23" s="354">
-        <v>286.0</v>
-      </c>
+      <c r="F23" s="354"/>
       <c r="G23" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H23" s="236">
         <f t="shared" si="8"/>
-        <v>27856.4</v>
+        <v>0</v>
       </c>
       <c r="I23" s="355"/>
       <c r="J23" s="259" t="b">
@@ -13122,7 +13088,7 @@
         <v>n/a</v>
       </c>
       <c r="AU23" s="247">
-        <f>iferror((Reference!$B$10-AT23)*AE23 - AG23, 0)</f>
+        <f>iferror((Reference!$B$10-AT23)*(AE23 - AG23), 0)</f>
         <v>0</v>
       </c>
       <c r="AV23" s="247">
@@ -13148,16 +13114,14 @@
       <c r="E24" s="353">
         <v>119.12</v>
       </c>
-      <c r="F24" s="354">
-        <v>20.0</v>
-      </c>
+      <c r="F24" s="354"/>
       <c r="G24" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H24" s="236">
         <f t="shared" si="8"/>
-        <v>2382.4</v>
+        <v>0</v>
       </c>
       <c r="I24" s="355"/>
       <c r="J24" s="259" t="b">
@@ -13299,7 +13263,7 @@
         <v>n/a</v>
       </c>
       <c r="AU24" s="247">
-        <f>iferror((Reference!$B$10-AT24)*AE24 - AG24, 0)</f>
+        <f>iferror((Reference!$B$10-AT24)*(AE24 - AG24), 0)</f>
         <v>0</v>
       </c>
       <c r="AV24" s="247">
@@ -13325,16 +13289,14 @@
       <c r="E25" s="353">
         <v>119.12</v>
       </c>
-      <c r="F25" s="354">
-        <v>20.0</v>
-      </c>
+      <c r="F25" s="354"/>
       <c r="G25" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H25" s="236">
         <f t="shared" si="8"/>
-        <v>2382.4</v>
+        <v>0</v>
       </c>
       <c r="I25" s="367"/>
       <c r="J25" s="259" t="b">
@@ -13476,7 +13438,7 @@
         <v>n/a</v>
       </c>
       <c r="AU25" s="247">
-        <f>iferror((Reference!$B$10-AT25)*AE25 - AG25, 0)</f>
+        <f>iferror((Reference!$B$10-AT25)*(AE25 - AG25), 0)</f>
         <v>0</v>
       </c>
       <c r="AV25" s="247">
@@ -13502,16 +13464,14 @@
       <c r="E26" s="353">
         <v>119.12</v>
       </c>
-      <c r="F26" s="354">
-        <v>58.0</v>
-      </c>
+      <c r="F26" s="354"/>
       <c r="G26" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H26" s="236">
         <f t="shared" si="8"/>
-        <v>6908.96</v>
+        <v>0</v>
       </c>
       <c r="I26" s="355"/>
       <c r="J26" s="259" t="b">
@@ -13653,7 +13613,7 @@
         <v>n/a</v>
       </c>
       <c r="AU26" s="247">
-        <f>iferror((Reference!$B$10-AT26)*AE26 - AG26, 0)</f>
+        <f>iferror((Reference!$B$10-AT26)*(AE26 - AG26), 0)</f>
         <v>0</v>
       </c>
       <c r="AV26" s="247">
@@ -13679,16 +13639,14 @@
       <c r="E27" s="353">
         <v>124.44</v>
       </c>
-      <c r="F27" s="354">
-        <v>290.0</v>
-      </c>
+      <c r="F27" s="354"/>
       <c r="G27" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H27" s="236">
         <f t="shared" si="8"/>
-        <v>36087.6</v>
+        <v>0</v>
       </c>
       <c r="I27" s="355"/>
       <c r="J27" s="259" t="b">
@@ -13830,7 +13788,7 @@
         <v>n/a</v>
       </c>
       <c r="AU27" s="247">
-        <f>iferror((Reference!$B$10-AT27)*AE27 - AG27, 0)</f>
+        <f>iferror((Reference!$B$10-AT27)*(AE27 - AG27), 0)</f>
         <v>0</v>
       </c>
       <c r="AV27" s="247">
@@ -13856,16 +13814,14 @@
       <c r="E28" s="353">
         <v>133.22</v>
       </c>
-      <c r="F28" s="354">
-        <v>23.0</v>
-      </c>
+      <c r="F28" s="354"/>
       <c r="G28" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H28" s="236">
         <f t="shared" si="8"/>
-        <v>3064.06</v>
+        <v>0</v>
       </c>
       <c r="I28" s="367"/>
       <c r="J28" s="259" t="b">
@@ -14007,7 +13963,7 @@
         <v>n/a</v>
       </c>
       <c r="AU28" s="247">
-        <f>iferror((Reference!$B$10-AT28)*AE28 - AG28, 0)</f>
+        <f>iferror((Reference!$B$10-AT28)*(AE28 - AG28), 0)</f>
         <v>0</v>
       </c>
       <c r="AV28" s="247">
@@ -14033,16 +13989,14 @@
       <c r="E29" s="353">
         <v>133.22</v>
       </c>
-      <c r="F29" s="354">
-        <v>22.0</v>
-      </c>
+      <c r="F29" s="354"/>
       <c r="G29" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H29" s="236">
         <f t="shared" si="8"/>
-        <v>2930.84</v>
+        <v>0</v>
       </c>
       <c r="I29" s="355"/>
       <c r="J29" s="259" t="b">
@@ -14184,7 +14138,7 @@
         <v>n/a</v>
       </c>
       <c r="AU29" s="247">
-        <f>iferror((Reference!$B$10-AT29)*AE29 - AG29, 0)</f>
+        <f>iferror((Reference!$B$10-AT29)*(AE29 - AG29), 0)</f>
         <v>0</v>
       </c>
       <c r="AV29" s="247">
@@ -14210,16 +14164,14 @@
       <c r="E30" s="353">
         <v>133.22</v>
       </c>
-      <c r="F30" s="354">
-        <v>63.0</v>
-      </c>
+      <c r="F30" s="354"/>
       <c r="G30" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H30" s="236">
         <f t="shared" si="8"/>
-        <v>8392.86</v>
+        <v>0</v>
       </c>
       <c r="I30" s="367"/>
       <c r="J30" s="259" t="b">
@@ -14361,7 +14313,7 @@
         <v>n/a</v>
       </c>
       <c r="AU30" s="247">
-        <f>iferror((Reference!$B$10-AT30)*AE30 - AG30, 0)</f>
+        <f>iferror((Reference!$B$10-AT30)*(AE30 - AG30), 0)</f>
         <v>0</v>
       </c>
       <c r="AV30" s="247">
@@ -14387,16 +14339,14 @@
       <c r="E31" s="353">
         <v>145.93</v>
       </c>
-      <c r="F31" s="354">
-        <v>264.0</v>
-      </c>
+      <c r="F31" s="354"/>
       <c r="G31" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H31" s="236">
         <f t="shared" si="8"/>
-        <v>38525.52</v>
+        <v>0</v>
       </c>
       <c r="I31" s="355"/>
       <c r="J31" s="259" t="b">
@@ -14538,7 +14488,7 @@
         <v>n/a</v>
       </c>
       <c r="AU31" s="247">
-        <f>iferror((Reference!$B$10-AT31)*AE31 - AG31, 0)</f>
+        <f>iferror((Reference!$B$10-AT31)*(AE31 - AG31), 0)</f>
         <v>0</v>
       </c>
       <c r="AV31" s="247">
@@ -14564,16 +14514,14 @@
       <c r="E32" s="353">
         <v>146.97</v>
       </c>
-      <c r="F32" s="354">
-        <v>85.0</v>
-      </c>
+      <c r="F32" s="354"/>
       <c r="G32" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H32" s="236">
         <f t="shared" si="8"/>
-        <v>12492.45</v>
+        <v>0</v>
       </c>
       <c r="I32" s="355"/>
       <c r="J32" s="259" t="b">
@@ -14715,7 +14663,7 @@
         <v>n/a</v>
       </c>
       <c r="AU32" s="247">
-        <f>iferror((Reference!$B$10-AT32)*AE32 - AG32, 0)</f>
+        <f>iferror((Reference!$B$10-AT32)*(AE32 - AG32), 0)</f>
         <v>0</v>
       </c>
       <c r="AV32" s="247">
@@ -14741,16 +14689,14 @@
       <c r="E33" s="353">
         <v>144.64</v>
       </c>
-      <c r="F33" s="354">
-        <v>19.0</v>
-      </c>
+      <c r="F33" s="354"/>
       <c r="G33" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H33" s="236">
         <f t="shared" si="8"/>
-        <v>2748.16</v>
+        <v>0</v>
       </c>
       <c r="I33" s="355"/>
       <c r="J33" s="259" t="b">
@@ -14892,7 +14838,7 @@
         <v>n/a</v>
       </c>
       <c r="AU33" s="247">
-        <f>iferror((Reference!$B$10-AT33)*AE33 - AG33, 0)</f>
+        <f>iferror((Reference!$B$10-AT33)*(AE33 - AG33), 0)</f>
         <v>0</v>
       </c>
       <c r="AV33" s="247">
@@ -14918,16 +14864,14 @@
       <c r="E34" s="353">
         <v>144.64</v>
       </c>
-      <c r="F34" s="354">
-        <v>54.0</v>
-      </c>
+      <c r="F34" s="354"/>
       <c r="G34" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H34" s="236">
         <f t="shared" si="8"/>
-        <v>7810.56</v>
+        <v>0</v>
       </c>
       <c r="I34" s="355"/>
       <c r="J34" s="259" t="b">
@@ -15069,7 +15013,7 @@
         <v>n/a</v>
       </c>
       <c r="AU34" s="247">
-        <f>iferror((Reference!$B$10-AT34)*AE34 - AG34, 0)</f>
+        <f>iferror((Reference!$B$10-AT34)*(AE34 - AG34), 0)</f>
         <v>0</v>
       </c>
       <c r="AV34" s="247">
@@ -15095,16 +15039,14 @@
       <c r="E35" s="353">
         <v>167.34</v>
       </c>
-      <c r="F35" s="354">
-        <v>267.0</v>
-      </c>
+      <c r="F35" s="354"/>
       <c r="G35" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H35" s="236">
         <f t="shared" si="8"/>
-        <v>44679.78</v>
+        <v>0</v>
       </c>
       <c r="I35" s="355"/>
       <c r="J35" s="259" t="b">
@@ -15246,7 +15188,7 @@
         <v>n/a</v>
       </c>
       <c r="AU35" s="247">
-        <f>iferror((Reference!$B$10-AT35)*AE35 - AG35, 0)</f>
+        <f>iferror((Reference!$B$10-AT35)*(AE35 - AG35), 0)</f>
         <v>0</v>
       </c>
       <c r="AV35" s="247">
@@ -15272,16 +15214,14 @@
       <c r="E36" s="353">
         <v>148.88</v>
       </c>
-      <c r="F36" s="354">
-        <v>61.0</v>
-      </c>
+      <c r="F36" s="354"/>
       <c r="G36" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H36" s="236">
         <f t="shared" si="8"/>
-        <v>9081.68</v>
+        <v>0</v>
       </c>
       <c r="I36" s="355"/>
       <c r="J36" s="259" t="b">
@@ -15423,7 +15363,7 @@
         <v>n/a</v>
       </c>
       <c r="AU36" s="247">
-        <f>iferror((Reference!$B$10-AT36)*AE36 - AG36, 0)</f>
+        <f>iferror((Reference!$B$10-AT36)*(AE36 - AG36), 0)</f>
         <v>0</v>
       </c>
       <c r="AV36" s="247">
@@ -15449,16 +15389,14 @@
       <c r="E37" s="353">
         <v>202.46</v>
       </c>
-      <c r="F37" s="354">
-        <v>23.0</v>
-      </c>
+      <c r="F37" s="354"/>
       <c r="G37" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H37" s="236">
         <f t="shared" si="8"/>
-        <v>4656.58</v>
+        <v>0</v>
       </c>
       <c r="I37" s="355"/>
       <c r="J37" s="259" t="b">
@@ -15600,7 +15538,7 @@
         <v>n/a</v>
       </c>
       <c r="AU37" s="247">
-        <f>iferror((Reference!$B$10-AT37)*AE37 - AG37, 0)</f>
+        <f>iferror((Reference!$B$10-AT37)*(AE37 - AG37), 0)</f>
         <v>0</v>
       </c>
       <c r="AV37" s="247">
@@ -15626,16 +15564,14 @@
       <c r="E38" s="353">
         <v>202.46</v>
       </c>
-      <c r="F38" s="354">
-        <v>63.0</v>
-      </c>
+      <c r="F38" s="354"/>
       <c r="G38" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H38" s="236">
         <f t="shared" si="8"/>
-        <v>12754.98</v>
+        <v>0</v>
       </c>
       <c r="I38" s="355"/>
       <c r="J38" s="259" t="b">
@@ -15777,7 +15713,7 @@
         <v>n/a</v>
       </c>
       <c r="AU38" s="247">
-        <f>iferror((Reference!$B$10-AT38)*AE38 - AG38, 0)</f>
+        <f>iferror((Reference!$B$10-AT38)*(AE38 - AG38), 0)</f>
         <v>0</v>
       </c>
       <c r="AV38" s="247">
@@ -15803,16 +15739,14 @@
       <c r="E39" s="353">
         <v>176.98</v>
       </c>
-      <c r="F39" s="354">
-        <v>71.0</v>
-      </c>
+      <c r="F39" s="354"/>
       <c r="G39" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H39" s="236">
         <f t="shared" si="8"/>
-        <v>12565.58</v>
+        <v>0</v>
       </c>
       <c r="I39" s="367"/>
       <c r="J39" s="259" t="b">
@@ -15954,7 +15888,7 @@
         <v>n/a</v>
       </c>
       <c r="AU39" s="247">
-        <f>iferror((Reference!$B$10-AT39)*AE39 - AG39, 0)</f>
+        <f>iferror((Reference!$B$10-AT39)*(AE39 - AG39), 0)</f>
         <v>0</v>
       </c>
       <c r="AV39" s="247">
@@ -15980,16 +15914,14 @@
       <c r="E40" s="353">
         <v>168.77</v>
       </c>
-      <c r="F40" s="354">
-        <v>51.0</v>
-      </c>
+      <c r="F40" s="354"/>
       <c r="G40" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H40" s="236">
         <f t="shared" si="8"/>
-        <v>8607.27</v>
+        <v>0</v>
       </c>
       <c r="I40" s="355"/>
       <c r="J40" s="259" t="b">
@@ -16131,7 +16063,7 @@
         <v>n/a</v>
       </c>
       <c r="AU40" s="247">
-        <f>iferror((Reference!$B$10-AT40)*AE40 - AG40, 0)</f>
+        <f>iferror((Reference!$B$10-AT40)*(AE40 - AG40), 0)</f>
         <v>0</v>
       </c>
       <c r="AV40" s="247">
@@ -16157,16 +16089,14 @@
       <c r="E41" s="353">
         <v>163.06</v>
       </c>
-      <c r="F41" s="354">
-        <v>65.0</v>
-      </c>
+      <c r="F41" s="354"/>
       <c r="G41" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H41" s="236">
         <f t="shared" si="8"/>
-        <v>10598.9</v>
+        <v>0</v>
       </c>
       <c r="I41" s="367"/>
       <c r="J41" s="259" t="b">
@@ -16308,7 +16238,7 @@
         <v>n/a</v>
       </c>
       <c r="AU41" s="247">
-        <f>iferror((Reference!$B$10-AT41)*AE41 - AG41, 0)</f>
+        <f>iferror((Reference!$B$10-AT41)*(AE41 - AG41), 0)</f>
         <v>0</v>
       </c>
       <c r="AV41" s="247">
@@ -16334,16 +16264,14 @@
       <c r="E42" s="353">
         <v>155.62</v>
       </c>
-      <c r="F42" s="354">
-        <v>36.0</v>
-      </c>
+      <c r="F42" s="354"/>
       <c r="G42" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H42" s="236">
         <f t="shared" si="8"/>
-        <v>5602.32</v>
+        <v>0</v>
       </c>
       <c r="I42" s="367"/>
       <c r="J42" s="259" t="b">
@@ -16485,7 +16413,7 @@
         <v>n/a</v>
       </c>
       <c r="AU42" s="247">
-        <f>iferror((Reference!$B$10-AT42)*AE42 - AG42, 0)</f>
+        <f>iferror((Reference!$B$10-AT42)*(AE42 - AG42), 0)</f>
         <v>0</v>
       </c>
       <c r="AV42" s="247">
@@ -16511,16 +16439,14 @@
       <c r="E43" s="353">
         <v>151.79</v>
       </c>
-      <c r="F43" s="354">
-        <v>61.0</v>
-      </c>
+      <c r="F43" s="354"/>
       <c r="G43" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H43" s="236">
         <f t="shared" si="8"/>
-        <v>9259.19</v>
+        <v>0</v>
       </c>
       <c r="I43" s="355"/>
       <c r="J43" s="259" t="b">
@@ -16662,7 +16588,7 @@
         <v>n/a</v>
       </c>
       <c r="AU43" s="247">
-        <f>iferror((Reference!$B$10-AT43)*AE43 - AG43, 0)</f>
+        <f>iferror((Reference!$B$10-AT43)*(AE43 - AG43), 0)</f>
         <v>0</v>
       </c>
       <c r="AV43" s="247">
@@ -16684,9 +16610,7 @@
       <c r="E44" s="353">
         <v>148.06</v>
       </c>
-      <c r="F44" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F44" s="354"/>
       <c r="G44" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -16835,7 +16759,7 @@
         <v>n/a</v>
       </c>
       <c r="AU44" s="247">
-        <f>iferror((Reference!$B$10-AT44)*AE44 - AG44, 0)</f>
+        <f>iferror((Reference!$B$10-AT44)*(AE44 - AG44), 0)</f>
         <v>0</v>
       </c>
       <c r="AV44" s="247">
@@ -16857,9 +16781,7 @@
       <c r="E45" s="223">
         <v>120.52</v>
       </c>
-      <c r="F45" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F45" s="354"/>
       <c r="G45" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -17008,7 +16930,7 @@
         <v>n/a</v>
       </c>
       <c r="AU45" s="247">
-        <f>iferror((Reference!$B$10-AT45)*AE45 - AG45, 0)</f>
+        <f>iferror((Reference!$B$10-AT45)*(AE45 - AG45), 0)</f>
         <v>0</v>
       </c>
       <c r="AV45" s="247">
@@ -17034,16 +16956,14 @@
       <c r="E46" s="353">
         <v>125.34</v>
       </c>
-      <c r="F46" s="354">
-        <v>68.0</v>
-      </c>
+      <c r="F46" s="354"/>
       <c r="G46" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H46" s="236">
         <f t="shared" si="8"/>
-        <v>8523.12</v>
+        <v>0</v>
       </c>
       <c r="I46" s="355"/>
       <c r="J46" s="259" t="b">
@@ -17185,7 +17105,7 @@
         <v>n/a</v>
       </c>
       <c r="AU46" s="247">
-        <f>iferror((Reference!$B$10-AT46)*AE46 - AG46, 0)</f>
+        <f>iferror((Reference!$B$10-AT46)*(AE46 - AG46), 0)</f>
         <v>0</v>
       </c>
       <c r="AV46" s="247">
@@ -17211,16 +17131,14 @@
       <c r="E47" s="353">
         <v>154.14</v>
       </c>
-      <c r="F47" s="354">
-        <v>89.0</v>
-      </c>
+      <c r="F47" s="354"/>
       <c r="G47" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H47" s="236">
         <f t="shared" si="8"/>
-        <v>13718.46</v>
+        <v>0</v>
       </c>
       <c r="I47" s="367"/>
       <c r="J47" s="259" t="b">
@@ -17362,7 +17280,7 @@
         <v>n/a</v>
       </c>
       <c r="AU47" s="247">
-        <f>iferror((Reference!$B$10-AT47)*AE47 - AG47, 0)</f>
+        <f>iferror((Reference!$B$10-AT47)*(AE47 - AG47), 0)</f>
         <v>0</v>
       </c>
       <c r="AV47" s="247">
@@ -17388,16 +17306,14 @@
       <c r="E48" s="353">
         <v>154.14</v>
       </c>
-      <c r="F48" s="354">
-        <v>35.0</v>
-      </c>
+      <c r="F48" s="354"/>
       <c r="G48" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H48" s="236">
         <f t="shared" si="8"/>
-        <v>5394.9</v>
+        <v>0</v>
       </c>
       <c r="I48" s="355"/>
       <c r="J48" s="259" t="b">
@@ -17539,7 +17455,7 @@
         <v>n/a</v>
       </c>
       <c r="AU48" s="247">
-        <f>iferror((Reference!$B$10-AT48)*AE48 - AG48, 0)</f>
+        <f>iferror((Reference!$B$10-AT48)*(AE48 - AG48), 0)</f>
         <v>0</v>
       </c>
       <c r="AV48" s="247">
@@ -17565,16 +17481,14 @@
       <c r="E49" s="353">
         <v>153.1</v>
       </c>
-      <c r="F49" s="354">
-        <v>51.0</v>
-      </c>
+      <c r="F49" s="354"/>
       <c r="G49" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H49" s="236">
         <f t="shared" si="8"/>
-        <v>7808.1</v>
+        <v>0</v>
       </c>
       <c r="I49" s="355"/>
       <c r="J49" s="259" t="b">
@@ -17716,7 +17630,7 @@
         <v>n/a</v>
       </c>
       <c r="AU49" s="247">
-        <f>iferror((Reference!$B$10-AT49)*AE49 - AG49, 0)</f>
+        <f>iferror((Reference!$B$10-AT49)*(AE49 - AG49), 0)</f>
         <v>0</v>
       </c>
       <c r="AV49" s="247">
@@ -17738,9 +17652,7 @@
       <c r="E50" s="353">
         <v>141.28</v>
       </c>
-      <c r="F50" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F50" s="354"/>
       <c r="G50" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -17889,7 +17801,7 @@
         <v>n/a</v>
       </c>
       <c r="AU50" s="247">
-        <f>iferror((Reference!$B$10-AT50)*AE50 - AG50, 0)</f>
+        <f>iferror((Reference!$B$10-AT50)*(AE50 - AG50), 0)</f>
         <v>0</v>
       </c>
       <c r="AV50" s="247">
@@ -17915,16 +17827,14 @@
       <c r="E51" s="353">
         <v>140.75</v>
       </c>
-      <c r="F51" s="354">
-        <v>45.0</v>
-      </c>
+      <c r="F51" s="354"/>
       <c r="G51" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H51" s="236">
         <f t="shared" si="8"/>
-        <v>6333.75</v>
+        <v>0</v>
       </c>
       <c r="I51" s="367"/>
       <c r="J51" s="259" t="b">
@@ -18066,7 +17976,7 @@
         <v>n/a</v>
       </c>
       <c r="AU51" s="247">
-        <f>iferror((Reference!$B$10-AT51)*AE51 - AG51, 0)</f>
+        <f>iferror((Reference!$B$10-AT51)*(AE51 - AG51), 0)</f>
         <v>0</v>
       </c>
       <c r="AV51" s="247">
@@ -18092,16 +18002,14 @@
       <c r="E52" s="353">
         <v>140.75</v>
       </c>
-      <c r="F52" s="354">
-        <v>36.0</v>
-      </c>
+      <c r="F52" s="354"/>
       <c r="G52" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H52" s="236">
         <f t="shared" si="8"/>
-        <v>5067</v>
+        <v>0</v>
       </c>
       <c r="I52" s="355"/>
       <c r="J52" s="259" t="b">
@@ -18243,7 +18151,7 @@
         <v>n/a</v>
       </c>
       <c r="AU52" s="247">
-        <f>iferror((Reference!$B$10-AT52)*AE52 - AG52, 0)</f>
+        <f>iferror((Reference!$B$10-AT52)*(AE52 - AG52), 0)</f>
         <v>0</v>
       </c>
       <c r="AV52" s="247">
@@ -18269,16 +18177,14 @@
       <c r="E53" s="353">
         <v>140.26</v>
       </c>
-      <c r="F53" s="354">
-        <v>61.0</v>
-      </c>
+      <c r="F53" s="354"/>
       <c r="G53" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H53" s="236">
         <f t="shared" si="8"/>
-        <v>8555.86</v>
+        <v>0</v>
       </c>
       <c r="I53" s="367"/>
       <c r="J53" s="259" t="b">
@@ -18420,7 +18326,7 @@
         <v>n/a</v>
       </c>
       <c r="AU53" s="247">
-        <f>iferror((Reference!$B$10-AT53)*AE53 - AG53, 0)</f>
+        <f>iferror((Reference!$B$10-AT53)*(AE53 - AG53), 0)</f>
         <v>0</v>
       </c>
       <c r="AV53" s="247">
@@ -18442,9 +18348,7 @@
       <c r="E54" s="353">
         <v>140.41</v>
       </c>
-      <c r="F54" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F54" s="354"/>
       <c r="G54" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -18593,7 +18497,7 @@
         <v>n/a</v>
       </c>
       <c r="AU54" s="247">
-        <f>iferror((Reference!$B$10-AT54)*AE54 - AG54, 0)</f>
+        <f>iferror((Reference!$B$10-AT54)*(AE54 - AG54), 0)</f>
         <v>0</v>
       </c>
       <c r="AV54" s="247">
@@ -18619,16 +18523,14 @@
       <c r="E55" s="353">
         <v>160.83</v>
       </c>
-      <c r="F55" s="354">
-        <v>107.0</v>
-      </c>
+      <c r="F55" s="354"/>
       <c r="G55" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H55" s="236">
         <f t="shared" si="8"/>
-        <v>17208.81</v>
+        <v>0</v>
       </c>
       <c r="I55" s="355"/>
       <c r="J55" s="259" t="b">
@@ -18770,7 +18672,7 @@
         <v>n/a</v>
       </c>
       <c r="AU55" s="247">
-        <f>iferror((Reference!$B$10-AT55)*AE55 - AG55, 0)</f>
+        <f>iferror((Reference!$B$10-AT55)*(AE55 - AG55), 0)</f>
         <v>0</v>
       </c>
       <c r="AV55" s="247">
@@ -18796,16 +18698,14 @@
       <c r="E56" s="353">
         <v>161.26</v>
       </c>
-      <c r="F56" s="354">
-        <v>45.0</v>
-      </c>
+      <c r="F56" s="354"/>
       <c r="G56" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H56" s="236">
         <f t="shared" si="8"/>
-        <v>7256.7</v>
+        <v>0</v>
       </c>
       <c r="I56" s="355"/>
       <c r="J56" s="259" t="b">
@@ -18947,7 +18847,7 @@
         <v>n/a</v>
       </c>
       <c r="AU56" s="247">
-        <f>iferror((Reference!$B$10-AT56)*AE56 - AG56, 0)</f>
+        <f>iferror((Reference!$B$10-AT56)*(AE56 - AG56), 0)</f>
         <v>0</v>
       </c>
       <c r="AV56" s="247">
@@ -18973,16 +18873,14 @@
       <c r="E57" s="353">
         <v>161.26</v>
       </c>
-      <c r="F57" s="354">
-        <v>36.0</v>
-      </c>
+      <c r="F57" s="354"/>
       <c r="G57" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H57" s="236">
         <f t="shared" si="8"/>
-        <v>5805.36</v>
+        <v>0</v>
       </c>
       <c r="I57" s="355"/>
       <c r="J57" s="259" t="b">
@@ -19124,7 +19022,7 @@
         <v>n/a</v>
       </c>
       <c r="AU57" s="247">
-        <f>iferror((Reference!$B$10-AT57)*AE57 - AG57, 0)</f>
+        <f>iferror((Reference!$B$10-AT57)*(AE57 - AG57), 0)</f>
         <v>0</v>
       </c>
       <c r="AV57" s="247">
@@ -19150,16 +19048,14 @@
       <c r="E58" s="353">
         <v>156.13</v>
       </c>
-      <c r="F58" s="354">
-        <v>50.0</v>
-      </c>
+      <c r="F58" s="354"/>
       <c r="G58" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H58" s="236">
         <f t="shared" si="8"/>
-        <v>7806.5</v>
+        <v>0</v>
       </c>
       <c r="I58" s="355"/>
       <c r="J58" s="259" t="b">
@@ -19301,7 +19197,7 @@
         <v>n/a</v>
       </c>
       <c r="AU58" s="247">
-        <f>iferror((Reference!$B$10-AT58)*AE58 - AG58, 0)</f>
+        <f>iferror((Reference!$B$10-AT58)*(AE58 - AG58), 0)</f>
         <v>0</v>
       </c>
       <c r="AV58" s="247">
@@ -19323,9 +19219,7 @@
       <c r="E59" s="353">
         <v>146.86</v>
       </c>
-      <c r="F59" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F59" s="354"/>
       <c r="G59" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -19474,7 +19368,7 @@
         <v>n/a</v>
       </c>
       <c r="AU59" s="247">
-        <f>iferror((Reference!$B$10-AT59)*AE59 - AG59, 0)</f>
+        <f>iferror((Reference!$B$10-AT59)*(AE59 - AG59), 0)</f>
         <v>0</v>
       </c>
       <c r="AV59" s="247">
@@ -19500,16 +19394,14 @@
       <c r="E60" s="353">
         <v>124.18</v>
       </c>
-      <c r="F60" s="354">
-        <v>67.0</v>
-      </c>
+      <c r="F60" s="354"/>
       <c r="G60" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H60" s="236">
         <f t="shared" si="8"/>
-        <v>8320.06</v>
+        <v>0</v>
       </c>
       <c r="I60" s="355"/>
       <c r="J60" s="259" t="b">
@@ -19651,7 +19543,7 @@
         <v>n/a</v>
       </c>
       <c r="AU60" s="247">
-        <f>iferror((Reference!$B$10-AT60)*AE60 - AG60, 0)</f>
+        <f>iferror((Reference!$B$10-AT60)*(AE60 - AG60), 0)</f>
         <v>0</v>
       </c>
       <c r="AV60" s="247">
@@ -19677,16 +19569,14 @@
       <c r="E61" s="353">
         <v>114.0</v>
       </c>
-      <c r="F61" s="354">
-        <v>44.0</v>
-      </c>
+      <c r="F61" s="354"/>
       <c r="G61" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H61" s="236">
         <f t="shared" si="8"/>
-        <v>5016</v>
+        <v>0</v>
       </c>
       <c r="I61" s="355"/>
       <c r="J61" s="259" t="b">
@@ -19828,7 +19718,7 @@
         <v>n/a</v>
       </c>
       <c r="AU61" s="247">
-        <f>iferror((Reference!$B$10-AT61)*AE61 - AG61, 0)</f>
+        <f>iferror((Reference!$B$10-AT61)*(AE61 - AG61), 0)</f>
         <v>0</v>
       </c>
       <c r="AV61" s="247">
@@ -19854,16 +19744,14 @@
       <c r="E62" s="353">
         <v>114.0</v>
       </c>
-      <c r="F62" s="354">
-        <v>55.0</v>
-      </c>
+      <c r="F62" s="354"/>
       <c r="G62" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H62" s="236">
         <f t="shared" si="8"/>
-        <v>6270</v>
+        <v>0</v>
       </c>
       <c r="I62" s="355"/>
       <c r="J62" s="259" t="b">
@@ -20005,7 +19893,7 @@
         <v>n/a</v>
       </c>
       <c r="AU62" s="247">
-        <f>iferror((Reference!$B$10-AT62)*AE62 - AG62, 0)</f>
+        <f>iferror((Reference!$B$10-AT62)*(AE62 - AG62), 0)</f>
         <v>0</v>
       </c>
       <c r="AV62" s="247">
@@ -20027,9 +19915,7 @@
       <c r="E63" s="353">
         <v>115.88</v>
       </c>
-      <c r="F63" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F63" s="354"/>
       <c r="G63" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -20178,7 +20064,7 @@
         <v>n/a</v>
       </c>
       <c r="AU63" s="247">
-        <f>iferror((Reference!$B$10-AT63)*AE63 - AG63, 0)</f>
+        <f>iferror((Reference!$B$10-AT63)*(AE63 - AG63), 0)</f>
         <v>0</v>
       </c>
       <c r="AV63" s="247">
@@ -20204,16 +20090,14 @@
       <c r="E64" s="353">
         <v>128.47</v>
       </c>
-      <c r="F64" s="354">
-        <v>92.0</v>
-      </c>
+      <c r="F64" s="354"/>
       <c r="G64" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H64" s="236">
         <f t="shared" si="8"/>
-        <v>11819.24</v>
+        <v>0</v>
       </c>
       <c r="I64" s="355"/>
       <c r="J64" s="259" t="b">
@@ -20355,7 +20239,7 @@
         <v>n/a</v>
       </c>
       <c r="AU64" s="247">
-        <f>iferror((Reference!$B$10-AT64)*AE64 - AG64, 0)</f>
+        <f>iferror((Reference!$B$10-AT64)*(AE64 - AG64), 0)</f>
         <v>0</v>
       </c>
       <c r="AV64" s="247">
@@ -20377,9 +20261,7 @@
       <c r="E65" s="353">
         <v>115.91</v>
       </c>
-      <c r="F65" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F65" s="354"/>
       <c r="G65" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -20528,7 +20410,7 @@
         <v>n/a</v>
       </c>
       <c r="AU65" s="247">
-        <f>iferror((Reference!$B$10-AT65)*AE65 - AG65, 0)</f>
+        <f>iferror((Reference!$B$10-AT65)*(AE65 - AG65), 0)</f>
         <v>0</v>
       </c>
       <c r="AV65" s="247">
@@ -20554,16 +20436,14 @@
       <c r="E66" s="353">
         <v>108.04</v>
       </c>
-      <c r="F66" s="354">
-        <v>65.0</v>
-      </c>
+      <c r="F66" s="354"/>
       <c r="G66" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H66" s="236">
         <f t="shared" si="8"/>
-        <v>7022.6</v>
+        <v>0</v>
       </c>
       <c r="I66" s="355"/>
       <c r="J66" s="259" t="b">
@@ -20705,7 +20585,7 @@
         <v>n/a</v>
       </c>
       <c r="AU66" s="247">
-        <f>iferror((Reference!$B$10-AT66)*AE66 - AG66, 0)</f>
+        <f>iferror((Reference!$B$10-AT66)*(AE66 - AG66), 0)</f>
         <v>0</v>
       </c>
       <c r="AV66" s="247">
@@ -20731,16 +20611,14 @@
       <c r="E67" s="353">
         <v>108.04</v>
       </c>
-      <c r="F67" s="354">
-        <v>26.0</v>
-      </c>
+      <c r="F67" s="354"/>
       <c r="G67" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H67" s="236">
         <f t="shared" si="8"/>
-        <v>2809.04</v>
+        <v>0</v>
       </c>
       <c r="I67" s="355"/>
       <c r="J67" s="259" t="b">
@@ -20882,7 +20760,7 @@
         <v>n/a</v>
       </c>
       <c r="AU67" s="247">
-        <f>iferror((Reference!$B$10-AT67)*AE67 - AG67, 0)</f>
+        <f>iferror((Reference!$B$10-AT67)*(AE67 - AG67), 0)</f>
         <v>0</v>
       </c>
       <c r="AV67" s="247">
@@ -20908,16 +20786,14 @@
       <c r="E68" s="353">
         <v>129.41</v>
       </c>
-      <c r="F68" s="354">
-        <v>44.0</v>
-      </c>
+      <c r="F68" s="354"/>
       <c r="G68" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H68" s="236">
         <f t="shared" si="8"/>
-        <v>5694.04</v>
+        <v>0</v>
       </c>
       <c r="I68" s="355"/>
       <c r="J68" s="259" t="b">
@@ -21059,7 +20935,7 @@
         <v>n/a</v>
       </c>
       <c r="AU68" s="247">
-        <f>iferror((Reference!$B$10-AT68)*AE68 - AG68, 0)</f>
+        <f>iferror((Reference!$B$10-AT68)*(AE68 - AG68), 0)</f>
         <v>0</v>
       </c>
       <c r="AV68" s="247">
@@ -21085,16 +20961,14 @@
       <c r="E69" s="353">
         <v>129.41</v>
       </c>
-      <c r="F69" s="354">
-        <v>55.0</v>
-      </c>
+      <c r="F69" s="354"/>
       <c r="G69" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H69" s="236">
         <f t="shared" si="8"/>
-        <v>7117.55</v>
+        <v>0</v>
       </c>
       <c r="I69" s="367"/>
       <c r="J69" s="259" t="b">
@@ -21236,7 +21110,7 @@
         <v>n/a</v>
       </c>
       <c r="AU69" s="247">
-        <f>iferror((Reference!$B$10-AT69)*AE69 - AG69, 0)</f>
+        <f>iferror((Reference!$B$10-AT69)*(AE69 - AG69), 0)</f>
         <v>0</v>
       </c>
       <c r="AV69" s="247">
@@ -21258,9 +21132,7 @@
       <c r="E70" s="353">
         <v>114.06</v>
       </c>
-      <c r="F70" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F70" s="354"/>
       <c r="G70" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -21409,7 +21281,7 @@
         <v>n/a</v>
       </c>
       <c r="AU70" s="247">
-        <f>iferror((Reference!$B$10-AT70)*AE70 - AG70, 0)</f>
+        <f>iferror((Reference!$B$10-AT70)*(AE70 - AG70), 0)</f>
         <v>0</v>
       </c>
       <c r="AV70" s="247">
@@ -21435,16 +21307,14 @@
       <c r="E71" s="353">
         <v>116.17</v>
       </c>
-      <c r="F71" s="354">
-        <v>26.0</v>
-      </c>
+      <c r="F71" s="354"/>
       <c r="G71" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H71" s="236">
         <f t="shared" si="8"/>
-        <v>3020.42</v>
+        <v>0</v>
       </c>
       <c r="I71" s="355"/>
       <c r="J71" s="259" t="b">
@@ -21586,7 +21456,7 @@
         <v>n/a</v>
       </c>
       <c r="AU71" s="247">
-        <f>iferror((Reference!$B$10-AT71)*AE71 - AG71, 0)</f>
+        <f>iferror((Reference!$B$10-AT71)*(AE71 - AG71), 0)</f>
         <v>0</v>
       </c>
       <c r="AV71" s="247">
@@ -21608,9 +21478,7 @@
       <c r="E72" s="353">
         <v>114.82</v>
       </c>
-      <c r="F72" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F72" s="354"/>
       <c r="G72" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -21759,7 +21627,7 @@
         <v>n/a</v>
       </c>
       <c r="AU72" s="247">
-        <f>iferror((Reference!$B$10-AT72)*AE72 - AG72, 0)</f>
+        <f>iferror((Reference!$B$10-AT72)*(AE72 - AG72), 0)</f>
         <v>0</v>
       </c>
       <c r="AV72" s="247">
@@ -21785,16 +21653,14 @@
       <c r="E73" s="353">
         <v>112.62</v>
       </c>
-      <c r="F73" s="354">
-        <v>66.0</v>
-      </c>
+      <c r="F73" s="354"/>
       <c r="G73" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H73" s="236">
         <f t="shared" si="8"/>
-        <v>7432.92</v>
+        <v>0</v>
       </c>
       <c r="I73" s="355"/>
       <c r="J73" s="259" t="b">
@@ -21936,7 +21802,7 @@
         <v>n/a</v>
       </c>
       <c r="AU73" s="247">
-        <f>iferror((Reference!$B$10-AT73)*AE73 - AG73, 0)</f>
+        <f>iferror((Reference!$B$10-AT73)*(AE73 - AG73), 0)</f>
         <v>0</v>
       </c>
       <c r="AV73" s="247">
@@ -21962,16 +21828,14 @@
       <c r="E74" s="353">
         <v>112.62</v>
       </c>
-      <c r="F74" s="354">
-        <v>26.0</v>
-      </c>
+      <c r="F74" s="354"/>
       <c r="G74" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H74" s="236">
         <f t="shared" si="8"/>
-        <v>2928.12</v>
+        <v>0</v>
       </c>
       <c r="I74" s="355"/>
       <c r="J74" s="259" t="b">
@@ -22113,7 +21977,7 @@
         <v>n/a</v>
       </c>
       <c r="AU74" s="247">
-        <f>iferror((Reference!$B$10-AT74)*AE74 - AG74, 0)</f>
+        <f>iferror((Reference!$B$10-AT74)*(AE74 - AG74), 0)</f>
         <v>0</v>
       </c>
       <c r="AV74" s="247">
@@ -22139,16 +22003,14 @@
       <c r="E75" s="353">
         <v>121.68</v>
       </c>
-      <c r="F75" s="354">
-        <v>55.0</v>
-      </c>
+      <c r="F75" s="354"/>
       <c r="G75" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H75" s="236">
         <f t="shared" si="8"/>
-        <v>6692.4</v>
+        <v>0</v>
       </c>
       <c r="I75" s="355"/>
       <c r="J75" s="259" t="b">
@@ -22290,7 +22152,7 @@
         <v>n/a</v>
       </c>
       <c r="AU75" s="247">
-        <f>iferror((Reference!$B$10-AT75)*AE75 - AG75, 0)</f>
+        <f>iferror((Reference!$B$10-AT75)*(AE75 - AG75), 0)</f>
         <v>0</v>
       </c>
       <c r="AV75" s="247">
@@ -22312,9 +22174,7 @@
       <c r="E76" s="353">
         <v>122.76</v>
       </c>
-      <c r="F76" s="354">
-        <v>0.0</v>
-      </c>
+      <c r="F76" s="354"/>
       <c r="G76" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -22463,7 +22323,7 @@
         <v>n/a</v>
       </c>
       <c r="AU76" s="247">
-        <f>iferror((Reference!$B$10-AT76)*AE76 - AG76, 0)</f>
+        <f>iferror((Reference!$B$10-AT76)*(AE76 - AG76), 0)</f>
         <v>0</v>
       </c>
       <c r="AV76" s="247">
@@ -22489,16 +22349,14 @@
       <c r="E77" s="353">
         <v>123.34</v>
       </c>
-      <c r="F77" s="354">
-        <v>31.0</v>
-      </c>
+      <c r="F77" s="354"/>
       <c r="G77" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H77" s="236">
         <f t="shared" si="8"/>
-        <v>3823.54</v>
+        <v>0</v>
       </c>
       <c r="I77" s="367"/>
       <c r="J77" s="259" t="b">
@@ -22640,7 +22498,7 @@
         <v>n/a</v>
       </c>
       <c r="AU77" s="247">
-        <f>iferror((Reference!$B$10-AT77)*AE77 - AG77, 0)</f>
+        <f>iferror((Reference!$B$10-AT77)*(AE77 - AG77), 0)</f>
         <v>0</v>
       </c>
       <c r="AV77" s="247">
@@ -22666,16 +22524,14 @@
       <c r="E78" s="353">
         <v>110.09</v>
       </c>
-      <c r="F78" s="354">
-        <v>178.0</v>
-      </c>
+      <c r="F78" s="354"/>
       <c r="G78" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H78" s="236">
         <f t="shared" si="8"/>
-        <v>19596.02</v>
+        <v>0</v>
       </c>
       <c r="I78" s="355"/>
       <c r="J78" s="259" t="b">
@@ -22817,7 +22673,7 @@
         <v>n/a</v>
       </c>
       <c r="AU78" s="247">
-        <f>iferror((Reference!$B$10-AT78)*AE78 - AG78, 0)</f>
+        <f>iferror((Reference!$B$10-AT78)*(AE78 - AG78), 0)</f>
         <v>0</v>
       </c>
       <c r="AV78" s="247">
@@ -22843,16 +22699,14 @@
       <c r="E79" s="353">
         <v>126.98</v>
       </c>
-      <c r="F79" s="354">
-        <v>66.0</v>
-      </c>
+      <c r="F79" s="354"/>
       <c r="G79" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H79" s="236">
         <f t="shared" si="8"/>
-        <v>8380.68</v>
+        <v>0</v>
       </c>
       <c r="I79" s="355"/>
       <c r="J79" s="259" t="b">
@@ -22994,7 +22848,7 @@
         <v>n/a</v>
       </c>
       <c r="AU79" s="247">
-        <f>iferror((Reference!$B$10-AT79)*AE79 - AG79, 0)</f>
+        <f>iferror((Reference!$B$10-AT79)*(AE79 - AG79), 0)</f>
         <v>0</v>
       </c>
       <c r="AV79" s="247">
@@ -23020,16 +22874,14 @@
       <c r="E80" s="353">
         <v>126.98</v>
       </c>
-      <c r="F80" s="354">
-        <v>26.0</v>
-      </c>
+      <c r="F80" s="354"/>
       <c r="G80" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H80" s="236">
         <f t="shared" si="8"/>
-        <v>3301.48</v>
+        <v>0</v>
       </c>
       <c r="I80" s="355"/>
       <c r="J80" s="259" t="b">
@@ -23171,7 +23023,7 @@
         <v>n/a</v>
       </c>
       <c r="AU80" s="247">
-        <f>iferror((Reference!$B$10-AT80)*AE80 - AG80, 0)</f>
+        <f>iferror((Reference!$B$10-AT80)*(AE80 - AG80), 0)</f>
         <v>0</v>
       </c>
       <c r="AV80" s="247">
@@ -23197,16 +23049,14 @@
       <c r="E81" s="353">
         <v>133.94</v>
       </c>
-      <c r="F81" s="354">
-        <v>25.0</v>
-      </c>
+      <c r="F81" s="354"/>
       <c r="G81" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H81" s="236">
         <f t="shared" si="8"/>
-        <v>3348.5</v>
+        <v>0</v>
       </c>
       <c r="I81" s="355"/>
       <c r="J81" s="259" t="b">
@@ -23348,7 +23198,7 @@
         <v>n/a</v>
       </c>
       <c r="AU81" s="247">
-        <f>iferror((Reference!$B$10-AT81)*AE81 - AG81, 0)</f>
+        <f>iferror((Reference!$B$10-AT81)*(AE81 - AG81), 0)</f>
         <v>0</v>
       </c>
       <c r="AV81" s="247">
@@ -23374,16 +23224,14 @@
       <c r="E82" s="353">
         <v>133.94</v>
       </c>
-      <c r="F82" s="354">
-        <v>55.0</v>
-      </c>
+      <c r="F82" s="354"/>
       <c r="G82" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H82" s="236">
         <f t="shared" si="8"/>
-        <v>7366.7</v>
+        <v>0</v>
       </c>
       <c r="I82" s="367"/>
       <c r="J82" s="259" t="b">
@@ -23525,7 +23373,7 @@
         <v>n/a</v>
       </c>
       <c r="AU82" s="247">
-        <f>iferror((Reference!$B$10-AT82)*AE82 - AG82, 0)</f>
+        <f>iferror((Reference!$B$10-AT82)*(AE82 - AG82), 0)</f>
         <v>0</v>
       </c>
       <c r="AV82" s="247">
@@ -23551,16 +23399,14 @@
       <c r="E83" s="353">
         <v>158.96</v>
       </c>
-      <c r="F83" s="354">
-        <v>26.0</v>
-      </c>
+      <c r="F83" s="354"/>
       <c r="G83" s="225">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H83" s="236">
         <f t="shared" si="8"/>
-        <v>4132.96</v>
+        <v>0</v>
       </c>
       <c r="I83" s="355"/>
       <c r="J83" s="259" t="b">
@@ -23702,7 +23548,7 @@
         <v>n/a</v>
       </c>
       <c r="AU83" s="247">
-        <f>iferror((Reference!$B$10-AT83)*AE83 - AG83, 0)</f>
+        <f>iferror((Reference!$B$10-AT83)*(AE83 - AG83), 0)</f>
         <v>0</v>
       </c>
       <c r="AV83" s="247">
@@ -23728,16 +23574,14 @@
       <c r="E84" s="372">
         <v>164.1</v>
       </c>
-      <c r="F84" s="373">
-        <v>26.0</v>
-      </c>
+      <c r="F84" s="373"/>
       <c r="G84" s="268">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H84" s="279">
         <f t="shared" si="8"/>
-        <v>4266.6</v>
+        <v>0</v>
       </c>
       <c r="I84" s="374"/>
       <c r="J84" s="271" t="b">
@@ -23879,7 +23723,7 @@
         <v>n/a</v>
       </c>
       <c r="AU84" s="290">
-        <f>iferror((Reference!$B$10-AT84)*AE84 - AG84, 0)</f>
+        <f>iferror((Reference!$B$10-AT84)*(AE84 - AG84), 0)</f>
         <v>0</v>
       </c>
       <c r="AV84" s="290">
@@ -23915,7 +23759,7 @@
       </c>
       <c r="H86" s="299">
         <f t="shared" si="19"/>
-        <v>571638.27</v>
+        <v>0</v>
       </c>
       <c r="I86" s="340">
         <f t="shared" si="19"/>
@@ -24289,9 +24133,9 @@
       <c r="A10" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B10" s="397" t="str">
+      <c r="B10" s="397">
         <f>Summary!M28</f>
-        <v>Loading...</v>
+        <v>1361.34</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -24603,9 +24447,9 @@
       <c r="A29" s="53" t="s">
         <v>236</v>
       </c>
-      <c r="B29" s="405">
+      <c r="B29" s="405" t="str">
         <f>SWITCH(Summary!$K$28,"today",TODAY(),"last year","2023-12-31",Summary!$K$28)</f>
-        <v>45354</v>
+        <v>2023-12-31</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>

</xml_diff>

<commit_message>
Fix failure to add Other LTG into tax estimate
The Other Income LTG value was not being included in the overall LTG value used for tax estimation.
</commit_message>
<xml_diff>
--- a/VMW_to_AVGO_ESPP_and_RSU.xlsx
+++ b/VMW_to_AVGO_ESPP_and_RSU.xlsx
@@ -3863,8 +3863,8 @@
         <v>59</v>
       </c>
       <c r="M28" s="58">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),1361.34)</f>
-        <v>1361.34</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),1357.29)</f>
+        <v>1357.29</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -24135,7 +24135,7 @@
       </c>
       <c r="B10" s="397">
         <f>Summary!M28</f>
-        <v>1361.34</v>
+        <v>1357.29</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -24519,7 +24519,7 @@
         <v>239</v>
       </c>
       <c r="B33" s="409">
-        <f>ESPP!AN5+RSU!AK5+C33</f>
+        <f>Summary!K31+ESPP!AN5+RSU!AK5+C33</f>
         <v>0</v>
       </c>
       <c r="C33" s="411">

</xml_diff>

<commit_message>
Fix failure to add Other LTG into tax estimate (#81)
The Other Income LTG value was not being included in the overall LTG value used for tax estimation.

Fixes #80
</commit_message>
<xml_diff>
--- a/VMW_to_AVGO_ESPP_and_RSU.xlsx
+++ b/VMW_to_AVGO_ESPP_and_RSU.xlsx
@@ -3863,8 +3863,8 @@
         <v>59</v>
       </c>
       <c r="M28" s="58">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),1361.34)</f>
-        <v>1361.34</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),1357.29)</f>
+        <v>1357.29</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -24135,7 +24135,7 @@
       </c>
       <c r="B10" s="397">
         <f>Summary!M28</f>
-        <v>1361.34</v>
+        <v>1357.29</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -24519,7 +24519,7 @@
         <v>239</v>
       </c>
       <c r="B33" s="409">
-        <f>ESPP!AN5+RSU!AK5+C33</f>
+        <f>Summary!K31+ESPP!AN5+RSU!AK5+C33</f>
         <v>0</v>
       </c>
       <c r="C33" s="411">

</xml_diff>

<commit_message>
Fixes row skewed formula and updates binaries for v0.1.6 to v0.1.6-b
This fixes a skew in the RSU Post-merger short term capital gain column where the formula was referencing cells offset down by one row.

This was introduced with the switch to comprehensible formula.

Fixes #111
</commit_message>
<xml_diff>
--- a/VMW_to_AVGO_ESPP_and_RSU.xlsx
+++ b/VMW_to_AVGO_ESPP_and_RSU.xlsx
@@ -324,6 +324,13 @@
 Alternatively you can 0 those rows for which you don't have a purchase and enter your earliest Carry Forward into the precise row.</t>
       </text>
     </comment>
+    <comment authorId="0" ref="BA7">
+      <text>
+        <t xml:space="preserve">This is modified vs the repo 0.1.6 commit to correct an incorrect row reference (A9 but should have been A7).
+This has been done in place in poor commit/release hygine style so that people copying this sheet from now onwards don't pick up the issue.
+It'll only impact people setting post-merger sale date prior to March 1st which was the last ESPP lot qualifying transition.</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -435,6 +442,13 @@
         <t xml:space="preserve">Not allowed to recognize a loss. I'm assuming that applies at a share level rather than the aggregate holding absent explicit indication otherwise.</t>
       </text>
     </comment>
+    <comment authorId="0" ref="AV7">
+      <text>
+        <t xml:space="preserve">This is modified vs the repo 0.1.6 commit to correct an incorrect row reference (row 8 but should have been A7).
+This has been done in place in poor commit/release hygine style so that people copying this sheet from now onwards don't pick up the issue.
+</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -476,7 +490,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="262">
   <si>
     <t>Instructions</t>
   </si>
@@ -1217,57 +1231,6 @@
     <t>Tax paid on receipt</t>
   </si>
   <si>
-    <t>00029420</t>
-  </si>
-  <si>
-    <t>00055305</t>
-  </si>
-  <si>
-    <t>00066258</t>
-  </si>
-  <si>
-    <t>00075897</t>
-  </si>
-  <si>
-    <t>00081755</t>
-  </si>
-  <si>
-    <t>00092836</t>
-  </si>
-  <si>
-    <t>VM092836</t>
-  </si>
-  <si>
-    <t>VM066258</t>
-  </si>
-  <si>
-    <t>VM081755</t>
-  </si>
-  <si>
-    <t>VM100361</t>
-  </si>
-  <si>
-    <t>00124568</t>
-  </si>
-  <si>
-    <t>00155805</t>
-  </si>
-  <si>
-    <t>SD155805</t>
-  </si>
-  <si>
-    <t>SD100361</t>
-  </si>
-  <si>
-    <t>SD124568</t>
-  </si>
-  <si>
-    <t>SD172058</t>
-  </si>
-  <si>
-    <t>00194291</t>
-  </si>
-  <si>
     <r>
       <rPr/>
       <t xml:space="preserve">NOTE: </t>
@@ -4376,8 +4339,8 @@
         <v>82</v>
       </c>
       <c r="M28" s="120">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),1257.87)</f>
-        <v>1257.87</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""AVGO"")"),1235.5)</f>
+        <v>1235.5</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -6259,7 +6222,7 @@
         <v>0</v>
       </c>
       <c r="BA7" s="329" t="b">
-        <f>LET(grantDate,B7, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A9, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B7, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A7, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB7" s="328">
@@ -6541,7 +6504,7 @@
         <v>0</v>
       </c>
       <c r="BA8" s="329" t="b">
-        <f>LET(grantDate,B8, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A10, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B8, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A8, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB8" s="328">
@@ -6823,7 +6786,7 @@
         <v>0</v>
       </c>
       <c r="BA9" s="329" t="b">
-        <f>LET(grantDate,B9, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A11, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B9, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A9, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB9" s="328">
@@ -7105,7 +7068,7 @@
         <v>0</v>
       </c>
       <c r="BA10" s="329" t="b">
-        <f>LET(grantDate,B10, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A12, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B10, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A10, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB10" s="328">
@@ -7386,7 +7349,7 @@
         <v>0</v>
       </c>
       <c r="BA11" s="329" t="b">
-        <f>LET(grantDate,B11, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A13, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B11, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A11, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB11" s="328">
@@ -7668,7 +7631,7 @@
         <v>0</v>
       </c>
       <c r="BA12" s="329" t="b">
-        <f>LET(grantDate,B12, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A14, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B12, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A12, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB12" s="328">
@@ -7950,7 +7913,7 @@
         <v>0</v>
       </c>
       <c r="BA13" s="329" t="b">
-        <f>LET(grantDate,B13, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A15, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B13, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A13, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB13" s="328">
@@ -8232,7 +8195,7 @@
         <v>0</v>
       </c>
       <c r="BA14" s="329" t="b">
-        <f>LET(grantDate,B14, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A16, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B14, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A14, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB14" s="328">
@@ -8513,7 +8476,7 @@
         <v>0</v>
       </c>
       <c r="BA15" s="329" t="b">
-        <f>LET(grantDate,B15, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A17, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B15, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A15, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB15" s="328">
@@ -8794,7 +8757,7 @@
         <v>0</v>
       </c>
       <c r="BA16" s="329" t="b">
-        <f>LET(grantDate,B16, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A18, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B16, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A16, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB16" s="328">
@@ -9075,7 +9038,7 @@
         <v>0</v>
       </c>
       <c r="BA17" s="329" t="b">
-        <f>LET(grantDate,B17, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A19, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B17, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A17, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB17" s="328">
@@ -9356,7 +9319,7 @@
         <v>0</v>
       </c>
       <c r="BA18" s="329" t="b">
-        <f>LET(grantDate,B18, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A20, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B18, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A18, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB18" s="328">
@@ -9637,7 +9600,7 @@
         <v>0</v>
       </c>
       <c r="BA19" s="329" t="b">
-        <f>LET(grantDate,B19, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A21, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B19, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A19, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB19" s="328">
@@ -9918,7 +9881,7 @@
         <v>0</v>
       </c>
       <c r="BA20" s="329" t="b">
-        <f>LET(grantDate,B20, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A22, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B20, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A20, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB20" s="328">
@@ -10199,7 +10162,7 @@
         <v>0</v>
       </c>
       <c r="BA21" s="329" t="b">
-        <f>LET(grantDate,B21, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A23, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B21, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A21, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB21" s="328">
@@ -10480,7 +10443,7 @@
         <v>0</v>
       </c>
       <c r="BA22" s="329" t="b">
-        <f>LET(grantDate,B22, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A24, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B22, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A22, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB22" s="328">
@@ -10761,7 +10724,7 @@
         <v>0</v>
       </c>
       <c r="BA23" s="329" t="b">
-        <f>LET(grantDate,B23, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A25, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B23, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A23, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB23" s="328">
@@ -11042,7 +11005,7 @@
         <v>0</v>
       </c>
       <c r="BA24" s="329" t="b">
-        <f>LET(grantDate,B24, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A26, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B24, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A24, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB24" s="328">
@@ -11323,7 +11286,7 @@
         <v>0</v>
       </c>
       <c r="BA25" s="329" t="b">
-        <f>LET(grantDate,B25, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A27, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B25, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A25, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB25" s="328">
@@ -11604,7 +11567,7 @@
         <v>0</v>
       </c>
       <c r="BA26" s="329" t="b">
-        <f>LET(grantDate,B26, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A28, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
+        <f>LET(grantDate,B26, postMergerSaleDate,Reference!$B$29, purchaseBeginDate,A26, AND(DATEDIF(grantDate,postMergerSaleDate,"Y")&gt;=1, DATEDIF(purchaseBeginDate, postMergerSaleDate, "Y")&gt;=2))</f>
         <v>1</v>
       </c>
       <c r="BB26" s="328">
@@ -12507,9 +12470,7 @@
     </row>
     <row r="7">
       <c r="A7" s="431"/>
-      <c r="B7" s="432">
-        <v>40953.0</v>
-      </c>
+      <c r="B7" s="432"/>
       <c r="C7" s="301">
         <v>41487.0</v>
       </c>
@@ -12704,11 +12665,11 @@
       </c>
       <c r="AV7" s="328">
         <f>LET(
-avgoQty,AE8, 
-purchaseDate,C8,
+avgoQty,AE7, 
+purchaseDate,C7,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT8, 
+postMergerBasis,AT7, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -12731,9 +12692,7 @@
     </row>
     <row r="8">
       <c r="A8" s="431"/>
-      <c r="B8" s="432">
-        <v>40953.0</v>
-      </c>
+      <c r="B8" s="432"/>
       <c r="C8" s="301">
         <v>41671.0</v>
       </c>
@@ -12928,11 +12887,11 @@
       </c>
       <c r="AV8" s="328">
         <f>LET(
-avgoQty,AE9, 
-purchaseDate,C9,
+avgoQty,AE8, 
+purchaseDate,C8,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT9, 
+postMergerBasis,AT8, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -12954,12 +12913,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="431" t="s">
-        <v>220</v>
-      </c>
-      <c r="B9" s="432">
-        <v>40953.0</v>
-      </c>
+      <c r="A9" s="431"/>
+      <c r="B9" s="432"/>
       <c r="C9" s="301">
         <v>41852.0</v>
       </c>
@@ -13154,11 +13109,11 @@
       </c>
       <c r="AV9" s="328">
         <f>LET(
-avgoQty,AE10, 
-purchaseDate,C10,
+avgoQty,AE9, 
+purchaseDate,C9,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT10, 
+postMergerBasis,AT9, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -13180,12 +13135,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="431" t="s">
-        <v>220</v>
-      </c>
-      <c r="B10" s="432">
-        <v>40953.0</v>
-      </c>
+      <c r="A10" s="431"/>
+      <c r="B10" s="432"/>
       <c r="C10" s="301">
         <v>42036.0</v>
       </c>
@@ -13380,11 +13331,11 @@
       </c>
       <c r="AV10" s="328">
         <f>LET(
-avgoQty,AE11, 
-purchaseDate,C11,
+avgoQty,AE10, 
+purchaseDate,C10,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT11, 
+postMergerBasis,AT10, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -13406,12 +13357,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="431" t="s">
-        <v>221</v>
-      </c>
-      <c r="B11" s="432">
-        <v>41803.0</v>
-      </c>
+      <c r="A11" s="431"/>
+      <c r="B11" s="432"/>
       <c r="C11" s="301">
         <v>42125.0</v>
       </c>
@@ -13606,11 +13553,11 @@
       </c>
       <c r="AV11" s="328">
         <f>LET(
-avgoQty,AE12, 
-purchaseDate,C12,
+avgoQty,AE11, 
+purchaseDate,C11,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT12, 
+postMergerBasis,AT11, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -13632,12 +13579,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="431" t="s">
-        <v>220</v>
-      </c>
-      <c r="B12" s="432">
-        <v>40953.0</v>
-      </c>
+      <c r="A12" s="431"/>
+      <c r="B12" s="432"/>
       <c r="C12" s="301">
         <v>42217.0</v>
       </c>
@@ -13832,11 +13775,11 @@
       </c>
       <c r="AV12" s="328">
         <f>LET(
-avgoQty,AE13, 
-purchaseDate,C13,
+avgoQty,AE12, 
+purchaseDate,C12,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT13, 
+postMergerBasis,AT12, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -13858,12 +13801,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="431" t="s">
-        <v>221</v>
-      </c>
-      <c r="B13" s="432">
-        <v>41803.0</v>
-      </c>
+      <c r="A13" s="431"/>
+      <c r="B13" s="432"/>
       <c r="C13" s="301">
         <v>42309.0</v>
       </c>
@@ -14058,11 +13997,11 @@
       </c>
       <c r="AV13" s="328">
         <f>LET(
-avgoQty,AE14, 
-purchaseDate,C14,
+avgoQty,AE13, 
+purchaseDate,C13,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT14, 
+postMergerBasis,AT13, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -14084,12 +14023,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="431" t="s">
-        <v>220</v>
-      </c>
-      <c r="B14" s="432">
-        <v>40953.0</v>
-      </c>
+      <c r="A14" s="431"/>
+      <c r="B14" s="432"/>
       <c r="C14" s="301">
         <v>42401.0</v>
       </c>
@@ -14284,11 +14219,11 @@
       </c>
       <c r="AV14" s="328">
         <f>LET(
-avgoQty,AE15, 
-purchaseDate,C15,
+avgoQty,AE14, 
+purchaseDate,C14,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT15, 
+postMergerBasis,AT14, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -14310,12 +14245,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="431" t="s">
-        <v>221</v>
-      </c>
-      <c r="B15" s="432">
-        <v>41803.0</v>
-      </c>
+      <c r="A15" s="431"/>
+      <c r="B15" s="432"/>
       <c r="C15" s="301">
         <v>42491.0</v>
       </c>
@@ -14510,11 +14441,11 @@
       </c>
       <c r="AV15" s="328">
         <f>LET(
-avgoQty,AE16, 
-purchaseDate,C16,
+avgoQty,AE15, 
+purchaseDate,C15,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT16, 
+postMergerBasis,AT15, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -14536,12 +14467,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="431" t="s">
-        <v>222</v>
-      </c>
-      <c r="B16" s="432">
-        <v>42170.0</v>
-      </c>
+      <c r="A16" s="431"/>
+      <c r="B16" s="432"/>
       <c r="C16" s="301">
         <v>42491.0</v>
       </c>
@@ -14736,11 +14663,11 @@
       </c>
       <c r="AV16" s="328">
         <f>LET(
-avgoQty,AE17, 
-purchaseDate,C17,
+avgoQty,AE16, 
+purchaseDate,C16,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT17, 
+postMergerBasis,AT16, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -14762,12 +14689,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="431" t="s">
-        <v>221</v>
-      </c>
-      <c r="B17" s="432">
-        <v>41803.0</v>
-      </c>
+      <c r="A17" s="431"/>
+      <c r="B17" s="432"/>
       <c r="C17" s="301">
         <v>42675.0</v>
       </c>
@@ -14962,11 +14885,11 @@
       </c>
       <c r="AV17" s="328">
         <f>LET(
-avgoQty,AE18, 
-purchaseDate,C18,
+avgoQty,AE17, 
+purchaseDate,C17,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT18, 
+postMergerBasis,AT17, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -14988,12 +14911,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="431" t="s">
-        <v>222</v>
-      </c>
-      <c r="B18" s="432">
-        <v>42170.0</v>
-      </c>
+      <c r="A18" s="431"/>
+      <c r="B18" s="432"/>
       <c r="C18" s="301">
         <v>42675.0</v>
       </c>
@@ -15188,11 +15107,11 @@
       </c>
       <c r="AV18" s="328">
         <f>LET(
-avgoQty,AE19, 
-purchaseDate,C19,
+avgoQty,AE18, 
+purchaseDate,C18,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT19, 
+postMergerBasis,AT18, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -15214,12 +15133,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="431" t="s">
-        <v>223</v>
-      </c>
-      <c r="B19" s="432">
-        <v>42342.0</v>
-      </c>
+      <c r="A19" s="431"/>
+      <c r="B19" s="432"/>
       <c r="C19" s="301">
         <v>42705.0</v>
       </c>
@@ -15414,11 +15329,11 @@
       </c>
       <c r="AV19" s="328">
         <f>LET(
-avgoQty,AE20, 
-purchaseDate,C20,
+avgoQty,AE19, 
+purchaseDate,C19,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT20, 
+postMergerBasis,AT19, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -15440,12 +15355,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="431" t="s">
-        <v>221</v>
-      </c>
-      <c r="B20" s="432">
-        <v>41803.0</v>
-      </c>
+      <c r="A20" s="431"/>
+      <c r="B20" s="432"/>
       <c r="C20" s="301">
         <v>42856.0</v>
       </c>
@@ -15640,11 +15551,11 @@
       </c>
       <c r="AV20" s="328">
         <f>LET(
-avgoQty,AE21, 
-purchaseDate,C21,
+avgoQty,AE20, 
+purchaseDate,C20,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT21, 
+postMergerBasis,AT20, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -15666,12 +15577,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="431" t="s">
-        <v>222</v>
-      </c>
-      <c r="B21" s="432">
-        <v>42170.0</v>
-      </c>
+      <c r="A21" s="431"/>
+      <c r="B21" s="432"/>
       <c r="C21" s="301">
         <v>42856.0</v>
       </c>
@@ -15866,11 +15773,11 @@
       </c>
       <c r="AV21" s="328">
         <f>LET(
-avgoQty,AE22, 
-purchaseDate,C22,
+avgoQty,AE21, 
+purchaseDate,C21,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT22, 
+postMergerBasis,AT21, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -15892,12 +15799,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="431" t="s">
-        <v>224</v>
-      </c>
-      <c r="B22" s="432">
-        <v>42489.0</v>
-      </c>
+      <c r="A22" s="431"/>
+      <c r="B22" s="432"/>
       <c r="C22" s="301">
         <v>42856.0</v>
       </c>
@@ -16092,11 +15995,11 @@
       </c>
       <c r="AV22" s="328">
         <f>LET(
-avgoQty,AE23, 
-purchaseDate,C23,
+avgoQty,AE22, 
+purchaseDate,C22,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT23, 
+postMergerBasis,AT22, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -16118,12 +16021,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="431" t="s">
-        <v>223</v>
-      </c>
-      <c r="B23" s="432">
-        <v>42342.0</v>
-      </c>
+      <c r="A23" s="431"/>
+      <c r="B23" s="432"/>
       <c r="C23" s="301">
         <v>42887.0</v>
       </c>
@@ -16318,11 +16217,11 @@
       </c>
       <c r="AV23" s="328">
         <f>LET(
-avgoQty,AE24, 
-purchaseDate,C24,
+avgoQty,AE23, 
+purchaseDate,C23,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT24, 
+postMergerBasis,AT23, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -16344,12 +16243,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="431" t="s">
-        <v>221</v>
-      </c>
-      <c r="B24" s="432">
-        <v>41803.0</v>
-      </c>
+      <c r="A24" s="431"/>
+      <c r="B24" s="432"/>
       <c r="C24" s="301">
         <v>43040.0</v>
       </c>
@@ -16544,11 +16439,11 @@
       </c>
       <c r="AV24" s="328">
         <f>LET(
-avgoQty,AE25, 
-purchaseDate,C25,
+avgoQty,AE24, 
+purchaseDate,C24,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT25, 
+postMergerBasis,AT24, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -16570,12 +16465,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="431" t="s">
-        <v>222</v>
-      </c>
-      <c r="B25" s="432">
-        <v>42170.0</v>
-      </c>
+      <c r="A25" s="431"/>
+      <c r="B25" s="432"/>
       <c r="C25" s="301">
         <v>43040.0</v>
       </c>
@@ -16770,11 +16661,11 @@
       </c>
       <c r="AV25" s="328">
         <f>LET(
-avgoQty,AE26, 
-purchaseDate,C26,
+avgoQty,AE25, 
+purchaseDate,C25,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT26, 
+postMergerBasis,AT25, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -16796,12 +16687,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="431" t="s">
-        <v>224</v>
-      </c>
-      <c r="B26" s="432">
-        <v>42489.0</v>
-      </c>
+      <c r="A26" s="431"/>
+      <c r="B26" s="432"/>
       <c r="C26" s="301">
         <v>43040.0</v>
       </c>
@@ -16996,11 +16883,11 @@
       </c>
       <c r="AV26" s="328">
         <f>LET(
-avgoQty,AE27, 
-purchaseDate,C27,
+avgoQty,AE26, 
+purchaseDate,C26,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT27, 
+postMergerBasis,AT26, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -17022,12 +16909,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="431" t="s">
-        <v>223</v>
-      </c>
-      <c r="B27" s="432">
-        <v>42342.0</v>
-      </c>
+      <c r="A27" s="431"/>
+      <c r="B27" s="432"/>
       <c r="C27" s="301">
         <v>43070.0</v>
       </c>
@@ -17222,11 +17105,11 @@
       </c>
       <c r="AV27" s="328">
         <f>LET(
-avgoQty,AE28, 
-purchaseDate,C28,
+avgoQty,AE27, 
+purchaseDate,C27,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT28, 
+postMergerBasis,AT27, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -17248,12 +17131,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="431" t="s">
-        <v>221</v>
-      </c>
-      <c r="B28" s="432">
-        <v>41803.0</v>
-      </c>
+      <c r="A28" s="431"/>
+      <c r="B28" s="432"/>
       <c r="C28" s="301">
         <v>43221.0</v>
       </c>
@@ -17448,11 +17327,11 @@
       </c>
       <c r="AV28" s="328">
         <f>LET(
-avgoQty,AE29, 
-purchaseDate,C29,
+avgoQty,AE28, 
+purchaseDate,C28,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT29, 
+postMergerBasis,AT28, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -17474,12 +17353,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="431" t="s">
-        <v>222</v>
-      </c>
-      <c r="B29" s="432">
-        <v>42170.0</v>
-      </c>
+      <c r="A29" s="431"/>
+      <c r="B29" s="432"/>
       <c r="C29" s="301">
         <v>43221.0</v>
       </c>
@@ -17674,11 +17549,11 @@
       </c>
       <c r="AV29" s="328">
         <f>LET(
-avgoQty,AE30, 
-purchaseDate,C30,
+avgoQty,AE29, 
+purchaseDate,C29,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT30, 
+postMergerBasis,AT29, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -17700,12 +17575,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="431" t="s">
-        <v>224</v>
-      </c>
-      <c r="B30" s="432">
-        <v>42489.0</v>
-      </c>
+      <c r="A30" s="431"/>
+      <c r="B30" s="432"/>
       <c r="C30" s="301">
         <v>43221.0</v>
       </c>
@@ -17900,11 +17771,11 @@
       </c>
       <c r="AV30" s="328">
         <f>LET(
-avgoQty,AE31, 
-purchaseDate,C31,
+avgoQty,AE30, 
+purchaseDate,C30,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT31, 
+postMergerBasis,AT30, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -17926,12 +17797,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="431" t="s">
-        <v>223</v>
-      </c>
-      <c r="B31" s="432">
-        <v>42342.0</v>
-      </c>
+      <c r="A31" s="431"/>
+      <c r="B31" s="432"/>
       <c r="C31" s="301">
         <v>43252.0</v>
       </c>
@@ -18126,11 +17993,11 @@
       </c>
       <c r="AV31" s="328">
         <f>LET(
-avgoQty,AE32, 
-purchaseDate,C32,
+avgoQty,AE31, 
+purchaseDate,C31,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT32, 
+postMergerBasis,AT31, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -18152,12 +18019,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="431" t="s">
-        <v>225</v>
-      </c>
-      <c r="B32" s="432">
-        <v>42929.0</v>
-      </c>
+      <c r="A32" s="431"/>
+      <c r="B32" s="432"/>
       <c r="C32" s="301">
         <v>43282.0</v>
       </c>
@@ -18352,11 +18215,11 @@
       </c>
       <c r="AV32" s="328">
         <f>LET(
-avgoQty,AE33, 
-purchaseDate,C33,
+avgoQty,AE32, 
+purchaseDate,C32,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT33, 
+postMergerBasis,AT32, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -18378,12 +18241,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="431" t="s">
-        <v>222</v>
-      </c>
-      <c r="B33" s="432">
-        <v>42170.0</v>
-      </c>
+      <c r="A33" s="431"/>
+      <c r="B33" s="432"/>
       <c r="C33" s="301">
         <v>43405.0</v>
       </c>
@@ -18578,11 +18437,11 @@
       </c>
       <c r="AV33" s="328">
         <f>LET(
-avgoQty,AE34, 
-purchaseDate,C34,
+avgoQty,AE33, 
+purchaseDate,C33,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT34, 
+postMergerBasis,AT33, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -18604,12 +18463,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="431" t="s">
-        <v>224</v>
-      </c>
-      <c r="B34" s="432">
-        <v>42489.0</v>
-      </c>
+      <c r="A34" s="431"/>
+      <c r="B34" s="432"/>
       <c r="C34" s="301">
         <v>43405.0</v>
       </c>
@@ -18804,11 +18659,11 @@
       </c>
       <c r="AV34" s="328">
         <f>LET(
-avgoQty,AE35, 
-purchaseDate,C35,
+avgoQty,AE34, 
+purchaseDate,C34,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT35, 
+postMergerBasis,AT34, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -18830,12 +18685,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="431" t="s">
-        <v>223</v>
-      </c>
-      <c r="B35" s="432">
-        <v>42342.0</v>
-      </c>
+      <c r="A35" s="431"/>
+      <c r="B35" s="432"/>
       <c r="C35" s="301">
         <v>43435.0</v>
       </c>
@@ -19030,11 +18881,11 @@
       </c>
       <c r="AV35" s="328">
         <f>LET(
-avgoQty,AE36, 
-purchaseDate,C36,
+avgoQty,AE35, 
+purchaseDate,C35,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT36, 
+postMergerBasis,AT35, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -19056,12 +18907,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="431" t="s">
-        <v>226</v>
-      </c>
-      <c r="B36" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A36" s="431"/>
+      <c r="B36" s="432"/>
       <c r="C36" s="301">
         <v>43475.0</v>
       </c>
@@ -19256,11 +19103,11 @@
       </c>
       <c r="AV36" s="328">
         <f>LET(
-avgoQty,AE37, 
-purchaseDate,C37,
+avgoQty,AE36, 
+purchaseDate,C36,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT37, 
+postMergerBasis,AT36, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -19282,12 +19129,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="431" t="s">
-        <v>227</v>
-      </c>
-      <c r="B37" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A37" s="431"/>
+      <c r="B37" s="432"/>
       <c r="C37" s="301">
         <v>43586.0</v>
       </c>
@@ -19482,11 +19325,11 @@
       </c>
       <c r="AV37" s="328">
         <f>LET(
-avgoQty,AE38, 
-purchaseDate,C38,
+avgoQty,AE37, 
+purchaseDate,C37,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT38, 
+postMergerBasis,AT37, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -19508,12 +19351,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="431" t="s">
-        <v>228</v>
-      </c>
-      <c r="B38" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A38" s="431"/>
+      <c r="B38" s="432"/>
       <c r="C38" s="301">
         <v>43586.0</v>
       </c>
@@ -19708,11 +19547,11 @@
       </c>
       <c r="AV38" s="328">
         <f>LET(
-avgoQty,AE39, 
-purchaseDate,C39,
+avgoQty,AE38, 
+purchaseDate,C38,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT39, 
+postMergerBasis,AT38, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -19734,12 +19573,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="431" t="s">
-        <v>229</v>
-      </c>
-      <c r="B39" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A39" s="431"/>
+      <c r="B39" s="432"/>
       <c r="C39" s="301">
         <v>43617.0</v>
       </c>
@@ -19934,11 +19769,11 @@
       </c>
       <c r="AV39" s="328">
         <f>LET(
-avgoQty,AE40, 
-purchaseDate,C40,
+avgoQty,AE39, 
+purchaseDate,C39,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT40, 
+postMergerBasis,AT39, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -19960,12 +19795,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="431" t="s">
-        <v>226</v>
-      </c>
-      <c r="B40" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A40" s="431"/>
+      <c r="B40" s="432"/>
       <c r="C40" s="301">
         <v>43647.0</v>
       </c>
@@ -20160,11 +19991,11 @@
       </c>
       <c r="AV40" s="328">
         <f>LET(
-avgoQty,AE41, 
-purchaseDate,C41,
+avgoQty,AE40, 
+purchaseDate,C40,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT41, 
+postMergerBasis,AT40, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -20186,12 +20017,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="431" t="s">
-        <v>228</v>
-      </c>
-      <c r="B41" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A41" s="431"/>
+      <c r="B41" s="432"/>
       <c r="C41" s="301">
         <v>43770.0</v>
       </c>
@@ -20386,11 +20213,11 @@
       </c>
       <c r="AV41" s="328">
         <f>LET(
-avgoQty,AE42, 
-purchaseDate,C42,
+avgoQty,AE41, 
+purchaseDate,C41,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT42, 
+postMergerBasis,AT41, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -20412,12 +20239,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="431" t="s">
-        <v>229</v>
-      </c>
-      <c r="B42" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A42" s="431"/>
+      <c r="B42" s="432"/>
       <c r="C42" s="301">
         <v>43800.0</v>
       </c>
@@ -20612,11 +20435,11 @@
       </c>
       <c r="AV42" s="328">
         <f>LET(
-avgoQty,AE43, 
-purchaseDate,C43,
+avgoQty,AE42, 
+purchaseDate,C42,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT43, 
+postMergerBasis,AT42, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -20638,12 +20461,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="431" t="s">
-        <v>226</v>
-      </c>
-      <c r="B43" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A43" s="431"/>
+      <c r="B43" s="432"/>
       <c r="C43" s="301">
         <v>43831.0</v>
       </c>
@@ -20838,11 +20657,11 @@
       </c>
       <c r="AV43" s="328">
         <f>LET(
-avgoQty,AE44, 
-purchaseDate,C44,
+avgoQty,AE43, 
+purchaseDate,C43,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT44, 
+postMergerBasis,AT43, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -21060,11 +20879,11 @@
       </c>
       <c r="AV44" s="328">
         <f>LET(
-avgoQty,AE45, 
-purchaseDate,C45,
+avgoQty,AE44, 
+purchaseDate,C44,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT45, 
+postMergerBasis,AT44, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -21282,11 +21101,11 @@
       </c>
       <c r="AV45" s="328">
         <f>LET(
-avgoQty,AE46, 
-purchaseDate,C46,
+avgoQty,AE45, 
+purchaseDate,C45,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT46, 
+postMergerBasis,AT45, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -21308,12 +21127,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="431" t="s">
-        <v>228</v>
-      </c>
-      <c r="B46" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A46" s="431"/>
+      <c r="B46" s="432"/>
       <c r="C46" s="301">
         <v>43952.0</v>
       </c>
@@ -21508,11 +21323,11 @@
       </c>
       <c r="AV46" s="328">
         <f>LET(
-avgoQty,AE47, 
-purchaseDate,C47,
+avgoQty,AE46, 
+purchaseDate,C46,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT47, 
+postMergerBasis,AT46, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -21534,12 +21349,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="431" t="s">
-        <v>230</v>
-      </c>
-      <c r="B47" s="432">
-        <v>43630.0</v>
-      </c>
+      <c r="A47" s="431"/>
+      <c r="B47" s="432"/>
       <c r="C47" s="301">
         <v>43983.0</v>
       </c>
@@ -21734,11 +21545,11 @@
       </c>
       <c r="AV47" s="328">
         <f>LET(
-avgoQty,AE48, 
-purchaseDate,C48,
+avgoQty,AE47, 
+purchaseDate,C47,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT48, 
+postMergerBasis,AT47, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -21760,12 +21571,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="431" t="s">
-        <v>229</v>
-      </c>
-      <c r="B48" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A48" s="431"/>
+      <c r="B48" s="432"/>
       <c r="C48" s="301">
         <v>43983.0</v>
       </c>
@@ -21960,11 +21767,11 @@
       </c>
       <c r="AV48" s="328">
         <f>LET(
-avgoQty,AE49, 
-purchaseDate,C49,
+avgoQty,AE48, 
+purchaseDate,C48,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT49, 
+postMergerBasis,AT48, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -21986,12 +21793,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="431" t="s">
-        <v>226</v>
-      </c>
-      <c r="B49" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A49" s="431"/>
+      <c r="B49" s="432"/>
       <c r="C49" s="301">
         <v>44013.0</v>
       </c>
@@ -22186,11 +21989,11 @@
       </c>
       <c r="AV49" s="328">
         <f>LET(
-avgoQty,AE50, 
-purchaseDate,C50,
+avgoQty,AE49, 
+purchaseDate,C49,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT50, 
+postMergerBasis,AT49, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -22408,11 +22211,11 @@
       </c>
       <c r="AV50" s="328">
         <f>LET(
-avgoQty,AE51, 
-purchaseDate,C51,
+avgoQty,AE50, 
+purchaseDate,C50,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT51, 
+postMergerBasis,AT50, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -22434,12 +22237,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="431" t="s">
-        <v>230</v>
-      </c>
-      <c r="B51" s="432">
-        <v>43630.0</v>
-      </c>
+      <c r="A51" s="431"/>
+      <c r="B51" s="432"/>
       <c r="C51" s="301">
         <v>44166.0</v>
       </c>
@@ -22634,11 +22433,11 @@
       </c>
       <c r="AV51" s="328">
         <f>LET(
-avgoQty,AE52, 
-purchaseDate,C52,
+avgoQty,AE51, 
+purchaseDate,C51,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT52, 
+postMergerBasis,AT51, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -22660,12 +22459,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="431" t="s">
-        <v>229</v>
-      </c>
-      <c r="B52" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A52" s="431"/>
+      <c r="B52" s="432"/>
       <c r="C52" s="301">
         <v>44166.0</v>
       </c>
@@ -22860,11 +22655,11 @@
       </c>
       <c r="AV52" s="328">
         <f>LET(
-avgoQty,AE53, 
-purchaseDate,C53,
+avgoQty,AE52, 
+purchaseDate,C52,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT53, 
+postMergerBasis,AT52, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -22886,12 +22681,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="431" t="s">
-        <v>226</v>
-      </c>
-      <c r="B53" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A53" s="431"/>
+      <c r="B53" s="432"/>
       <c r="C53" s="301">
         <v>44197.0</v>
       </c>
@@ -23086,11 +22877,11 @@
       </c>
       <c r="AV53" s="328">
         <f>LET(
-avgoQty,AE54, 
-purchaseDate,C54,
+avgoQty,AE53, 
+purchaseDate,C53,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT54, 
+postMergerBasis,AT53, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -23308,11 +23099,11 @@
       </c>
       <c r="AV54" s="328">
         <f>LET(
-avgoQty,AE55, 
-purchaseDate,C55,
+avgoQty,AE54, 
+purchaseDate,C54,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT55, 
+postMergerBasis,AT54, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -23334,12 +23125,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="431" t="s">
-        <v>231</v>
-      </c>
-      <c r="B55" s="432">
-        <v>43980.0</v>
-      </c>
+      <c r="A55" s="431"/>
+      <c r="B55" s="432"/>
       <c r="C55" s="301">
         <v>44317.0</v>
       </c>
@@ -23534,11 +23321,11 @@
       </c>
       <c r="AV55" s="328">
         <f>LET(
-avgoQty,AE56, 
-purchaseDate,C56,
+avgoQty,AE55, 
+purchaseDate,C55,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT56, 
+postMergerBasis,AT55, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -23560,12 +23347,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="431" t="s">
-        <v>230</v>
-      </c>
-      <c r="B56" s="432">
-        <v>43630.0</v>
-      </c>
+      <c r="A56" s="431"/>
+      <c r="B56" s="432"/>
       <c r="C56" s="301">
         <v>44348.0</v>
       </c>
@@ -23760,11 +23543,11 @@
       </c>
       <c r="AV56" s="328">
         <f>LET(
-avgoQty,AE57, 
-purchaseDate,C57,
+avgoQty,AE56, 
+purchaseDate,C56,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT57, 
+postMergerBasis,AT56, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -23786,12 +23569,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="431" t="s">
-        <v>229</v>
-      </c>
-      <c r="B57" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A57" s="431"/>
+      <c r="B57" s="432"/>
       <c r="C57" s="301">
         <v>44348.0</v>
       </c>
@@ -23986,11 +23765,11 @@
       </c>
       <c r="AV57" s="328">
         <f>LET(
-avgoQty,AE58, 
-purchaseDate,C58,
+avgoQty,AE57, 
+purchaseDate,C57,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT58, 
+postMergerBasis,AT57, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -24012,12 +23791,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="431" t="s">
-        <v>226</v>
-      </c>
-      <c r="B58" s="432">
-        <v>43462.0</v>
-      </c>
+      <c r="A58" s="431"/>
+      <c r="B58" s="432"/>
       <c r="C58" s="301">
         <v>44378.0</v>
       </c>
@@ -24212,11 +23987,11 @@
       </c>
       <c r="AV58" s="328">
         <f>LET(
-avgoQty,AE59, 
-purchaseDate,C59,
+avgoQty,AE58, 
+purchaseDate,C58,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT59, 
+postMergerBasis,AT58, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -24434,11 +24209,11 @@
       </c>
       <c r="AV59" s="328">
         <f>LET(
-avgoQty,AE60, 
-purchaseDate,C60,
+avgoQty,AE59, 
+purchaseDate,C59,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT60, 
+postMergerBasis,AT59, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -24460,12 +24235,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="431" t="s">
-        <v>232</v>
-      </c>
-      <c r="B60" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A60" s="431"/>
+      <c r="B60" s="432"/>
       <c r="C60" s="301">
         <v>44511.0</v>
       </c>
@@ -24660,11 +24431,11 @@
       </c>
       <c r="AV60" s="328">
         <f>LET(
-avgoQty,AE61, 
-purchaseDate,C61,
+avgoQty,AE60, 
+purchaseDate,C60,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT61, 
+postMergerBasis,AT60, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -24686,12 +24457,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="431" t="s">
-        <v>233</v>
-      </c>
-      <c r="B61" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A61" s="431"/>
+      <c r="B61" s="432"/>
       <c r="C61" s="301">
         <v>44531.0</v>
       </c>
@@ -24886,11 +24653,11 @@
       </c>
       <c r="AV61" s="328">
         <f>LET(
-avgoQty,AE62, 
-purchaseDate,C62,
+avgoQty,AE61, 
+purchaseDate,C61,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT62, 
+postMergerBasis,AT61, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -24912,12 +24679,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="431" t="s">
-        <v>234</v>
-      </c>
-      <c r="B62" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A62" s="431"/>
+      <c r="B62" s="432"/>
       <c r="C62" s="301">
         <v>44531.0</v>
       </c>
@@ -25112,11 +24875,11 @@
       </c>
       <c r="AV62" s="328">
         <f>LET(
-avgoQty,AE63, 
-purchaseDate,C63,
+avgoQty,AE62, 
+purchaseDate,C62,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT63, 
+postMergerBasis,AT62, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -25334,11 +25097,11 @@
       </c>
       <c r="AV63" s="328">
         <f>LET(
-avgoQty,AE64, 
-purchaseDate,C64,
+avgoQty,AE63, 
+purchaseDate,C63,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT64, 
+postMergerBasis,AT63, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -25360,12 +25123,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="431" t="s">
-        <v>235</v>
-      </c>
-      <c r="B64" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A64" s="431"/>
+      <c r="B64" s="432"/>
       <c r="C64" s="301">
         <v>44593.0</v>
       </c>
@@ -25560,11 +25319,11 @@
       </c>
       <c r="AV64" s="328">
         <f>LET(
-avgoQty,AE65, 
-purchaseDate,C65,
+avgoQty,AE64, 
+purchaseDate,C64,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT65, 
+postMergerBasis,AT64, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -25782,11 +25541,11 @@
       </c>
       <c r="AV65" s="328">
         <f>LET(
-avgoQty,AE66, 
-purchaseDate,C66,
+avgoQty,AE65, 
+purchaseDate,C65,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT66, 
+postMergerBasis,AT65, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -25808,12 +25567,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="431" t="s">
-        <v>232</v>
-      </c>
-      <c r="B66" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A66" s="431"/>
+      <c r="B66" s="432"/>
       <c r="C66" s="301">
         <v>44682.0</v>
       </c>
@@ -26008,11 +25763,11 @@
       </c>
       <c r="AV66" s="328">
         <f>LET(
-avgoQty,AE67, 
-purchaseDate,C67,
+avgoQty,AE66, 
+purchaseDate,C66,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT67, 
+postMergerBasis,AT66, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -26034,12 +25789,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="431" t="s">
-        <v>235</v>
-      </c>
-      <c r="B67" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A67" s="431"/>
+      <c r="B67" s="432"/>
       <c r="C67" s="301">
         <v>44682.0</v>
       </c>
@@ -26234,11 +25985,11 @@
       </c>
       <c r="AV67" s="328">
         <f>LET(
-avgoQty,AE68, 
-purchaseDate,C68,
+avgoQty,AE67, 
+purchaseDate,C67,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT68, 
+postMergerBasis,AT67, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -26260,12 +26011,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="431" t="s">
-        <v>233</v>
-      </c>
-      <c r="B68" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A68" s="431"/>
+      <c r="B68" s="432"/>
       <c r="C68" s="301">
         <v>44713.0</v>
       </c>
@@ -26460,11 +26207,11 @@
       </c>
       <c r="AV68" s="328">
         <f>LET(
-avgoQty,AE69, 
-purchaseDate,C69,
+avgoQty,AE68, 
+purchaseDate,C68,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT69, 
+postMergerBasis,AT68, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -26486,12 +26233,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="431" t="s">
-        <v>234</v>
-      </c>
-      <c r="B69" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A69" s="431"/>
+      <c r="B69" s="432"/>
       <c r="C69" s="301">
         <v>44713.0</v>
       </c>
@@ -26686,11 +26429,11 @@
       </c>
       <c r="AV69" s="328">
         <f>LET(
-avgoQty,AE70, 
-purchaseDate,C70,
+avgoQty,AE69, 
+purchaseDate,C69,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT70, 
+postMergerBasis,AT69, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -26908,11 +26651,11 @@
       </c>
       <c r="AV70" s="328">
         <f>LET(
-avgoQty,AE71, 
-purchaseDate,C71,
+avgoQty,AE70, 
+purchaseDate,C70,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT71, 
+postMergerBasis,AT70, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -26934,12 +26677,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="431" t="s">
-        <v>235</v>
-      </c>
-      <c r="B71" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A71" s="431"/>
+      <c r="B71" s="432"/>
       <c r="C71" s="301">
         <v>44774.0</v>
       </c>
@@ -27134,11 +26873,11 @@
       </c>
       <c r="AV71" s="328">
         <f>LET(
-avgoQty,AE72, 
-purchaseDate,C72,
+avgoQty,AE71, 
+purchaseDate,C71,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT72, 
+postMergerBasis,AT71, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -27356,11 +27095,11 @@
       </c>
       <c r="AV72" s="328">
         <f>LET(
-avgoQty,AE73, 
-purchaseDate,C73,
+avgoQty,AE72, 
+purchaseDate,C72,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT73, 
+postMergerBasis,AT72, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -27382,12 +27121,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="431" t="s">
-        <v>232</v>
-      </c>
-      <c r="B73" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A73" s="431"/>
+      <c r="B73" s="432"/>
       <c r="C73" s="301">
         <v>44866.0</v>
       </c>
@@ -27582,11 +27317,11 @@
       </c>
       <c r="AV73" s="328">
         <f>LET(
-avgoQty,AE74, 
-purchaseDate,C74,
+avgoQty,AE73, 
+purchaseDate,C73,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT74, 
+postMergerBasis,AT73, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -27608,12 +27343,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="431" t="s">
-        <v>235</v>
-      </c>
-      <c r="B74" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A74" s="431"/>
+      <c r="B74" s="432"/>
       <c r="C74" s="301">
         <v>44866.0</v>
       </c>
@@ -27808,11 +27539,11 @@
       </c>
       <c r="AV74" s="328">
         <f>LET(
-avgoQty,AE75, 
-purchaseDate,C75,
+avgoQty,AE74, 
+purchaseDate,C74,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT75, 
+postMergerBasis,AT74, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -27834,12 +27565,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="431" t="s">
-        <v>234</v>
-      </c>
-      <c r="B75" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A75" s="431"/>
+      <c r="B75" s="432"/>
       <c r="C75" s="301">
         <v>44896.0</v>
       </c>
@@ -28034,11 +27761,11 @@
       </c>
       <c r="AV75" s="328">
         <f>LET(
-avgoQty,AE76, 
-purchaseDate,C76,
+avgoQty,AE75, 
+purchaseDate,C75,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT76, 
+postMergerBasis,AT75, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -28256,11 +27983,11 @@
       </c>
       <c r="AV76" s="328">
         <f>LET(
-avgoQty,AE77, 
-purchaseDate,C77,
+avgoQty,AE76, 
+purchaseDate,C76,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT77, 
+postMergerBasis,AT76, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -28282,12 +28009,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="431" t="s">
-        <v>235</v>
-      </c>
-      <c r="B77" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A77" s="431"/>
+      <c r="B77" s="432"/>
       <c r="C77" s="301">
         <v>44958.0</v>
       </c>
@@ -28482,11 +28205,11 @@
       </c>
       <c r="AV77" s="328">
         <f>LET(
-avgoQty,AE78, 
-purchaseDate,C78,
+avgoQty,AE77, 
+purchaseDate,C77,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT78, 
+postMergerBasis,AT77, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -28508,12 +28231,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="431" t="s">
-        <v>236</v>
-      </c>
-      <c r="B78" s="432">
-        <v>44741.0</v>
-      </c>
+      <c r="A78" s="431"/>
+      <c r="B78" s="432"/>
       <c r="C78" s="301">
         <v>44986.0</v>
       </c>
@@ -28708,11 +28427,11 @@
       </c>
       <c r="AV78" s="328">
         <f>LET(
-avgoQty,AE79, 
-purchaseDate,C79,
+avgoQty,AE78, 
+purchaseDate,C78,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT79, 
+postMergerBasis,AT78, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -28734,12 +28453,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="431" t="s">
-        <v>232</v>
-      </c>
-      <c r="B79" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A79" s="431"/>
+      <c r="B79" s="432"/>
       <c r="C79" s="301">
         <v>45047.0</v>
       </c>
@@ -28934,11 +28649,11 @@
       </c>
       <c r="AV79" s="328">
         <f>LET(
-avgoQty,AE80, 
-purchaseDate,C80,
+avgoQty,AE79, 
+purchaseDate,C79,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT80, 
+postMergerBasis,AT79, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -28960,12 +28675,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="431" t="s">
-        <v>235</v>
-      </c>
-      <c r="B80" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A80" s="431"/>
+      <c r="B80" s="432"/>
       <c r="C80" s="301">
         <v>45047.0</v>
       </c>
@@ -29160,11 +28871,11 @@
       </c>
       <c r="AV80" s="328">
         <f>LET(
-avgoQty,AE81, 
-purchaseDate,C81,
+avgoQty,AE80, 
+purchaseDate,C80,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT81, 
+postMergerBasis,AT80, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -29186,12 +28897,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="431" t="s">
-        <v>236</v>
-      </c>
-      <c r="B81" s="432">
-        <v>44741.0</v>
-      </c>
+      <c r="A81" s="431"/>
+      <c r="B81" s="432"/>
       <c r="C81" s="301">
         <v>45078.0</v>
       </c>
@@ -29386,11 +29093,11 @@
       </c>
       <c r="AV81" s="328">
         <f>LET(
-avgoQty,AE82, 
-purchaseDate,C82,
+avgoQty,AE81, 
+purchaseDate,C81,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT82, 
+postMergerBasis,AT81, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -29412,12 +29119,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="431" t="s">
-        <v>234</v>
-      </c>
-      <c r="B82" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A82" s="431"/>
+      <c r="B82" s="432"/>
       <c r="C82" s="301">
         <v>45078.0</v>
       </c>
@@ -29612,11 +29315,11 @@
       </c>
       <c r="AV82" s="328">
         <f>LET(
-avgoQty,AE83, 
-purchaseDate,C83,
+avgoQty,AE82, 
+purchaseDate,C82,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT83, 
+postMergerBasis,AT82, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -29638,12 +29341,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="431" t="s">
-        <v>235</v>
-      </c>
-      <c r="B83" s="432">
-        <v>44501.0</v>
-      </c>
+      <c r="A83" s="431"/>
+      <c r="B83" s="432"/>
       <c r="C83" s="301">
         <v>45139.0</v>
       </c>
@@ -29838,11 +29537,11 @@
       </c>
       <c r="AV83" s="328">
         <f>LET(
-avgoQty,AE84, 
-purchaseDate,C84,
+avgoQty,AE83, 
+purchaseDate,C83,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT84, 
+postMergerBasis,AT83, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -29864,12 +29563,8 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="449" t="s">
-        <v>236</v>
-      </c>
-      <c r="B84" s="450">
-        <v>44741.0</v>
-      </c>
+      <c r="A84" s="449"/>
+      <c r="B84" s="450"/>
       <c r="C84" s="347">
         <v>45170.0</v>
       </c>
@@ -30064,11 +29759,11 @@
       </c>
       <c r="AV84" s="328">
         <f>LET(
-avgoQty,AE85, 
-purchaseDate,C85,
+avgoQty,AE84, 
+purchaseDate,C84,
 postMergerSaleDate,Reference!$B$29,
 saleFMV,Reference!$B$10,
-postMergerBasis,AT85, 
+postMergerBasis,AT84, 
 IFERROR(IF(DATEDIF(purchaseDate,postMergerSaleDate,"Y")&gt;=1,
   0,
   avgoQty * (saleFMV - postMergerBasis)
@@ -30293,7 +29988,7 @@
       <c r="AM88" s="393"/>
       <c r="AN88" s="393"/>
       <c r="AO88" s="43" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -30376,7 +30071,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="114" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="B1" s="114"/>
       <c r="C1" s="2"/>
@@ -30404,14 +30099,14 @@
     </row>
     <row r="3">
       <c r="A3" s="114" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="B3" s="477">
         <v>142.5</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="114" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="E3" s="478">
         <f>B3*B4 + B18*B5*B6</f>
@@ -30426,7 +30121,7 @@
     </row>
     <row r="4">
       <c r="A4" s="114" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="B4" s="479">
         <f>1-B5</f>
@@ -30434,7 +30129,7 @@
       </c>
       <c r="C4" s="480"/>
       <c r="D4" s="110" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="E4" s="481" t="str">
         <f>SWITCH(Summary!K26,"Pro-rata - from eTrade transaction log", "eTradeTransactionLog", "Pro-rata - from Necessary Inputs", "eTradeHoldingRatio","Pro-rata - from eTrade share qty","eTradeLotQtyRatio", "Per-lot - from strategy or manual selection", "manualLotRatio")</f>
@@ -30449,7 +30144,7 @@
     </row>
     <row r="5">
       <c r="A5" s="114" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="B5" s="479">
         <f>IF(EQ($E$4, "eTradeTransactionLog"), $B$7,iferror(Summary!B26/(Summary!B26+Summary!B25),0))</f>
@@ -30457,7 +30152,7 @@
       </c>
       <c r="C5" s="114"/>
       <c r="D5" s="114" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="E5" s="482">
         <v>0.0</v>
@@ -30471,14 +30166,14 @@
     </row>
     <row r="6">
       <c r="A6" s="114" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B6" s="483">
         <v>0.252</v>
       </c>
       <c r="C6" s="114"/>
       <c r="D6" s="114" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="E6" s="484">
         <v>1.0</v>
@@ -30492,14 +30187,14 @@
     </row>
     <row r="7">
       <c r="A7" s="114" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="B7" s="485" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="C7" s="114"/>
       <c r="D7" s="114" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="E7" s="486" t="str">
         <f>LET(
@@ -30530,7 +30225,7 @@
       <c r="B8" s="144"/>
       <c r="C8" s="114"/>
       <c r="D8" s="114" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="E8" s="114" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("LET(
@@ -30555,7 +30250,7 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="114" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="E9" s="488" t="str">
         <f>iferror(SWITCH(#REF!, "Cash Only", "cashOnly", "Cash &amp; AVGO FMV", "combined"),"combined")</f>
@@ -30570,11 +30265,11 @@
     </row>
     <row r="10">
       <c r="A10" s="96" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B10" s="489">
         <f>Summary!M28</f>
-        <v>1257.87</v>
+        <v>1235.5</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -30601,7 +30296,7 @@
     </row>
     <row r="12">
       <c r="A12" s="490" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -30616,7 +30311,7 @@
     </row>
     <row r="13">
       <c r="A13" s="490" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="B13" s="477">
         <v>983.69</v>
@@ -30633,7 +30328,7 @@
     </row>
     <row r="14">
       <c r="A14" s="490" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="B14" s="477">
         <v>972.0</v>
@@ -30667,7 +30362,7 @@
     </row>
     <row r="16">
       <c r="A16" s="490" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="B16" s="477">
         <v>987.99</v>
@@ -30684,7 +30379,7 @@
     </row>
     <row r="17">
       <c r="A17" s="490" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="B17" s="477">
         <v>971.0</v>
@@ -30732,7 +30427,7 @@
     </row>
     <row r="20">
       <c r="A20" s="96" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="B20" s="114"/>
       <c r="C20" s="2"/>
@@ -30764,7 +30459,7 @@
     </row>
     <row r="22">
       <c r="A22" s="96" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="B22" s="477">
         <v>981.2</v>
@@ -30812,11 +30507,11 @@
     </row>
     <row r="25">
       <c r="A25" s="96" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="B25" s="495"/>
       <c r="C25" s="96" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -30829,7 +30524,7 @@
     </row>
     <row r="26">
       <c r="A26" s="114" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="B26" s="496">
         <v>43461.0</v>
@@ -30848,7 +30543,7 @@
     </row>
     <row r="27">
       <c r="A27" s="114" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="B27" s="496">
         <v>44498.0</v>
@@ -30867,7 +30562,7 @@
     </row>
     <row r="28">
       <c r="A28" s="114" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="B28" s="496">
         <v>45252.0</v>
@@ -30884,11 +30579,11 @@
     </row>
     <row r="29">
       <c r="A29" s="114" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="B29" s="497">
         <f>SWITCH(Summary!$K$28,"today",TODAY(),"last year","2023-12-31",Summary!$K$28)</f>
-        <v>45364</v>
+        <v>45366</v>
       </c>
       <c r="C29" s="96"/>
       <c r="D29" s="96"/>
@@ -30921,7 +30616,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="500" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="D31" s="241"/>
       <c r="E31" s="114"/>
@@ -30934,7 +30629,7 @@
     </row>
     <row r="32">
       <c r="A32" s="96" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="B32" s="501">
         <f>Summary!K32+Summary!K30+Summary!G26+ESPP!AN5+RSU!AJ5+C32</f>
@@ -30955,7 +30650,7 @@
     </row>
     <row r="33">
       <c r="A33" s="96" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="B33" s="501">
         <f>Summary!K31+ESPP!AO5+RSU!AK5+C33</f>
@@ -30993,10 +30688,10 @@
         <v>92</v>
       </c>
       <c r="C35" s="139" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="D35" s="139" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="E35" s="114"/>
       <c r="F35" s="114"/>
@@ -31008,7 +30703,7 @@
     </row>
     <row r="36">
       <c r="A36" s="96" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="B36" s="506">
         <v>13850.0</v>
@@ -31042,7 +30737,7 @@
     </row>
     <row r="38">
       <c r="A38" s="96" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="B38" s="507">
         <v>0.0</v>
@@ -31084,7 +30779,7 @@
     </row>
     <row r="40">
       <c r="A40" s="96" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="B40" s="489">
         <v>0.0</v>
@@ -31105,7 +30800,7 @@
     </row>
     <row r="41">
       <c r="A41" s="96" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="B41" s="489">
         <v>0.0</v>
@@ -31163,7 +30858,7 @@
     </row>
     <row r="44">
       <c r="A44" s="96" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="B44" s="509">
         <f>LET(agi,B32+B33,if(agi&lt;C42,0%,if(agi&lt;D42,15%,20%)))</f>
@@ -31194,7 +30889,7 @@
     </row>
     <row r="46">
       <c r="A46" s="96" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="B46" s="507">
         <v>0.1</v>
@@ -31252,7 +30947,7 @@
     </row>
     <row r="48">
       <c r="A48" s="96" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="B48" s="489">
         <v>0.0</v>
@@ -31330,7 +31025,7 @@
     </row>
     <row r="51">
       <c r="A51" s="96" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="B51" s="511">
         <v>0.01</v>
@@ -31400,7 +31095,7 @@
     </row>
     <row r="53">
       <c r="A53" s="96" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="B53" s="510">
         <v>0.0</v>
@@ -31435,7 +31130,7 @@
     </row>
     <row r="54">
       <c r="A54" s="96" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="B54" s="510">
         <v>0.0</v>
@@ -31530,7 +31225,7 @@
       <c r="A57" s="96"/>
       <c r="B57" s="480"/>
       <c r="C57" s="114" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="114"/>
@@ -31543,7 +31238,7 @@
     </row>
     <row r="58">
       <c r="A58" s="96" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="B58" s="501">
         <f>LET(income, B32 - Summary!L34, 
@@ -31571,7 +31266,7 @@
     </row>
     <row r="59">
       <c r="A59" s="96" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="B59" s="199">
         <f>B33*B44</f>
@@ -31589,7 +31284,7 @@
     </row>
     <row r="60">
       <c r="A60" s="96" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="B60" s="199">
         <f>LET(income,B32+B33,

</xml_diff>